<commit_message>
Adjustment following integration tests
</commit_message>
<xml_diff>
--- a/import/raw_data/primes/renewable_energy_system_utilization_primes.xlsx
+++ b/import/raw_data/primes/renewable_energy_system_utilization_primes.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_env\workspace\micat\back_end\import\public\primes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\primes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7139926-029C-4B50-8A59-6515398CBD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="1125" windowWidth="43200" windowHeight="11325"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -47,10 +43,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -61,12 +54,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -75,13 +83,15 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -104,44 +114,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -168,15 +178,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -203,7 +212,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -215,162 +223,180 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +434,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -416,157 +442,157 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3.7043000420312024E-5</v>
+        <v>4.9289702887829936</v>
       </c>
       <c r="D2">
-        <v>2.8436730460753743E-5</v>
+        <v>3.7838133509921792</v>
       </c>
       <c r="E2">
-        <v>2.2430912134312783E-5</v>
+        <v>2.9846745189599941</v>
       </c>
       <c r="F2">
-        <v>2.1518932426900993E-5</v>
+        <v>2.8633257936731269</v>
       </c>
       <c r="G2">
-        <v>1.9274810138295901E-5</v>
+        <v>2.5647211461169608</v>
       </c>
       <c r="H2">
-        <v>1.7847643413079343E-5</v>
+        <v>2.374821237742506</v>
       </c>
       <c r="I2">
-        <v>1.7266014332376066E-5</v>
+        <v>2.2974292223725352</v>
       </c>
       <c r="J2">
-        <v>1.6584341628840938E-5</v>
+        <v>2.2067253251645589</v>
       </c>
       <c r="K2">
-        <v>1.6114278700627293E-5</v>
+        <v>2.1441783883415648</v>
       </c>
       <c r="L2">
-        <v>1.6056270525238428E-5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.13645977565485</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4.9238048114803618E-2</v>
+      </c>
+      <c r="D3">
+        <v>5.7051334009565517E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.1056434026421734</v>
+      </c>
+      <c r="F3">
+        <v>0.17174892024400601</v>
+      </c>
+      <c r="G3">
+        <v>0.25447060823031281</v>
+      </c>
+      <c r="H3">
+        <v>0.3192359057390009</v>
+      </c>
+      <c r="I3">
+        <v>0.34489903763181468</v>
+      </c>
+      <c r="J3">
+        <v>0.35738775626019043</v>
+      </c>
+      <c r="K3">
+        <v>0.35549724797416249</v>
+      </c>
+      <c r="L3">
+        <v>0.35899975162708042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>5.0714892089427259E-7</v>
-      </c>
-      <c r="D3">
-        <v>5.8762529357517089E-7</v>
-      </c>
-      <c r="E3">
-        <v>1.0881206648293039E-6</v>
-      </c>
-      <c r="F3">
-        <v>1.7690035024015598E-6</v>
-      </c>
-      <c r="G3">
-        <v>2.6210318910775744E-6</v>
-      </c>
-      <c r="H3">
-        <v>3.2881105426590639E-6</v>
-      </c>
-      <c r="I3">
-        <v>3.5524392507317729E-6</v>
-      </c>
-      <c r="J3">
-        <v>3.6810722981053272E-6</v>
-      </c>
-      <c r="K3">
-        <v>3.6616001769732057E-6</v>
-      </c>
-      <c r="L3">
-        <v>3.6976757529965261E-6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.57434484172056188</v>
+      </c>
+      <c r="D4">
+        <v>2.7989278185775639</v>
+      </c>
+      <c r="E4">
+        <v>4.2353979375655451</v>
+      </c>
+      <c r="F4">
+        <v>4.295696625002833</v>
+      </c>
+      <c r="G4">
+        <v>4.6589271396068037</v>
+      </c>
+      <c r="H4">
+        <v>4.8572522541302368</v>
+      </c>
+      <c r="I4">
+        <v>4.9400434923078507</v>
+      </c>
+      <c r="J4">
+        <v>5.0843447344253594</v>
+      </c>
+      <c r="K4">
+        <v>5.2120761093703978</v>
+      </c>
+      <c r="L4">
+        <v>5.2177988478685364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>3</v>
-      </c>
-      <c r="C4">
-        <v>2.2011970868875508E-6</v>
-      </c>
-      <c r="D4">
-        <v>1.0726990673764926E-5</v>
-      </c>
-      <c r="E4">
-        <v>1.6232313628951761E-5</v>
-      </c>
-      <c r="F4">
-        <v>1.6463410498791292E-5</v>
-      </c>
-      <c r="G4">
-        <v>1.7855504398720366E-5</v>
-      </c>
-      <c r="H4">
-        <v>1.8615592472355438E-5</v>
-      </c>
-      <c r="I4">
-        <v>1.8932892844986002E-5</v>
-      </c>
-      <c r="J4">
-        <v>1.9485932501147579E-5</v>
-      </c>
-      <c r="K4">
-        <v>1.9975467550493345E-5</v>
-      </c>
-      <c r="L4">
-        <v>1.9997400149858884E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>4.2381815082829986E-5</v>
+        <v>5.7324329244767958</v>
       </c>
       <c r="D5">
-        <v>3.8043850109028021E-5</v>
+        <v>5.1456932298117648</v>
       </c>
       <c r="E5">
-        <v>3.2155418311938866E-5</v>
+        <v>4.3492421990760608</v>
       </c>
       <c r="F5">
-        <v>2.93828826237283E-5</v>
+        <v>3.9742376167493352</v>
       </c>
       <c r="G5">
-        <v>3.1587203303243795E-5</v>
+        <v>4.2723871984664923</v>
       </c>
       <c r="H5">
-        <v>2.2713150533125333E-5</v>
+        <v>3.0721103303438642</v>
       </c>
       <c r="I5">
-        <v>2.2957864049545577E-5</v>
+        <v>3.105209521962963</v>
       </c>
       <c r="J5">
-        <v>2.3209289793360049E-5</v>
+        <v>3.1392165886515042</v>
       </c>
       <c r="K5">
-        <v>2.1954335577394848E-5</v>
+        <v>2.9694753717581208</v>
       </c>
       <c r="L5">
-        <v>1.8860871334834992E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.5510629880486291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
       <c r="C6">
         <v>0</v>
       </c>
@@ -598,205 +624,205 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
       <c r="C7">
-        <v>1.634260221702956E-6</v>
+        <v>0.41422713124311172</v>
       </c>
       <c r="D7">
-        <v>5.9722251955049098E-6</v>
+        <v>1.513747735531362</v>
       </c>
       <c r="E7">
-        <v>1.1860656992594071E-5</v>
+        <v>3.006256809935246</v>
       </c>
       <c r="F7">
-        <v>1.4633192680804638E-5</v>
+        <v>3.7089964894214629</v>
       </c>
       <c r="G7">
-        <v>1.2428872001289148E-5</v>
+        <v>3.1502792060355298</v>
       </c>
       <c r="H7">
-        <v>2.1302924771407601E-5</v>
+        <v>5.3995375387359168</v>
       </c>
       <c r="I7">
-        <v>2.1058211254987361E-5</v>
+        <v>5.3375113225085258</v>
       </c>
       <c r="J7">
-        <v>2.0806785511172896E-5</v>
+        <v>5.2737837941762216</v>
       </c>
       <c r="K7">
-        <v>2.2061739727138092E-5</v>
+        <v>5.5918702762537382</v>
       </c>
       <c r="L7">
-        <v>2.5155203969697942E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.3759539869026174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>4.2541333447942263E-5</v>
+        <v>5.7540088840349499</v>
       </c>
       <c r="D8">
-        <v>1.6997484099710846E-5</v>
+        <v>2.2990270071261669</v>
       </c>
       <c r="E8">
-        <v>1.2103223904064955E-5</v>
+        <v>1.637044545269714</v>
       </c>
       <c r="F8">
-        <v>1.2007695290135007E-5</v>
+        <v>1.6241236410882529</v>
       </c>
       <c r="G8">
-        <v>1.5877208797756263E-5</v>
+        <v>2.1475020426372269</v>
       </c>
       <c r="H8">
-        <v>1.4088003557587992E-5</v>
+        <v>1.9054996883883131</v>
       </c>
       <c r="I8">
-        <v>1.2329215950373367E-5</v>
+        <v>1.667611528878046</v>
       </c>
       <c r="J8">
-        <v>1.0902757222002617E-5</v>
+        <v>1.4746731433006779</v>
       </c>
       <c r="K8">
-        <v>1.0570203477268059E-5</v>
+        <v>1.4296929547044901</v>
       </c>
       <c r="L8">
-        <v>1.0166861692361196E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.375138195237521</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>4.622746721678682E-6</v>
+        <v>0.34770466624767632</v>
       </c>
       <c r="E9">
-        <v>5.6622320945290487E-6</v>
+        <v>0.42589063151834738</v>
       </c>
       <c r="F9">
-        <v>9.4143030516393675E-6</v>
+        <v>0.70810652142673769</v>
       </c>
       <c r="G9">
-        <v>7.1469449419290075E-6</v>
+        <v>0.53756484084889322</v>
       </c>
       <c r="H9">
-        <v>8.9834306755934125E-6</v>
+        <v>0.67569801091807657</v>
       </c>
       <c r="I9">
-        <v>8.4804635197105733E-6</v>
+        <v>0.63786681712810422</v>
       </c>
       <c r="J9">
-        <v>8.2879553884757958E-6</v>
+        <v>0.62338711933132651</v>
       </c>
       <c r="K9">
-        <v>7.7883984608326586E-6</v>
+        <v>0.58581242937842437</v>
       </c>
       <c r="L9">
-        <v>7.2409012421206561E-6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.54463186094904292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>5.0947704728074559E-7</v>
+        <v>0.1454772705211764</v>
       </c>
       <c r="D10">
-        <v>2.1430579673833477E-5</v>
+        <v>6.119337962869837</v>
       </c>
       <c r="E10">
-        <v>2.5285354496629004E-5</v>
+        <v>7.2200394030762816</v>
       </c>
       <c r="F10">
-        <v>2.1628812153448629E-5</v>
+        <v>6.1759417298441814</v>
       </c>
       <c r="G10">
-        <v>2.0026656755537735E-5</v>
+        <v>5.7184585213603851</v>
       </c>
       <c r="H10">
-        <v>1.9979376262041604E-5</v>
+        <v>5.7049579384010114</v>
       </c>
       <c r="I10">
-        <v>2.2241131025139061E-5</v>
+        <v>6.3507846960142427</v>
       </c>
       <c r="J10">
-        <v>2.3860097884744589E-5</v>
+        <v>6.8130682886838629</v>
       </c>
       <c r="K10">
-        <v>2.469220855712229E-5</v>
+        <v>7.0506711209118338</v>
       </c>
       <c r="L10">
-        <v>2.5643047560741154E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.3221759191943816</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2.7832821190277892</v>
       </c>
       <c r="D11">
-        <v>5.6877814502062717E-5</v>
+        <v>7.6931168683240037</v>
       </c>
       <c r="E11">
-        <v>4.1641052926002553E-5</v>
+        <v>5.6322397315070027</v>
       </c>
       <c r="F11">
-        <v>3.5212460488157338E-5</v>
+        <v>4.7627282470006218</v>
       </c>
       <c r="G11">
-        <v>2.326957573374657E-5</v>
+        <v>3.147370678061769</v>
       </c>
       <c r="H11">
-        <v>1.2709087681499121E-5</v>
+        <v>1.718991801627749</v>
       </c>
       <c r="I11">
-        <v>1.2341661546412258E-5</v>
+        <v>1.6692948816169191</v>
       </c>
       <c r="J11">
-        <v>1.0153828934348794E-5</v>
+        <v>1.373375424790314</v>
       </c>
       <c r="K11">
-        <v>7.9092721005946686E-6</v>
+        <v>1.069783625582917</v>
       </c>
       <c r="L11">
-        <v>1.0882021865123346E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.4718685432087939</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1.114715004849921</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -826,88 +852,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>2.3921181455428031</v>
       </c>
       <c r="D13">
-        <v>4.8554231892004752E-6</v>
+        <v>0.56443237142021196</v>
       </c>
       <c r="E13">
-        <v>2.0092184765260637E-5</v>
+        <v>2.33567272144131</v>
       </c>
       <c r="F13">
-        <v>2.6520777203105845E-5</v>
+        <v>3.082982591908956</v>
       </c>
       <c r="G13">
-        <v>3.8463661957516614E-5</v>
+        <v>4.4713169349428892</v>
       </c>
       <c r="H13">
-        <v>4.9024150009764061E-5</v>
+        <v>5.6989506719861813</v>
       </c>
       <c r="I13">
-        <v>4.9391576144850919E-5</v>
+        <v>5.7416631599954897</v>
       </c>
       <c r="J13">
-        <v>5.1579408756914386E-5</v>
+        <v>5.9959939364032202</v>
       </c>
       <c r="K13">
-        <v>5.3823965590668515E-5</v>
+        <v>6.2569187800463339</v>
       </c>
       <c r="L13">
-        <v>5.0851215826139829E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.9113430940867966</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>3.5429510327159738E-5</v>
+        <v>4.7920857353695858</v>
       </c>
       <c r="D14">
-        <v>4.0667565860533169E-6</v>
+        <v>0.55005688888415194</v>
       </c>
       <c r="E14">
-        <v>4.418444375916347E-6</v>
+        <v>0.59762508910887646</v>
       </c>
       <c r="F14">
-        <v>5.9372430373945241E-6</v>
+        <v>0.80305308778456319</v>
       </c>
       <c r="G14">
-        <v>1.0164013798060665E-5</v>
+        <v>1.3747529978829041</v>
       </c>
       <c r="H14">
-        <v>1.0728414118673707E-5</v>
+        <v>1.4510920356080299</v>
       </c>
       <c r="I14">
-        <v>1.4420569619335652E-5</v>
+        <v>1.95048154294551</v>
       </c>
       <c r="J14">
-        <v>1.5139022077604027E-5</v>
+        <v>2.0476571952482692</v>
       </c>
       <c r="K14">
-        <v>1.4458629186533428E-5</v>
+        <v>1.955629362020022</v>
       </c>
       <c r="L14">
-        <v>1.487288520637609E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.0116603470702792</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -940,316 +966,316 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>1.6104322875981698E-6</v>
+        <v>0.46178280722652371</v>
       </c>
       <c r="D16">
-        <v>3.2973186028704584E-5</v>
+        <v>9.4548839617756428</v>
       </c>
       <c r="E16">
-        <v>3.2621498238841553E-5</v>
+        <v>9.3540393772992267</v>
       </c>
       <c r="F16">
-        <v>3.110269957736338E-5</v>
+        <v>8.9185320201067722</v>
       </c>
       <c r="G16">
-        <v>2.6875928816697243E-5</v>
+        <v>7.7065282106982904</v>
       </c>
       <c r="H16">
-        <v>2.6311528496084202E-5</v>
+        <v>7.5446894507210223</v>
       </c>
       <c r="I16">
-        <v>2.261937299542225E-5</v>
+        <v>6.4859836951655643</v>
       </c>
       <c r="J16">
-        <v>2.1900920537153879E-5</v>
+        <v>6.279971312283716</v>
       </c>
       <c r="K16">
-        <v>2.2581313428224482E-5</v>
+        <v>6.4750703187275986</v>
       </c>
       <c r="L16">
-        <v>2.216705740838182E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.3562846304210554</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>4.0494627603075015E-5</v>
+        <v>5.4771777962463268</v>
       </c>
       <c r="D17">
-        <v>2.729679368562529E-5</v>
+        <v>3.6920796938572309</v>
       </c>
       <c r="E17">
-        <v>2.2179316232551195E-5</v>
+        <v>2.9999055577345368</v>
       </c>
       <c r="F17">
-        <v>2.1381023519202086E-5</v>
+        <v>2.8919309600343488</v>
       </c>
       <c r="G17">
-        <v>2.2347443448434197E-5</v>
+        <v>3.022645923760503</v>
       </c>
       <c r="H17">
-        <v>1.7638585521681602E-5</v>
+        <v>2.3857403980475231</v>
       </c>
       <c r="I17">
-        <v>1.7185796931565558E-5</v>
+        <v>2.3244976169930571</v>
       </c>
       <c r="J17">
-        <v>1.7362520564132959E-5</v>
+        <v>2.3484007076908631</v>
       </c>
       <c r="K17">
-        <v>1.6209898469885625E-5</v>
+        <v>2.1925006163514609</v>
       </c>
       <c r="L17">
-        <v>1.6255972008813701E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.1987323803989018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>6.0391136472622327E-8</v>
+        <v>4.1800312292828773E-3</v>
       </c>
       <c r="E18">
-        <v>1.7690002962662048E-6</v>
+        <v>0.12244307550588331</v>
       </c>
       <c r="F18">
-        <v>3.0047985817308089E-6</v>
+        <v>0.20798005540156861</v>
       </c>
       <c r="G18">
-        <v>4.7588306771192109E-6</v>
+        <v>0.32938709233010588</v>
       </c>
       <c r="H18">
-        <v>5.026791655477341E-6</v>
+        <v>0.34793427198574889</v>
       </c>
       <c r="I18">
-        <v>6.0531113294583808E-6</v>
+        <v>0.41897198611144698</v>
       </c>
       <c r="J18">
-        <v>6.7269367631383937E-6</v>
+        <v>0.46561146866439429</v>
       </c>
       <c r="K18">
-        <v>6.3057523727248775E-6</v>
+        <v>0.43645878156414247</v>
       </c>
       <c r="L18">
-        <v>6.2956700867724202E-6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.43576092633893182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>4.5309907130297808E-6</v>
+        <v>1.214552829041422</v>
       </c>
       <c r="D19">
-        <v>1.7668433494006876E-5</v>
+        <v>4.7361045837427689</v>
       </c>
       <c r="E19">
-        <v>2.1077301787287392E-5</v>
+        <v>5.6498673547692739</v>
       </c>
       <c r="F19">
-        <v>2.0639796215171896E-5</v>
+        <v>5.5325919807972674</v>
       </c>
       <c r="G19">
-        <v>1.7919344190551385E-5</v>
+        <v>4.8033623460349171</v>
       </c>
       <c r="H19">
-        <v>2.236024113894585E-5</v>
+        <v>5.9937651285087874</v>
       </c>
       <c r="I19">
-        <v>2.1786710055080858E-5</v>
+        <v>5.8400274926208446</v>
       </c>
       <c r="J19">
-        <v>2.0936160988833441E-5</v>
+        <v>5.612033916805597</v>
       </c>
       <c r="K19">
-        <v>2.2509967473494283E-5</v>
+        <v>6.0338999587755664</v>
       </c>
       <c r="L19">
-        <v>2.2473976220518675E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.0242523384446383</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>2.4225136454825605E-5</v>
+        <v>3.2766168589566842</v>
       </c>
       <c r="D20">
-        <v>2.1638452232056018E-5</v>
+        <v>2.9267499697059609</v>
       </c>
       <c r="E20">
-        <v>1.8587772688827899E-5</v>
+        <v>2.5141245117955129</v>
       </c>
       <c r="F20">
-        <v>1.7440127823072519E-5</v>
+        <v>2.3588976249525242</v>
       </c>
       <c r="G20">
-        <v>1.5860063586085393E-5</v>
+        <v>2.1451830344567822</v>
       </c>
       <c r="H20">
-        <v>1.5741814007832762E-5</v>
+        <v>2.129188963076023</v>
       </c>
       <c r="I20">
-        <v>1.5361514382807952E-5</v>
+        <v>2.077750814724006</v>
       </c>
       <c r="J20">
-        <v>1.518801061101876E-5</v>
+        <v>2.0542832324134919</v>
       </c>
       <c r="K20">
-        <v>1.5403936260052652E-5</v>
+        <v>2.083488666332304</v>
       </c>
       <c r="L20">
-        <v>1.3908719247170362E-5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.881250248342587</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>4.3643005252433348E-6</v>
+        <v>0.47640824372113949</v>
       </c>
       <c r="D21">
-        <v>6.9258223322121546E-6</v>
+        <v>0.75602466753360709</v>
       </c>
       <c r="E21">
-        <v>6.2089511399475072E-6</v>
+        <v>0.67777081134160266</v>
       </c>
       <c r="F21">
-        <v>6.626072635279182E-6</v>
+        <v>0.72330390830866353</v>
       </c>
       <c r="G21">
-        <v>3.9059425143280567E-6</v>
+        <v>0.42637375738991062</v>
       </c>
       <c r="H21">
-        <v>3.016729540697772E-6</v>
+        <v>0.329307025021008</v>
       </c>
       <c r="I21">
-        <v>2.7726282361922031E-6</v>
+        <v>0.30266085959383388</v>
       </c>
       <c r="J21">
-        <v>2.7413122184637069E-6</v>
+        <v>0.29924239449958112</v>
       </c>
       <c r="K21">
-        <v>2.6972340275586297E-6</v>
+        <v>0.29443080707703018</v>
       </c>
       <c r="L21">
-        <v>3.7873426148178577E-6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.41342735979324008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>2.7428305385419503E-8</v>
+        <v>1.368262981321504E-2</v>
       </c>
       <c r="D22">
-        <v>5.2590721186185483E-8</v>
+        <v>2.623491898201992E-2</v>
       </c>
       <c r="E22">
-        <v>3.8201414566789525E-6</v>
+        <v>1.9056803054861691</v>
       </c>
       <c r="F22">
-        <v>4.5506648271026569E-6</v>
+        <v>2.2701024127565348</v>
       </c>
       <c r="G22">
-        <v>8.8508591850409099E-6</v>
+        <v>4.4152574523319084</v>
       </c>
       <c r="H22">
-        <v>9.8583217369238235E-6</v>
+        <v>4.917830868895174</v>
       </c>
       <c r="I22">
-        <v>1.0482722666454202E-5</v>
+        <v>5.2293137204144351</v>
       </c>
       <c r="J22">
-        <v>1.068754245597189E-5</v>
+        <v>5.3314882193129671</v>
       </c>
       <c r="K22">
-        <v>1.0515694997843076E-5</v>
+        <v>5.2457619915756712</v>
       </c>
       <c r="L22">
-        <v>1.0920803423466138E-5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.447850620243238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>3.6086708797466337E-5</v>
+        <v>4.8809763631479983</v>
       </c>
       <c r="D23">
-        <v>3.6086708797466337E-5</v>
+        <v>4.8809763631479983</v>
       </c>
       <c r="E23">
-        <v>3.6086708797466337E-5</v>
+        <v>4.8809763631479983</v>
       </c>
       <c r="F23">
-        <v>2.5709713453580391E-5</v>
+        <v>3.477416141619559</v>
       </c>
       <c r="G23">
-        <v>1.7962040534482077E-5</v>
+        <v>2.429489920368376</v>
       </c>
       <c r="H23">
-        <v>8.5427617717553883E-6</v>
+        <v>1.1554674746861351</v>
       </c>
       <c r="I23">
-        <v>1.3900308672421357E-5</v>
+        <v>1.8801126600748179</v>
       </c>
       <c r="J23">
-        <v>1.0017661340987525E-5</v>
+        <v>1.3549578182318081</v>
       </c>
       <c r="K23">
-        <v>8.675244303257375E-6</v>
+        <v>1.1733866512012461</v>
       </c>
       <c r="L23">
-        <v>1.0208870496938814E-5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.3808201759173959</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1267,27 +1293,27 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>1.8923839367812572E-5</v>
+        <v>1.568030898479303</v>
       </c>
       <c r="I24">
-        <v>1.1732877458296698E-5</v>
+        <v>0.97218719864916747</v>
       </c>
       <c r="J24">
-        <v>9.1606126744841852E-6</v>
+        <v>0.75904912546574299</v>
       </c>
       <c r="K24">
-        <v>1.1686550851012522E-5</v>
+        <v>0.96834857212991798</v>
       </c>
       <c r="L24">
-        <v>1.067530161527308E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.88455637664129605</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1299,71 +1325,71 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>1.037699534388595E-5</v>
+        <v>4.0613657474014433</v>
       </c>
       <c r="G25">
-        <v>1.8124668262984267E-5</v>
+        <v>7.0936628982559329</v>
       </c>
       <c r="H25">
-        <v>8.6201076578983843E-6</v>
+        <v>3.373752114221451</v>
       </c>
       <c r="I25">
-        <v>1.0453522666748289E-5</v>
+        <v>4.0913171386773932</v>
       </c>
       <c r="J25">
-        <v>1.6908434781994632E-5</v>
+        <v>6.617651409685255</v>
       </c>
       <c r="K25">
-        <v>1.5724913643196442E-5</v>
+        <v>6.154442932168438</v>
       </c>
       <c r="L25">
-        <v>1.5202536685254451E-5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.949994166999879</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>3.6013361828365801E-5</v>
+        <v>4.8710556794830628</v>
       </c>
       <c r="D26">
-        <v>3.1227032012740872E-5</v>
+        <v>4.2236715462440682</v>
       </c>
       <c r="E26">
-        <v>1.6069709386226235E-5</v>
+        <v>2.1735390754818522</v>
       </c>
       <c r="F26">
-        <v>2.0570935356834532E-5</v>
+        <v>2.782360946465817</v>
       </c>
       <c r="G26">
-        <v>1.9352259587800058E-5</v>
+        <v>2.617526639841099</v>
       </c>
       <c r="H26">
-        <v>1.5024090935327096E-5</v>
+        <v>2.032111965230432</v>
       </c>
       <c r="I26">
-        <v>1.5788760770050962E-5</v>
+        <v>2.1355388365986938</v>
       </c>
       <c r="J26">
-        <v>1.6688642976166111E-5</v>
+        <v>2.2572541141629898</v>
       </c>
       <c r="K26">
-        <v>1.6140900785432632E-5</v>
+        <v>2.183168203445172</v>
       </c>
       <c r="L26">
-        <v>1.4848288672532698E-5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.0083334961518768</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1381,100 +1407,100 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>2.5182759490081578E-6</v>
+        <v>0.26932285439654863</v>
       </c>
       <c r="I27">
-        <v>2.3715726249872191E-6</v>
+        <v>0.2536333276032906</v>
       </c>
       <c r="J27">
-        <v>2.2831903786686927E-6</v>
+        <v>0.24418108355280849</v>
       </c>
       <c r="K27">
-        <v>1.9765879787305105E-6</v>
+        <v>0.211390779714698</v>
       </c>
       <c r="L27">
-        <v>3.4493746375068418E-6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.36890136032244392</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>7.334696910054131E-8</v>
+        <v>1.615823926264855E-2</v>
       </c>
       <c r="D28">
-        <v>4.8596767847254667E-6</v>
+        <v>1.0705803005860419</v>
       </c>
       <c r="E28">
-        <v>2.0016999411240102E-5</v>
+        <v>4.409718217037077</v>
       </c>
       <c r="F28">
-        <v>1.5515773440631809E-5</v>
+        <v>3.418104151721876</v>
       </c>
       <c r="G28">
-        <v>1.6734449209666287E-5</v>
+        <v>3.6865767948471659</v>
       </c>
       <c r="H28">
-        <v>1.8544341913131089E-5</v>
+        <v>4.0852937384500922</v>
       </c>
       <c r="I28">
-        <v>1.7926375402428162E-5</v>
+        <v>3.9491565420711319</v>
       </c>
       <c r="J28">
-        <v>1.7114875442631537E-5</v>
+        <v>3.7703841855194988</v>
       </c>
       <c r="K28">
-        <v>1.7969220033303196E-5</v>
+        <v>3.9585951569898969</v>
       </c>
       <c r="L28">
-        <v>1.7789045487426799E-5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.918902945341463</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>3.0887940479648834E-5</v>
+        <v>4.1778070766617921</v>
       </c>
       <c r="D29">
-        <v>2.615393152450036E-5</v>
+        <v>3.537499700816173</v>
       </c>
       <c r="E29">
-        <v>3.0996841051234936E-5</v>
+        <v>4.1925366303827563</v>
       </c>
       <c r="F29">
-        <v>2.9245851588672428E-5</v>
+        <v>3.9557032237438858</v>
       </c>
       <c r="G29">
-        <v>2.9150456089030943E-5</v>
+        <v>3.9428003241884282</v>
       </c>
       <c r="H29">
-        <v>2.6509538584949669E-5</v>
+        <v>3.585598009430659</v>
       </c>
       <c r="I29">
-        <v>2.5025374115365736E-5</v>
+        <v>3.3848545241845929</v>
       </c>
       <c r="J29">
-        <v>2.462309173643984E-5</v>
+        <v>3.3304430566864509</v>
       </c>
       <c r="K29">
-        <v>2.3851618258910257E-5</v>
+        <v>3.226095945683582</v>
       </c>
       <c r="L29">
-        <v>2.4016796258181032E-5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.2484374098131479</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1483,112 +1509,112 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>5.1291559698929063E-6</v>
+        <v>0.48323536101051451</v>
       </c>
       <c r="E30">
-        <v>9.2129588037902295E-7</v>
+        <v>8.6798442076182841E-2</v>
       </c>
       <c r="F30">
-        <v>7.6621230574968485E-7</v>
+        <v>7.2187487054985885E-2</v>
       </c>
       <c r="G30">
-        <v>5.6783774189310772E-7</v>
+        <v>5.3497939584949021E-2</v>
       </c>
       <c r="H30">
-        <v>1.296546871646887E-6</v>
+        <v>0.12215212390985609</v>
       </c>
       <c r="I30">
-        <v>2.675903401647976E-6</v>
+        <v>0.25210602951339428</v>
       </c>
       <c r="J30">
-        <v>3.4072976352451792E-6</v>
+        <v>0.32101318667296352</v>
       </c>
       <c r="K30">
-        <v>3.9260329162253689E-6</v>
+        <v>0.3698850151462526</v>
       </c>
       <c r="L30">
-        <v>3.8866153320592816E-6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.36617134946198221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>0.69382052300823405</v>
+      </c>
+      <c r="D31">
+        <v>0.51186268976832949</v>
+      </c>
+      <c r="E31">
+        <v>0.2194342636757432</v>
+      </c>
+      <c r="F31">
+        <v>1.0971453608195449</v>
+      </c>
+      <c r="G31">
+        <v>1.232420998064147</v>
+      </c>
+      <c r="H31">
+        <v>2.1129573035727929</v>
+      </c>
+      <c r="I31">
+        <v>2.1612194057303098</v>
+      </c>
+      <c r="J31">
+        <v>2.009669532556424</v>
+      </c>
+      <c r="K31">
+        <v>2.1260507600619198</v>
+      </c>
+      <c r="L31">
+        <v>2.0681404335607838</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>4.9274662932560336</v>
+      </c>
+      <c r="D32">
+        <v>4.3712685755523086</v>
+      </c>
+      <c r="E32">
+        <v>3.0158905049045019</v>
+      </c>
+      <c r="F32">
+        <v>3.1030183816523711</v>
+      </c>
+      <c r="G32">
+        <v>2.3841962265132208</v>
+      </c>
+      <c r="H32">
+        <v>2.395517140767629</v>
+      </c>
+      <c r="I32">
+        <v>2.5831477540069079</v>
+      </c>
+      <c r="J32">
+        <v>2.7295179679955162</v>
+      </c>
+      <c r="K32">
+        <v>2.829238768600181</v>
+      </c>
+      <c r="L32">
+        <v>2.6342958917336179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>3</v>
-      </c>
-      <c r="C31">
-        <v>1.5067288038853092E-6</v>
-      </c>
-      <c r="D31">
-        <v>1.1115817891408777E-6</v>
-      </c>
-      <c r="E31">
-        <v>4.7653235192018425E-7</v>
-      </c>
-      <c r="F31">
-        <v>2.3826053891120343E-6</v>
-      </c>
-      <c r="G31">
-        <v>2.6763754526100888E-6</v>
-      </c>
-      <c r="H31">
-        <v>4.5885838269375901E-6</v>
-      </c>
-      <c r="I31">
-        <v>4.6933917665204363E-6</v>
-      </c>
-      <c r="J31">
-        <v>4.3642799118491263E-6</v>
-      </c>
-      <c r="K31">
-        <v>4.6170181083985214E-6</v>
-      </c>
-      <c r="L31">
-        <v>4.4912576932938377E-6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>10</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>3.6430424571730246E-5</v>
-      </c>
-      <c r="D32">
-        <v>3.2318266761639015E-5</v>
-      </c>
-      <c r="E32">
-        <v>2.2297498352427999E-5</v>
-      </c>
-      <c r="F32">
-        <v>2.2941664208276165E-5</v>
-      </c>
-      <c r="G32">
-        <v>1.7627168939353435E-5</v>
-      </c>
-      <c r="H32">
-        <v>1.7710868286702136E-5</v>
-      </c>
-      <c r="I32">
-        <v>1.9098084859307897E-5</v>
-      </c>
-      <c r="J32">
-        <v>2.0180249347689699E-5</v>
-      </c>
-      <c r="K32">
-        <v>2.0917518948018147E-5</v>
-      </c>
-      <c r="L32">
-        <v>1.9476240337710187E-5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>10</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1603,106 +1629,106 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>7.5619395291796389E-9</v>
+        <v>6.1882007341698025E-4</v>
       </c>
       <c r="G33">
-        <v>1.9246531508683876E-6</v>
+        <v>0.1575011277896064</v>
       </c>
       <c r="H33">
-        <v>2.3966334083116231E-6</v>
+        <v>0.19612493011377991</v>
       </c>
       <c r="I33">
-        <v>2.2624354526560054E-6</v>
+        <v>0.1851430400245018</v>
       </c>
       <c r="J33">
-        <v>2.0737505114256625E-6</v>
+        <v>0.1697022885169972</v>
       </c>
       <c r="K33">
-        <v>2.5770062740875609E-6</v>
+        <v>0.21088547529021101</v>
       </c>
       <c r="L33">
-        <v>2.5785395464464457E-6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.21101094835304529</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>6.0951804302766173E-7</v>
+        <v>0.16805386971851341</v>
       </c>
       <c r="D34">
-        <v>4.7216758531188917E-6</v>
+        <v>1.3018415250376461</v>
       </c>
       <c r="E34">
-        <v>1.4742444262329914E-5</v>
+        <v>4.0647275921274062</v>
       </c>
       <c r="F34">
-        <v>1.4090716466952561E-5</v>
+        <v>3.885035818817081</v>
       </c>
       <c r="G34">
-        <v>1.748812052453608E-5</v>
+        <v>4.821754436756958</v>
       </c>
       <c r="H34">
-        <v>1.6932440919744146E-5</v>
+        <v>4.668544685253833</v>
       </c>
       <c r="I34">
-        <v>1.5679422302794002E-5</v>
+        <v>4.3230674187207168</v>
       </c>
       <c r="J34">
-        <v>1.4785942755642548E-5</v>
+        <v>4.0767208222076867</v>
       </c>
       <c r="K34">
-        <v>1.3545417392652196E-5</v>
+        <v>3.7346881455391951</v>
       </c>
       <c r="L34">
-        <v>1.4985162730601275E-5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.1316489545247146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>3.9900751190694494E-5</v>
+        <v>5.3968519137246167</v>
       </c>
       <c r="D35">
-        <v>3.9900751190694494E-5</v>
+        <v>5.3968519137246167</v>
       </c>
       <c r="E35">
-        <v>3.5788154976064178E-5</v>
+        <v>4.8405948987819896</v>
       </c>
       <c r="F35">
-        <v>3.6852380638180906E-5</v>
+        <v>4.9845387627403444</v>
       </c>
       <c r="G35">
-        <v>3.3656459762710099E-5</v>
+        <v>4.5522684124788793</v>
       </c>
       <c r="H35">
-        <v>3.1020021470486641E-5</v>
+        <v>4.1956719420314412</v>
       </c>
       <c r="I35">
-        <v>2.6461552135958386E-5</v>
+        <v>3.579107511098091</v>
       </c>
       <c r="J35">
-        <v>2.2851038564457683E-5</v>
+        <v>3.0907606380089798</v>
       </c>
       <c r="K35">
-        <v>2.210367893907954E-5</v>
+        <v>2.989675091895172</v>
       </c>
       <c r="L35">
-        <v>1.9945519271133552E-5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.6977691055037689</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1735,15 +1761,15 @@
         <v>0</v>
       </c>
       <c r="L36">
-        <v>2.4506053402540262E-6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.2053891063873198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1752,71 +1778,71 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>4.1125962146303122E-6</v>
+        <v>0.99882646478749182</v>
       </c>
       <c r="F37">
-        <v>3.0483705525135859E-6</v>
+        <v>0.74035792074548212</v>
       </c>
       <c r="G37">
-        <v>6.2442914279843937E-6</v>
+        <v>1.516551396397456</v>
       </c>
       <c r="H37">
-        <v>8.8807297202078515E-6</v>
+        <v>2.1568633068359202</v>
       </c>
       <c r="I37">
-        <v>1.3439199054736107E-5</v>
+        <v>3.2639790003366822</v>
       </c>
       <c r="J37">
-        <v>1.7049712626236815E-5</v>
+        <v>4.1408646264674944</v>
       </c>
       <c r="K37">
-        <v>1.7797072251614948E-5</v>
+        <v>4.3223758990514112</v>
       </c>
       <c r="L37">
-        <v>1.750462657930691E-5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.251349602821624</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38">
-        <v>4.1591460986910369E-5</v>
+        <v>5.625532079560406</v>
       </c>
       <c r="D38">
-        <v>4.130948498021945E-5</v>
+        <v>5.5873928790210128</v>
       </c>
       <c r="E38">
-        <v>2.7532375582884329E-5</v>
+        <v>3.7239437709766068</v>
       </c>
       <c r="F38">
-        <v>7.6701741394021926E-6</v>
+        <v>1.0374439765557031</v>
       </c>
       <c r="G38">
-        <v>5.1406585329380192E-6</v>
+        <v>0.69530953712374055</v>
       </c>
       <c r="H38">
-        <v>3.5276915915912479E-6</v>
+        <v>0.47714462883469561</v>
       </c>
       <c r="I38">
-        <v>5.8602211542286105E-6</v>
+        <v>0.79263534663537938</v>
       </c>
       <c r="J38">
-        <v>7.6403221048501382E-6</v>
+        <v>1.0334062829034989</v>
       </c>
       <c r="K38">
-        <v>9.6058030641914605E-6</v>
+        <v>1.299251144473031</v>
       </c>
       <c r="L38">
-        <v>1.0124790691806121E-5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.369447802122544</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -1852,126 +1878,126 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>7.3177653067452428E-2</v>
+      </c>
+      <c r="E40">
+        <v>3.6485759416729802</v>
+      </c>
+      <c r="F40">
+        <v>8.8031609130821931</v>
+      </c>
+      <c r="G40">
+        <v>9.4596139838622193</v>
+      </c>
+      <c r="H40">
+        <v>9.8782068160265641</v>
+      </c>
+      <c r="I40">
+        <v>9.2728750322789111</v>
+      </c>
+      <c r="J40">
+        <v>8.8109080326099996</v>
+      </c>
+      <c r="K40">
+        <v>8.3008317128505738</v>
+      </c>
+      <c r="L40">
+        <v>8.1661454428889062</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>4.2396880611031493</v>
+      </c>
+      <c r="D41">
+        <v>4.3740582412032891</v>
+      </c>
+      <c r="E41">
+        <v>4.4058673391209933</v>
+      </c>
+      <c r="F41">
+        <v>4.4280652012731698</v>
+      </c>
+      <c r="G41">
+        <v>3.786097766171383</v>
+      </c>
+      <c r="H41">
+        <v>2.8105752326058822</v>
+      </c>
+      <c r="I41">
+        <v>2.8089099631704948</v>
+      </c>
+      <c r="J41">
+        <v>2.5708451056621229</v>
+      </c>
+      <c r="K41">
+        <v>2.4178804657074879</v>
+      </c>
+      <c r="L41">
+        <v>2.3485898812335191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>12</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>2.8197600669091774E-7</v>
-      </c>
-      <c r="E40">
-        <v>1.405908540402604E-5</v>
-      </c>
-      <c r="F40">
-        <v>3.3921286847508178E-5</v>
-      </c>
-      <c r="G40">
-        <v>3.6450802453972348E-5</v>
-      </c>
-      <c r="H40">
-        <v>3.8063769395319121E-5</v>
-      </c>
-      <c r="I40">
-        <v>3.5731239832681757E-5</v>
-      </c>
-      <c r="J40">
-        <v>3.3951138882060231E-5</v>
-      </c>
-      <c r="K40">
-        <v>3.1985657922718916E-5</v>
-      </c>
-      <c r="L40">
-        <v>3.1466670295104245E-5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>13</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>3.134544752321821E-5</v>
-      </c>
-      <c r="D41">
-        <v>3.2338891703146476E-5</v>
-      </c>
-      <c r="E41">
-        <v>3.2574067120575858E-5</v>
-      </c>
-      <c r="F41">
-        <v>3.2738183421867529E-5</v>
-      </c>
-      <c r="G41">
-        <v>2.7991901087274682E-5</v>
-      </c>
-      <c r="H41">
-        <v>2.0779533115174878E-5</v>
-      </c>
-      <c r="I41">
-        <v>2.0767221215113687E-5</v>
-      </c>
-      <c r="J41">
-        <v>1.90071272198471E-5</v>
-      </c>
-      <c r="K41">
-        <v>1.7876207910335818E-5</v>
-      </c>
-      <c r="L41">
-        <v>1.7363919188104496E-5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>13</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42">
-        <v>1.5927564798383231E-6</v>
+        <v>0.17165381969924379</v>
       </c>
       <c r="D42">
-        <v>5.9931229991005322E-7</v>
+        <v>6.4588809886833382E-2</v>
       </c>
       <c r="E42">
-        <v>3.3716378007468944E-7</v>
+        <v>3.6336660027232182E-2</v>
       </c>
       <c r="F42">
-        <v>1.8520424184166545E-7</v>
+        <v>1.995974647665626E-2</v>
       </c>
       <c r="G42">
-        <v>4.2939141820391241E-6</v>
+        <v>0.46276174678164711</v>
       </c>
       <c r="H42">
-        <v>1.0347382417900702E-5</v>
+        <v>1.1151533447861079</v>
       </c>
       <c r="I42">
-        <v>9.9835093827968231E-6</v>
+        <v>1.0759381871949869</v>
       </c>
       <c r="J42">
-        <v>1.0072659374069482E-5</v>
+        <v>1.0855460191026369</v>
       </c>
       <c r="K42">
-        <v>1.0349760625934394E-5</v>
+        <v>1.115409647929865</v>
       </c>
       <c r="L42">
-        <v>1.0913273647509731E-5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.1761403144367051</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>13</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1980,71 +2006,71 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>2.6973102405975148E-8</v>
+        <v>1.1565881574625391E-2</v>
       </c>
       <c r="F43">
-        <v>1.4816339347333239E-8</v>
+        <v>6.3531448359739921E-3</v>
       </c>
       <c r="G43">
-        <v>6.5238873374272422E-7</v>
+        <v>0.27973982086008309</v>
       </c>
       <c r="H43">
-        <v>1.81128846998095E-6</v>
+        <v>0.77666809052871033</v>
       </c>
       <c r="I43">
-        <v>2.1874734051460198E-6</v>
+        <v>0.93797361426088244</v>
       </c>
       <c r="J43">
-        <v>3.8584174091399478E-6</v>
+        <v>1.654462958984648</v>
       </c>
       <c r="K43">
-        <v>4.7122354667863194E-6</v>
+        <v>2.020574294358032</v>
       </c>
       <c r="L43">
-        <v>4.6610111674423023E-6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.998609665631274</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>14</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>4.7467218406874669E-5</v>
+        <v>6.4202688133367722</v>
       </c>
       <c r="D44">
-        <v>3.1454817611539962E-5</v>
+        <v>4.2544811202022768</v>
       </c>
       <c r="E44">
-        <v>1.575407639177613E-5</v>
+        <v>2.130847535114814</v>
       </c>
       <c r="F44">
-        <v>1.7041797110212283E-5</v>
+        <v>2.3050206475562591</v>
       </c>
       <c r="G44">
-        <v>1.7169694260229273E-5</v>
+        <v>2.3223196195863922</v>
       </c>
       <c r="H44">
-        <v>1.2149187458859345E-5</v>
+        <v>1.6432614332041831</v>
       </c>
       <c r="I44">
-        <v>1.3627762475504958E-5</v>
+        <v>1.843248906373117</v>
       </c>
       <c r="J44">
-        <v>1.178490947753865E-5</v>
+        <v>1.593990322712489</v>
       </c>
       <c r="K44">
-        <v>1.0480861438857243E-5</v>
+        <v>1.417608827549363</v>
       </c>
       <c r="L44">
-        <v>1.0985510498448055E-5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.48586609493753</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -2065,100 +2091,100 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <v>4.1249401610495894E-7</v>
+        <v>3.878736425699323E-2</v>
       </c>
       <c r="I45">
-        <v>3.0921225276550345E-7</v>
+        <v>2.9075641857770122E-2</v>
       </c>
       <c r="J45">
-        <v>3.4651274560458205E-7</v>
+        <v>3.2583057107999053E-2</v>
       </c>
       <c r="K45">
-        <v>3.5913483134926103E-7</v>
+        <v>3.3769928719094837E-2</v>
       </c>
       <c r="L45">
-        <v>3.9731779020866852E-7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.736032342996691E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46">
-        <v>8.8541604096199626E-7</v>
+        <v>0.16882640047840811</v>
       </c>
       <c r="D46">
-        <v>1.6897816836296716E-5</v>
+        <v>3.2219854401055121</v>
       </c>
       <c r="E46">
-        <v>3.2598558056060539E-5</v>
+        <v>6.2157188968607544</v>
       </c>
       <c r="F46">
-        <v>3.1310837337624385E-5</v>
+        <v>5.970183189738437</v>
       </c>
       <c r="G46">
-        <v>3.1182940187607395E-5</v>
+        <v>5.9457964444459588</v>
       </c>
       <c r="H46">
-        <v>3.5790952972872375E-5</v>
+        <v>6.8244277046719759</v>
       </c>
       <c r="I46">
-        <v>3.4415659719566209E-5</v>
+        <v>6.5621941344447512</v>
       </c>
       <c r="J46">
-        <v>3.6221212224693437E-5</v>
+        <v>6.9064672402089222</v>
       </c>
       <c r="K46">
-        <v>3.7512638177630169E-5</v>
+        <v>7.1527094416511066</v>
       </c>
       <c r="L46">
-        <v>3.6969806159179957E-5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.0492051323776872</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47">
-        <v>3.5307858967305202E-5</v>
+        <v>4.775631549554876</v>
       </c>
       <c r="D47">
-        <v>3.5307858967305202E-5</v>
+        <v>4.775631549554876</v>
       </c>
       <c r="E47">
-        <v>3.5307858967305202E-5</v>
+        <v>4.775631549554876</v>
       </c>
       <c r="F47">
-        <v>3.4958276205252673E-5</v>
+        <v>4.7283480688662154</v>
       </c>
       <c r="G47">
-        <v>3.4050106301818193E-5</v>
+        <v>4.6055118230543677</v>
       </c>
       <c r="H47">
-        <v>2.0006504778884667E-5</v>
+        <v>2.7060178162271109</v>
       </c>
       <c r="I47">
-        <v>2.3290945278084292E-5</v>
+        <v>3.150261056383302</v>
       </c>
       <c r="J47">
-        <v>2.3313526781951046E-5</v>
+        <v>3.1533153605936568</v>
       </c>
       <c r="K47">
-        <v>2.2504283488077949E-5</v>
+        <v>3.0438596213185942</v>
       </c>
       <c r="L47">
-        <v>1.9329505534813363E-5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.6144489971716829</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -2179,27 +2205,27 @@
         <v>0</v>
       </c>
       <c r="H48">
-        <v>1.4236340891621799E-5</v>
+        <v>1.1175503288175981</v>
       </c>
       <c r="I48">
-        <v>1.07350430072937E-5</v>
+        <v>0.8426990428230352</v>
       </c>
       <c r="J48">
-        <v>7.3533676952011805E-6</v>
+        <v>0.57723810832072697</v>
       </c>
       <c r="K48">
-        <v>8.3189900190981269E-6</v>
+        <v>0.65303929584495402</v>
       </c>
       <c r="L48">
-        <v>1.0033866100287165E-5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.78765677536471568</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2211,68 +2237,68 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>3.4958276205252673E-7</v>
+        <v>0.13692507949425081</v>
       </c>
       <c r="G49">
-        <v>1.257752665487006E-6</v>
+        <v>0.49263837465772248</v>
       </c>
       <c r="H49">
-        <v>1.065013296798731E-6</v>
+        <v>0.41714594126551657</v>
       </c>
       <c r="I49">
-        <v>1.281870681927207E-6</v>
+        <v>0.502084954056915</v>
       </c>
       <c r="J49">
-        <v>4.6409644901529689E-6</v>
+        <v>1.817779652558235</v>
       </c>
       <c r="K49">
-        <v>4.4845854601291204E-6</v>
+        <v>1.7565288889578501</v>
       </c>
       <c r="L49">
-        <v>5.9444873322046726E-6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.328345355862802</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50">
-        <v>3.7607604570539635E-5</v>
+        <v>5.0866880106369949</v>
       </c>
       <c r="D50">
-        <v>3.7607604570539635E-5</v>
+        <v>5.0866880106369949</v>
       </c>
       <c r="E50">
-        <v>3.247150951070144E-5</v>
+        <v>4.3919957147379689</v>
       </c>
       <c r="F50">
-        <v>3.0741574924228019E-5</v>
+        <v>4.1580101253687944</v>
       </c>
       <c r="G50">
-        <v>2.5901030478045263E-5</v>
+        <v>3.503293089265902</v>
       </c>
       <c r="H50">
-        <v>2.5996534405156056E-5</v>
+        <v>3.5162106543847331</v>
       </c>
       <c r="I50">
-        <v>2.1628388944619828E-5</v>
+        <v>2.9253888406435342</v>
       </c>
       <c r="J50">
-        <v>1.6611071314058277E-5</v>
+        <v>2.2467620116184368</v>
       </c>
       <c r="K50">
-        <v>1.800322952465774E-5</v>
+        <v>2.435061015493666</v>
       </c>
       <c r="L50">
-        <v>1.8593285081717893E-5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.5148701009693948</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -2308,12 +2334,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2322,71 +2348,71 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>5.1360950598382016E-6</v>
+        <v>1.4861859772921779</v>
       </c>
       <c r="F52">
-        <v>6.8660296463116151E-6</v>
+        <v>1.986761705368856</v>
       </c>
       <c r="G52">
-        <v>1.1706574092494371E-5</v>
+        <v>3.387426839982421</v>
       </c>
       <c r="H52">
-        <v>1.161107016538358E-5</v>
+        <v>3.359791721162626</v>
       </c>
       <c r="I52">
-        <v>1.5979215625919806E-5</v>
+        <v>4.6237629784286334</v>
       </c>
       <c r="J52">
-        <v>2.0996533256481354E-5</v>
+        <v>6.0755793913429796</v>
       </c>
       <c r="K52">
-        <v>1.9604375045881894E-5</v>
+        <v>5.6727429978066297</v>
       </c>
       <c r="L52">
-        <v>1.9014319488821745E-5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.5020038887151106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C53">
-        <v>2.9114022690837249E-5</v>
+        <v>3.9378724556922831</v>
       </c>
       <c r="D53">
-        <v>2.9581214444388848E-5</v>
+        <v>4.0010633639832358</v>
       </c>
       <c r="E53">
-        <v>1.7449928520730391E-5</v>
+        <v>2.3602232369355658</v>
       </c>
       <c r="F53">
-        <v>2.2232355136830906E-5</v>
+        <v>3.007079435506808</v>
       </c>
       <c r="G53">
-        <v>1.3491897101701966E-5</v>
+        <v>1.8248721770951819</v>
       </c>
       <c r="H53">
-        <v>9.6512754299257553E-6</v>
+        <v>1.3054015956979179</v>
       </c>
       <c r="I53">
-        <v>9.6041340452413746E-6</v>
+        <v>1.2990253981438009</v>
       </c>
       <c r="J53">
-        <v>1.0231132465421803E-5</v>
+        <v>1.383831260762302</v>
       </c>
       <c r="K53">
-        <v>1.0027108428434233E-5</v>
+        <v>1.356235601993879</v>
       </c>
       <c r="L53">
-        <v>1.0656425394473435E-5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.4413550639377459</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -2422,53 +2448,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>1.9963901273716976E-5</v>
+        <v>5.3470403924534544</v>
       </c>
       <c r="D55">
-        <v>1.9496709520165376E-5</v>
+        <v>5.2219098809862219</v>
       </c>
       <c r="E55">
-        <v>3.1627995443823833E-5</v>
+        <v>8.4710982513776472</v>
       </c>
       <c r="F55">
-        <v>2.6845568827723318E-5</v>
+        <v>7.1901948878702386</v>
       </c>
       <c r="G55">
-        <v>3.5586026862852269E-5</v>
+        <v>9.5311993599724669</v>
       </c>
       <c r="H55">
-        <v>3.9426648534628471E-5</v>
+        <v>10.55985397660071</v>
       </c>
       <c r="I55">
-        <v>3.9473789919312848E-5</v>
+        <v>10.57248011037124</v>
       </c>
       <c r="J55">
-        <v>3.884679149913243E-5</v>
+        <v>10.40454770914649</v>
       </c>
       <c r="K55">
-        <v>3.9050815536119993E-5</v>
+        <v>10.45919257799485</v>
       </c>
       <c r="L55">
-        <v>3.8421498570080786E-5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>10.29063918800699</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1.763114967830353</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2498,15 +2524,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B57">
         <v>2</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1.114715004849921</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2536,202 +2562,202 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>2.714980717333856</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="K58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="L58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.144942152001569</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C59">
-        <v>3.596550153127638E-5</v>
+        <v>4.8645822440656694</v>
       </c>
       <c r="D59">
-        <v>3.2372174093339721E-5</v>
+        <v>4.3785599141254172</v>
       </c>
       <c r="E59">
-        <v>2.316876691081765E-5</v>
+        <v>3.133735589179754</v>
       </c>
       <c r="F59">
-        <v>1.1794096210478745E-5</v>
+        <v>1.595232891731093</v>
       </c>
       <c r="G59">
-        <v>6.2378722351952938E-6</v>
+        <v>0.84371526112858153</v>
       </c>
       <c r="H59">
-        <v>9.2524635296339373E-6</v>
+        <v>1.2514595343813379</v>
       </c>
       <c r="I59">
-        <v>9.0754469961826628E-6</v>
+        <v>1.2275168268179719</v>
       </c>
       <c r="J59">
-        <v>8.7402797162197039E-6</v>
+        <v>1.1821831395487501</v>
       </c>
       <c r="K59">
-        <v>1.187618187121918E-5</v>
+        <v>1.606335543737297</v>
       </c>
       <c r="L59">
-        <v>1.3104573171959302E-5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.772483943062372</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>3.6738953177110282E-6</v>
+        <v>0.31072305298019998</v>
       </c>
       <c r="E60">
-        <v>2.7261864822550765E-6</v>
+        <v>0.23056971239110219</v>
       </c>
       <c r="F60">
-        <v>4.9359839971260183E-6</v>
+        <v>0.41746535609075902</v>
       </c>
       <c r="G60">
-        <v>8.1108902790770763E-6</v>
+        <v>0.68598595549327135</v>
       </c>
       <c r="H60">
-        <v>9.1595863351374586E-6</v>
+        <v>0.77468038252729909</v>
       </c>
       <c r="I60">
-        <v>8.8820259363934467E-6</v>
+        <v>0.75120545822328422</v>
       </c>
       <c r="J60">
-        <v>8.3135923189733795E-6</v>
+        <v>0.70312966570685875</v>
       </c>
       <c r="K60">
-        <v>7.1644437831736135E-6</v>
+        <v>0.60593937842510348</v>
       </c>
       <c r="L60">
-        <v>6.9099550283214742E-6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.58441575948158586</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B61">
         <v>3</v>
       </c>
       <c r="C61">
-        <v>1.4985625638031827E-6</v>
+        <v>0.5310502283105023</v>
       </c>
       <c r="D61">
-        <v>1.417994684028818E-6</v>
+        <v>0.50249914076692692</v>
       </c>
       <c r="E61">
-        <v>1.1569110702006839E-5</v>
+        <v>4.0997813691928817</v>
       </c>
       <c r="F61">
-        <v>2.0733983887474801E-5</v>
+        <v>7.3475656894068093</v>
       </c>
       <c r="G61">
-        <v>2.31153015808072E-5</v>
+        <v>8.1914405700888668</v>
       </c>
       <c r="H61">
-        <v>1.9052014230308172E-5</v>
+        <v>6.75152092489407</v>
       </c>
       <c r="I61">
-        <v>1.9506591162503453E-5</v>
+        <v>6.9126107515439097</v>
       </c>
       <c r="J61">
-        <v>2.0410192059886484E-5</v>
+        <v>7.2328225828330934</v>
       </c>
       <c r="K61">
-        <v>1.8423438440686764E-5</v>
+        <v>6.5287705875696531</v>
       </c>
       <c r="L61">
-        <v>1.7449535894798787E-5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.1836457447112956</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>3.7039942614757905E-5</v>
+        <v>5.0099078142500204</v>
       </c>
       <c r="D62">
-        <v>3.7039942614757905E-5</v>
+        <v>5.0099078142500204</v>
       </c>
       <c r="E62">
-        <v>3.6239499154112822E-5</v>
+        <v>4.9016423131378959</v>
       </c>
       <c r="F62">
-        <v>2.8943803978884688E-5</v>
+        <v>3.9148492003915871</v>
       </c>
       <c r="G62">
-        <v>1.8770323740955706E-5</v>
+        <v>2.5388158011980582</v>
       </c>
       <c r="H62">
-        <v>1.7338795086390913E-5</v>
+        <v>2.3451916731204538</v>
       </c>
       <c r="I62">
-        <v>1.5507854253602239E-5</v>
+        <v>2.097544291994041</v>
       </c>
       <c r="J62">
-        <v>1.3777875505273133E-5</v>
+        <v>1.8635527294291681</v>
       </c>
       <c r="K62">
-        <v>1.2658050422968892E-5</v>
+        <v>1.7120886602544521</v>
       </c>
       <c r="L62">
-        <v>1.3817769762642125E-5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.8689487030086991</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2746,27 +2772,27 @@
         <v>0</v>
       </c>
       <c r="G63">
-        <v>1.3330276644094868E-6</v>
+        <v>0.10165918131510771</v>
       </c>
       <c r="H63">
-        <v>4.4514076093966692E-6</v>
+        <v>0.3394726646363857</v>
       </c>
       <c r="I63">
-        <v>7.7833948113716906E-6</v>
+        <v>0.59357623663933345</v>
       </c>
       <c r="J63">
-        <v>9.8055918688698312E-6</v>
+        <v>0.74779276403161954</v>
       </c>
       <c r="K63">
-        <v>1.0812656823418499E-5</v>
+        <v>0.82459341981988921</v>
       </c>
       <c r="L63">
-        <v>1.0298355179693281E-5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.78537181516303367</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B64">
         <v>3</v>
@@ -2778,74 +2804,74 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>8.0044346064507953E-7</v>
+        <v>0.2785471630554669</v>
       </c>
       <c r="F64">
-        <v>8.0961386358732181E-6</v>
+        <v>2.8173838123542252</v>
       </c>
       <c r="G64">
-        <v>1.6936591209392716E-5</v>
+        <v>5.893782215928832</v>
       </c>
       <c r="H64">
-        <v>1.5249739918970325E-5</v>
+        <v>5.3067730584488739</v>
       </c>
       <c r="I64">
-        <v>1.3748693549783977E-5</v>
+        <v>4.7844223512363886</v>
       </c>
       <c r="J64">
-        <v>1.3456475240614942E-5</v>
+        <v>4.6827329940064581</v>
       </c>
       <c r="K64">
-        <v>1.3569235368370513E-5</v>
+        <v>4.7219725096454184</v>
       </c>
       <c r="L64">
-        <v>1.29238176724225E-5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.4973729257507236</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>4.8897960001728569</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>4.7319480828396072</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>4.4218568912111129</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>4.0131556991008486</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>2.4818866545407872</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>2.6704506990745172</v>
       </c>
       <c r="I65">
-        <v>0</v>
+        <v>2.8591759288398189</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>2.9322109016576632</v>
       </c>
       <c r="K65">
-        <v>0</v>
+        <v>2.838406766572418</v>
       </c>
       <c r="L65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.8683166598238592</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2854,112 +2880,112 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>1.395524831450477E-3</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>1.197619214559016E-3</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>2.973563001781435E-2</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>5.3563697162564032E-2</v>
       </c>
       <c r="I66">
-        <v>0</v>
+        <v>4.8976761295615977E-2</v>
       </c>
       <c r="J66">
-        <v>0</v>
+        <v>4.8291262449908313E-2</v>
       </c>
       <c r="K66">
-        <v>0</v>
+        <v>4.7674226765596343E-2</v>
       </c>
       <c r="L66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.6472704347461107E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B67">
         <v>3</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1.465208664359624E-2</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>0.26628023721601302</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>0.75774535656881903</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>1.4096682637250539</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>3.7922722832323701</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>3.442901557144054</v>
       </c>
       <c r="I67">
-        <v>0</v>
+        <v>3.1514410654693541</v>
       </c>
       <c r="J67">
-        <v>0</v>
+        <v>3.0364179829085929</v>
       </c>
       <c r="K67">
-        <v>0</v>
+        <v>3.187215918357075</v>
       </c>
       <c r="L67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.1215250285357259</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C68">
-        <v>4.0393353057246278E-5</v>
+        <v>5.4634797151286243</v>
       </c>
       <c r="D68">
-        <v>8.4152818869263087E-6</v>
+        <v>1.138224940651797</v>
       </c>
       <c r="E68">
-        <v>2.2608219994727401E-7</v>
+        <v>3.057917751004828E-2</v>
       </c>
       <c r="F68">
-        <v>4.4633539289774912E-7</v>
+        <v>6.0369941603631218E-2</v>
       </c>
       <c r="G68">
-        <v>9.7227554025259788E-6</v>
+        <v>1.315069755203909</v>
       </c>
       <c r="H68">
-        <v>1.0651512508847549E-5</v>
+        <v>1.440690562257934</v>
       </c>
       <c r="I68">
-        <v>1.5823647078695016E-5</v>
+        <v>2.1402574505583321</v>
       </c>
       <c r="J68">
-        <v>1.4431105883013533E-5</v>
+        <v>1.951906645308163</v>
       </c>
       <c r="K68">
-        <v>1.4494831299427109E-5</v>
+        <v>1.960525947583472</v>
       </c>
       <c r="L68">
-        <v>1.4293870810322304E-5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.933344654804672</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2992,9 +3018,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -3003,80 +3029,80 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <v>3.1978071170319974E-5</v>
+        <v>9.3012115946714076</v>
       </c>
       <c r="E70">
-        <v>4.0167270857299002E-5</v>
+        <v>11.68314009417092</v>
       </c>
       <c r="F70">
-        <v>3.9947017664348529E-5</v>
+        <v>11.61907676961569</v>
       </c>
       <c r="G70">
-        <v>3.0670597654720299E-5</v>
+        <v>8.9209169934664239</v>
       </c>
       <c r="H70">
-        <v>2.9741840548398729E-5</v>
+        <v>8.6507766738723681</v>
       </c>
       <c r="I70">
-        <v>2.4569705978551265E-5</v>
+        <v>7.1463983211555826</v>
       </c>
       <c r="J70">
-        <v>2.5962247174232748E-5</v>
+        <v>7.551435893507719</v>
       </c>
       <c r="K70">
-        <v>2.5898521757819165E-5</v>
+        <v>7.5329005797652382</v>
       </c>
       <c r="L70">
-        <v>2.6099482246923979E-5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.5913523863603576</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>3.2068250501841922</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <v>1.518319439183277E-6</v>
+        <v>0.20536318055366751</v>
       </c>
       <c r="F71">
-        <v>1.3247228344736617E-6</v>
+        <v>0.17917790395011959</v>
       </c>
       <c r="G71">
-        <v>2.2867310107072324E-6</v>
+        <v>0.30929614764212537</v>
       </c>
       <c r="H71">
-        <v>7.9000775661886936E-6</v>
+        <v>1.068540001362221</v>
       </c>
       <c r="I71">
-        <v>5.8747386762516323E-6</v>
+        <v>0.79459894165989509</v>
       </c>
       <c r="J71">
-        <v>5.5742602807180468E-6</v>
+        <v>0.75395716536304869</v>
       </c>
       <c r="K71">
-        <v>7.1191186762144388E-6</v>
+        <v>0.96290992287686339</v>
       </c>
       <c r="L71">
-        <v>7.0140098963811483E-6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.94869323515383019</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1.114715004849921</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -3106,88 +3132,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B73">
         <v>3</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>3.3025511710852129</v>
       </c>
       <c r="D73">
-        <v>7.1127426035585837E-5</v>
+        <v>9.9076535132556387</v>
       </c>
       <c r="E73">
-        <v>6.9609106596402553E-5</v>
+        <v>9.6961600885063408</v>
       </c>
       <c r="F73">
-        <v>6.9802703201112174E-5</v>
+        <v>9.7231270151577558</v>
       </c>
       <c r="G73">
-        <v>6.884069502487859E-5</v>
+        <v>9.5891246447883756</v>
       </c>
       <c r="H73">
-        <v>6.3227348469397146E-5</v>
+        <v>8.8072167954348437</v>
       </c>
       <c r="I73">
-        <v>6.5252687359334196E-5</v>
+        <v>9.0893352002029104</v>
       </c>
       <c r="J73">
-        <v>6.5553165754867786E-5</v>
+        <v>9.1311901638519029</v>
       </c>
       <c r="K73">
-        <v>6.4008307359371394E-5</v>
+        <v>8.9160000105914055</v>
       </c>
       <c r="L73">
-        <v>6.411341613920468E-5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.9306410770524423</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C74">
-        <v>3.7525236279850195E-5</v>
+        <v>5.0755471309800413</v>
       </c>
       <c r="D74">
-        <v>3.0821719118128809E-5</v>
+        <v>4.1688501805888141</v>
       </c>
       <c r="E74">
-        <v>2.8581079709583175E-5</v>
+        <v>3.8657882401710988</v>
       </c>
       <c r="F74">
-        <v>2.6490950058039732E-5</v>
+        <v>3.5830837829052542</v>
       </c>
       <c r="G74">
-        <v>2.3131248164509581E-5</v>
+        <v>3.1286609198622388</v>
       </c>
       <c r="H74">
-        <v>2.6511898302505238E-5</v>
+        <v>3.5859171775121008</v>
       </c>
       <c r="I74">
-        <v>2.3560579801346069E-5</v>
+        <v>3.1867309861326678</v>
       </c>
       <c r="J74">
-        <v>1.9245779519197543E-5</v>
+        <v>2.603124475850136</v>
       </c>
       <c r="K74">
-        <v>1.8100943749195667E-5</v>
+        <v>2.44827753859057</v>
       </c>
       <c r="L74">
-        <v>1.8159777741135295E-5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.4562352419549489</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -3196,229 +3222,229 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>6.2299908252972484E-9</v>
+        <v>7.3029601325039044E-4</v>
       </c>
       <c r="F75">
-        <v>2.0384286624062847E-8</v>
+        <v>2.389500028484566E-3</v>
       </c>
       <c r="G75">
-        <v>1.1427257137986762E-8</v>
+        <v>1.3395333258553589E-3</v>
       </c>
       <c r="H75">
-        <v>8.2206107889770553E-9</v>
+        <v>9.636417539004399E-4</v>
       </c>
       <c r="I75">
-        <v>7.3054880604757924E-9</v>
+        <v>8.563686456407011E-4</v>
       </c>
       <c r="J75">
-        <v>5.9675871170205414E-9</v>
+        <v>6.9953635607104716E-4</v>
       </c>
       <c r="K75">
-        <v>5.11341689341413E-8</v>
+        <v>5.9940826175604563E-3</v>
       </c>
       <c r="L75">
-        <v>5.0981078479672207E-8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.9761369493081867E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B76">
         <v>3</v>
       </c>
       <c r="C76">
-        <v>2.2701292365305624E-7</v>
+        <v>3.8943008397291277E-2</v>
       </c>
       <c r="D76">
-        <v>6.9305300853744433E-6</v>
+        <v>1.188900116210557</v>
       </c>
       <c r="E76">
-        <v>9.1649395030947796E-6</v>
+        <v>1.572202631842901</v>
       </c>
       <c r="F76">
-        <v>1.1240914858839456E-5</v>
+        <v>1.928326522987045</v>
       </c>
       <c r="G76">
-        <v>1.4609573781855682E-5</v>
+        <v>2.5062042517771559</v>
       </c>
       <c r="H76">
-        <v>1.1232130290209043E-5</v>
+        <v>1.926819571204583</v>
       </c>
       <c r="I76">
-        <v>1.4184363914096703E-5</v>
+        <v>2.4332614818930232</v>
       </c>
       <c r="J76">
-        <v>1.8500502097188691E-5</v>
+        <v>3.1736748592604842</v>
       </c>
       <c r="K76">
-        <v>1.9600171285373443E-5</v>
+        <v>3.3623179802801921</v>
       </c>
       <c r="L76">
-        <v>1.9541490383888283E-5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.3522515452837882</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C77">
-        <v>2.7773709184630078E-5</v>
+        <v>3.7565858058145718</v>
       </c>
       <c r="D77">
-        <v>2.6858875057207002E-5</v>
+        <v>3.6328481777251209</v>
       </c>
       <c r="E77">
-        <v>2.7870165214698516E-5</v>
+        <v>3.769632149427935</v>
       </c>
       <c r="F77">
-        <v>2.6572385332422734E-5</v>
+        <v>3.594098465668949</v>
       </c>
       <c r="G77">
-        <v>2.5355569676726646E-5</v>
+        <v>3.42951575220803</v>
       </c>
       <c r="H77">
-        <v>2.4447696559780618E-5</v>
+        <v>3.3067196488165731</v>
       </c>
       <c r="I77">
-        <v>2.375547151037517E-5</v>
+        <v>3.2130914345316461</v>
       </c>
       <c r="J77">
-        <v>2.4037879323515098E-5</v>
+        <v>3.2512890398727321</v>
       </c>
       <c r="K77">
-        <v>2.4223630967706385E-5</v>
+        <v>3.276413231435948</v>
       </c>
       <c r="L77">
-        <v>2.3895102849087974E-5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.2319775365487891</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C78">
-        <v>1.3777462720925715E-6</v>
+        <v>0.1778308467898061</v>
       </c>
       <c r="D78">
-        <v>2.369858161410438E-6</v>
+        <v>0.3058864263702647</v>
       </c>
       <c r="E78">
-        <v>1.00363544319094E-6</v>
+        <v>0.12954296763208009</v>
       </c>
       <c r="F78">
-        <v>5.8679240752009128E-7</v>
+        <v>7.5739483265403071E-2</v>
       </c>
       <c r="G78">
-        <v>5.5429386947977018E-7</v>
+        <v>7.154477582455962E-2</v>
       </c>
       <c r="H78">
-        <v>4.7623990727979003E-7</v>
+        <v>6.1470059982839421E-2</v>
       </c>
       <c r="I78">
-        <v>3.9615008319681535E-7</v>
+        <v>5.1132567859351372E-2</v>
       </c>
       <c r="J78">
-        <v>3.7020590080527526E-7</v>
+        <v>4.7783855532988598E-2</v>
       </c>
       <c r="K78">
-        <v>3.3998965624707616E-7</v>
+        <v>4.3883732218968567E-2</v>
       </c>
       <c r="L78">
-        <v>3.3467339169227091E-7</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.3197542136883468E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B79">
         <v>3</v>
       </c>
       <c r="C79">
-        <v>2.3652296516610667E-7</v>
+        <v>9.9860890259407323E-2</v>
       </c>
       <c r="D79">
-        <v>1.5924520327131838E-7</v>
+        <v>6.7233926976376826E-2</v>
       </c>
       <c r="E79">
-        <v>5.1417776399929951E-7</v>
+        <v>0.21708779622520691</v>
       </c>
       <c r="F79">
-        <v>2.2288006819459316E-6</v>
+        <v>0.94100807570033274</v>
       </c>
       <c r="G79">
-        <v>3.4781148756823397E-6</v>
+        <v>1.468473252338111</v>
       </c>
       <c r="H79">
-        <v>4.464041954828346E-6</v>
+        <v>1.884735393247909</v>
       </c>
       <c r="I79">
-        <v>5.2363568283167743E-6</v>
+        <v>2.2108096531954491</v>
       </c>
       <c r="J79">
-        <v>4.9798931975683813E-6</v>
+        <v>2.1025297385253938</v>
       </c>
       <c r="K79">
-        <v>4.8243577979352913E-6</v>
+        <v>2.0368621046729891</v>
       </c>
       <c r="L79">
-        <v>5.1582021811085094E-6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.1778124656172948</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1.695562670212331</v>
       </c>
       <c r="D80">
-        <v>3.7607604570539635E-5</v>
+        <v>5.0866880106369949</v>
       </c>
       <c r="E80">
-        <v>2.6155272148825468E-5</v>
+        <v>3.537681029506452</v>
       </c>
       <c r="F80">
-        <v>2.6366775281355212E-5</v>
+        <v>3.5662882875527151</v>
       </c>
       <c r="G80">
-        <v>2.4640710005222199E-5</v>
+        <v>3.332826049105321</v>
       </c>
       <c r="H80">
-        <v>2.0286709765632486E-5</v>
+        <v>2.7439174740991619</v>
       </c>
       <c r="I80">
-        <v>1.5938611677699823E-5</v>
+        <v>2.1558072058294648</v>
       </c>
       <c r="J80">
-        <v>1.8552371756009763E-5</v>
+        <v>2.509336291365424</v>
       </c>
       <c r="K80">
-        <v>1.9526092033647094E-5</v>
+        <v>2.641038677585787</v>
       </c>
       <c r="L80">
-        <v>2.1028218597156306E-5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.8442116599736962</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1.114715004849921</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -3448,88 +3474,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B82">
         <v>3</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>2.6820718601540521</v>
       </c>
       <c r="D82">
         <v>0</v>
       </c>
       <c r="E82">
-        <v>1.1452332421714167E-5</v>
+        <v>2.4502474065155848</v>
       </c>
       <c r="F82">
-        <v>1.1240829289184421E-5</v>
+        <v>2.4049959256060429</v>
       </c>
       <c r="G82">
-        <v>1.2966894565317436E-5</v>
+        <v>2.774290739150103</v>
       </c>
       <c r="H82">
-        <v>1.7320894804907152E-5</v>
+        <v>3.7058370305234818</v>
       </c>
       <c r="I82">
-        <v>2.1668992892839815E-5</v>
+        <v>4.636120545786456</v>
       </c>
       <c r="J82">
-        <v>1.9055232814529872E-5</v>
+        <v>4.076901810484121</v>
       </c>
       <c r="K82">
-        <v>1.8081512536892544E-5</v>
+        <v>3.868572581371911</v>
       </c>
       <c r="L82">
-        <v>1.6579385973383325E-5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.5471898637764911</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C83">
-        <v>4.1415969590341123E-5</v>
+        <v>5.6017956572837786</v>
       </c>
       <c r="D83">
-        <v>3.9397647485548673E-5</v>
+        <v>5.3288036661880804</v>
       </c>
       <c r="E83">
-        <v>1.675333492109285E-5</v>
+        <v>2.266004146088751</v>
       </c>
       <c r="F83">
-        <v>1.6685742215359336E-5</v>
+        <v>2.2568617662486239</v>
       </c>
       <c r="G83">
-        <v>9.2442929010097834E-6</v>
+        <v>1.2503544004825839</v>
       </c>
       <c r="H83">
-        <v>9.2442929010097834E-6</v>
+        <v>1.2503544004825839</v>
       </c>
       <c r="I83">
-        <v>6.4559862463312983E-6</v>
+        <v>0.87321668612140313</v>
       </c>
       <c r="J83">
-        <v>1.2011537719823847E-5</v>
+        <v>1.624643356216434</v>
       </c>
       <c r="K83">
-        <v>1.260617138061766E-5</v>
+        <v>1.7050716618110551</v>
       </c>
       <c r="L83">
-        <v>1.260617138061766E-5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.7050716618110551</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B84">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -3550,19 +3576,19 @@
         <v>0</v>
       </c>
       <c r="I84">
-        <v>2.2670599051952546E-6</v>
+        <v>0.18305443901553539</v>
       </c>
       <c r="J84">
-        <v>2.921832356846577E-6</v>
+        <v>0.23592423903501761</v>
       </c>
       <c r="K84">
-        <v>3.4253476017835582E-6</v>
+        <v>0.27658073006398792</v>
       </c>
       <c r="L84">
-        <v>3.4253476017835582E-6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.27658073006398792</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>27</v>
       </c>
@@ -3573,38 +3599,34 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <v>2.0183221047924522E-6</v>
+        <v>0.42012403824468231</v>
       </c>
       <c r="E85">
-        <v>2.4662634669248273E-5</v>
+        <v>5.1336531698261156</v>
       </c>
       <c r="F85">
-        <v>2.4730227374981787E-5</v>
+        <v>5.1477229362034533</v>
       </c>
       <c r="G85">
-        <v>3.217167668933134E-5</v>
+        <v>6.6966985575446989</v>
       </c>
       <c r="H85">
-        <v>3.217167668933134E-5</v>
+        <v>6.6966985575446989</v>
       </c>
       <c r="I85">
-        <v>3.2692923438814569E-5</v>
+        <v>6.8051987264695812</v>
       </c>
       <c r="J85">
-        <v>2.64825995136707E-5</v>
+        <v>5.5124881328315514</v>
       </c>
       <c r="K85">
-        <v>2.5384450607939901E-5</v>
+        <v>5.2839028382573527</v>
       </c>
       <c r="L85">
-        <v>2.5384450607939904E-5</v>
+        <v>5.2839028382573554</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L85">
-    <sortCondition ref="A2:A85"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Adjustment following integration tests"
This reverts commit 41e235505eeb094c0b1e41416da0217deb728d88.
</commit_message>
<xml_diff>
--- a/import/raw_data/primes/renewable_energy_system_utilization_primes.xlsx
+++ b/import/raw_data/primes/renewable_energy_system_utilization_primes.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\primes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_env\workspace\micat\back_end\import\public\primes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7139926-029C-4B50-8A59-6515398CBD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2025" yWindow="1125" windowWidth="43200" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -43,7 +47,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,27 +61,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -83,15 +75,13 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -114,44 +104,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -178,14 +168,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -212,6 +203,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -223,180 +215,162 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +408,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -442,387 +416,387 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>4.9289702887829936</v>
+        <v>3.7043000420312024E-5</v>
       </c>
       <c r="D2">
-        <v>3.7838133509921792</v>
+        <v>2.8436730460753743E-5</v>
       </c>
       <c r="E2">
-        <v>2.9846745189599941</v>
+        <v>2.2430912134312783E-5</v>
       </c>
       <c r="F2">
-        <v>2.8633257936731269</v>
+        <v>2.1518932426900993E-5</v>
       </c>
       <c r="G2">
-        <v>2.5647211461169608</v>
+        <v>1.9274810138295901E-5</v>
       </c>
       <c r="H2">
-        <v>2.374821237742506</v>
+        <v>1.7847643413079343E-5</v>
       </c>
       <c r="I2">
-        <v>2.2974292223725352</v>
+        <v>1.7266014332376066E-5</v>
       </c>
       <c r="J2">
-        <v>2.2067253251645589</v>
+        <v>1.6584341628840938E-5</v>
       </c>
       <c r="K2">
-        <v>2.1441783883415648</v>
+        <v>1.6114278700627293E-5</v>
       </c>
       <c r="L2">
-        <v>2.13645977565485</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.6056270525238428E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>5.0714892089427259E-7</v>
+      </c>
+      <c r="D3">
+        <v>5.8762529357517089E-7</v>
+      </c>
+      <c r="E3">
+        <v>1.0881206648293039E-6</v>
+      </c>
+      <c r="F3">
+        <v>1.7690035024015598E-6</v>
+      </c>
+      <c r="G3">
+        <v>2.6210318910775744E-6</v>
+      </c>
+      <c r="H3">
+        <v>3.2881105426590639E-6</v>
+      </c>
+      <c r="I3">
+        <v>3.5524392507317729E-6</v>
+      </c>
+      <c r="J3">
+        <v>3.6810722981053272E-6</v>
+      </c>
+      <c r="K3">
+        <v>3.6616001769732057E-6</v>
+      </c>
+      <c r="L3">
+        <v>3.6976757529965261E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2.2011970868875508E-6</v>
+      </c>
+      <c r="D4">
+        <v>1.0726990673764926E-5</v>
+      </c>
+      <c r="E4">
+        <v>1.6232313628951761E-5</v>
+      </c>
+      <c r="F4">
+        <v>1.6463410498791292E-5</v>
+      </c>
+      <c r="G4">
+        <v>1.7855504398720366E-5</v>
+      </c>
+      <c r="H4">
+        <v>1.8615592472355438E-5</v>
+      </c>
+      <c r="I4">
+        <v>1.8932892844986002E-5</v>
+      </c>
+      <c r="J4">
+        <v>1.9485932501147579E-5</v>
+      </c>
+      <c r="K4">
+        <v>1.9975467550493345E-5</v>
+      </c>
+      <c r="L4">
+        <v>1.9997400149858884E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>4.9238048114803618E-2</v>
-      </c>
-      <c r="D3">
-        <v>5.7051334009565517E-2</v>
-      </c>
-      <c r="E3">
-        <v>0.1056434026421734</v>
-      </c>
-      <c r="F3">
-        <v>0.17174892024400601</v>
-      </c>
-      <c r="G3">
-        <v>0.25447060823031281</v>
-      </c>
-      <c r="H3">
-        <v>0.3192359057390009</v>
-      </c>
-      <c r="I3">
-        <v>0.34489903763181468</v>
-      </c>
-      <c r="J3">
-        <v>0.35738775626019043</v>
-      </c>
-      <c r="K3">
-        <v>0.35549724797416249</v>
-      </c>
-      <c r="L3">
-        <v>0.35899975162708042</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0.57434484172056188</v>
-      </c>
-      <c r="D4">
-        <v>2.7989278185775639</v>
-      </c>
-      <c r="E4">
-        <v>4.2353979375655451</v>
-      </c>
-      <c r="F4">
-        <v>4.295696625002833</v>
-      </c>
-      <c r="G4">
-        <v>4.6589271396068037</v>
-      </c>
-      <c r="H4">
-        <v>4.8572522541302368</v>
-      </c>
-      <c r="I4">
-        <v>4.9400434923078507</v>
-      </c>
-      <c r="J4">
-        <v>5.0843447344253594</v>
-      </c>
-      <c r="K4">
-        <v>5.2120761093703978</v>
-      </c>
-      <c r="L4">
-        <v>5.2177988478685364</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>5.7324329244767958</v>
+        <v>4.2381815082829986E-5</v>
       </c>
       <c r="D5">
-        <v>5.1456932298117648</v>
+        <v>3.8043850109028021E-5</v>
       </c>
       <c r="E5">
-        <v>4.3492421990760608</v>
+        <v>3.2155418311938866E-5</v>
       </c>
       <c r="F5">
-        <v>3.9742376167493352</v>
+        <v>2.93828826237283E-5</v>
       </c>
       <c r="G5">
-        <v>4.2723871984664923</v>
+        <v>3.1587203303243795E-5</v>
       </c>
       <c r="H5">
-        <v>3.0721103303438642</v>
+        <v>2.2713150533125333E-5</v>
       </c>
       <c r="I5">
-        <v>3.105209521962963</v>
+        <v>2.2957864049545577E-5</v>
       </c>
       <c r="J5">
-        <v>3.1392165886515042</v>
+        <v>2.3209289793360049E-5</v>
       </c>
       <c r="K5">
-        <v>2.9694753717581208</v>
+        <v>2.1954335577394848E-5</v>
       </c>
       <c r="L5">
-        <v>2.5510629880486291</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.8860871334834992E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>0.41422713124311172</v>
+        <v>1.634260221702956E-6</v>
       </c>
       <c r="D7">
-        <v>1.513747735531362</v>
+        <v>5.9722251955049098E-6</v>
       </c>
       <c r="E7">
-        <v>3.006256809935246</v>
+        <v>1.1860656992594071E-5</v>
       </c>
       <c r="F7">
-        <v>3.7089964894214629</v>
+        <v>1.4633192680804638E-5</v>
       </c>
       <c r="G7">
-        <v>3.1502792060355298</v>
+        <v>1.2428872001289148E-5</v>
       </c>
       <c r="H7">
-        <v>5.3995375387359168</v>
+        <v>2.1302924771407601E-5</v>
       </c>
       <c r="I7">
-        <v>5.3375113225085258</v>
+        <v>2.1058211254987361E-5</v>
       </c>
       <c r="J7">
-        <v>5.2737837941762216</v>
+        <v>2.0806785511172896E-5</v>
       </c>
       <c r="K7">
-        <v>5.5918702762537382</v>
+        <v>2.2061739727138092E-5</v>
       </c>
       <c r="L7">
-        <v>6.3759539869026174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.5155203969697942E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>5.7540088840349499</v>
+        <v>4.2541333447942263E-5</v>
       </c>
       <c r="D8">
-        <v>2.2990270071261669</v>
+        <v>1.6997484099710846E-5</v>
       </c>
       <c r="E8">
-        <v>1.637044545269714</v>
+        <v>1.2103223904064955E-5</v>
       </c>
       <c r="F8">
-        <v>1.6241236410882529</v>
+        <v>1.2007695290135007E-5</v>
       </c>
       <c r="G8">
-        <v>2.1475020426372269</v>
+        <v>1.5877208797756263E-5</v>
       </c>
       <c r="H8">
-        <v>1.9054996883883131</v>
+        <v>1.4088003557587992E-5</v>
       </c>
       <c r="I8">
-        <v>1.667611528878046</v>
+        <v>1.2329215950373367E-5</v>
       </c>
       <c r="J8">
-        <v>1.4746731433006779</v>
+        <v>1.0902757222002617E-5</v>
       </c>
       <c r="K8">
-        <v>1.4296929547044901</v>
+        <v>1.0570203477268059E-5</v>
       </c>
       <c r="L8">
-        <v>1.375138195237521</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.0166861692361196E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0.34770466624767632</v>
+        <v>4.622746721678682E-6</v>
       </c>
       <c r="E9">
-        <v>0.42589063151834738</v>
+        <v>5.6622320945290487E-6</v>
       </c>
       <c r="F9">
-        <v>0.70810652142673769</v>
+        <v>9.4143030516393675E-6</v>
       </c>
       <c r="G9">
-        <v>0.53756484084889322</v>
+        <v>7.1469449419290075E-6</v>
       </c>
       <c r="H9">
-        <v>0.67569801091807657</v>
+        <v>8.9834306755934125E-6</v>
       </c>
       <c r="I9">
-        <v>0.63786681712810422</v>
+        <v>8.4804635197105733E-6</v>
       </c>
       <c r="J9">
-        <v>0.62338711933132651</v>
+        <v>8.2879553884757958E-6</v>
       </c>
       <c r="K9">
-        <v>0.58581242937842437</v>
+        <v>7.7883984608326586E-6</v>
       </c>
       <c r="L9">
-        <v>0.54463186094904292</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>7.2409012421206561E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>0.1454772705211764</v>
+        <v>5.0947704728074559E-7</v>
       </c>
       <c r="D10">
-        <v>6.119337962869837</v>
+        <v>2.1430579673833477E-5</v>
       </c>
       <c r="E10">
-        <v>7.2200394030762816</v>
+        <v>2.5285354496629004E-5</v>
       </c>
       <c r="F10">
-        <v>6.1759417298441814</v>
+        <v>2.1628812153448629E-5</v>
       </c>
       <c r="G10">
-        <v>5.7184585213603851</v>
+        <v>2.0026656755537735E-5</v>
       </c>
       <c r="H10">
-        <v>5.7049579384010114</v>
+        <v>1.9979376262041604E-5</v>
       </c>
       <c r="I10">
-        <v>6.3507846960142427</v>
+        <v>2.2241131025139061E-5</v>
       </c>
       <c r="J10">
-        <v>6.8130682886838629</v>
+        <v>2.3860097884744589E-5</v>
       </c>
       <c r="K10">
-        <v>7.0506711209118338</v>
+        <v>2.469220855712229E-5</v>
       </c>
       <c r="L10">
-        <v>7.3221759191943816</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.5643047560741154E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>2.7832821190277892</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>7.6931168683240037</v>
+        <v>5.6877814502062717E-5</v>
       </c>
       <c r="E11">
-        <v>5.6322397315070027</v>
+        <v>4.1641052926002553E-5</v>
       </c>
       <c r="F11">
-        <v>4.7627282470006218</v>
+        <v>3.5212460488157338E-5</v>
       </c>
       <c r="G11">
-        <v>3.147370678061769</v>
+        <v>2.326957573374657E-5</v>
       </c>
       <c r="H11">
-        <v>1.718991801627749</v>
+        <v>1.2709087681499121E-5</v>
       </c>
       <c r="I11">
-        <v>1.6692948816169191</v>
+        <v>1.2341661546412258E-5</v>
       </c>
       <c r="J11">
-        <v>1.373375424790314</v>
+        <v>1.0153828934348794E-5</v>
       </c>
       <c r="K11">
-        <v>1.069783625582917</v>
+        <v>7.9092721005946686E-6</v>
       </c>
       <c r="L11">
-        <v>1.4718685432087939</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.0882021865123346E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>1.114715004849921</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -852,88 +826,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>2.3921181455428031</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0.56443237142021196</v>
+        <v>4.8554231892004752E-6</v>
       </c>
       <c r="E13">
-        <v>2.33567272144131</v>
+        <v>2.0092184765260637E-5</v>
       </c>
       <c r="F13">
-        <v>3.082982591908956</v>
+        <v>2.6520777203105845E-5</v>
       </c>
       <c r="G13">
-        <v>4.4713169349428892</v>
+        <v>3.8463661957516614E-5</v>
       </c>
       <c r="H13">
-        <v>5.6989506719861813</v>
+        <v>4.9024150009764061E-5</v>
       </c>
       <c r="I13">
-        <v>5.7416631599954897</v>
+        <v>4.9391576144850919E-5</v>
       </c>
       <c r="J13">
-        <v>5.9959939364032202</v>
+        <v>5.1579408756914386E-5</v>
       </c>
       <c r="K13">
-        <v>6.2569187800463339</v>
+        <v>5.3823965590668515E-5</v>
       </c>
       <c r="L13">
-        <v>5.9113430940867966</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>5.0851215826139829E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>4.7920857353695858</v>
+        <v>3.5429510327159738E-5</v>
       </c>
       <c r="D14">
-        <v>0.55005688888415194</v>
+        <v>4.0667565860533169E-6</v>
       </c>
       <c r="E14">
-        <v>0.59762508910887646</v>
+        <v>4.418444375916347E-6</v>
       </c>
       <c r="F14">
-        <v>0.80305308778456319</v>
+        <v>5.9372430373945241E-6</v>
       </c>
       <c r="G14">
-        <v>1.3747529978829041</v>
+        <v>1.0164013798060665E-5</v>
       </c>
       <c r="H14">
-        <v>1.4510920356080299</v>
+        <v>1.0728414118673707E-5</v>
       </c>
       <c r="I14">
-        <v>1.95048154294551</v>
+        <v>1.4420569619335652E-5</v>
       </c>
       <c r="J14">
-        <v>2.0476571952482692</v>
+        <v>1.5139022077604027E-5</v>
       </c>
       <c r="K14">
-        <v>1.955629362020022</v>
+        <v>1.4458629186533428E-5</v>
       </c>
       <c r="L14">
-        <v>2.0116603470702792</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.487288520637609E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -966,316 +940,316 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>0.46178280722652371</v>
+        <v>1.6104322875981698E-6</v>
       </c>
       <c r="D16">
-        <v>9.4548839617756428</v>
+        <v>3.2973186028704584E-5</v>
       </c>
       <c r="E16">
-        <v>9.3540393772992267</v>
+        <v>3.2621498238841553E-5</v>
       </c>
       <c r="F16">
-        <v>8.9185320201067722</v>
+        <v>3.110269957736338E-5</v>
       </c>
       <c r="G16">
-        <v>7.7065282106982904</v>
+        <v>2.6875928816697243E-5</v>
       </c>
       <c r="H16">
-        <v>7.5446894507210223</v>
+        <v>2.6311528496084202E-5</v>
       </c>
       <c r="I16">
-        <v>6.4859836951655643</v>
+        <v>2.261937299542225E-5</v>
       </c>
       <c r="J16">
-        <v>6.279971312283716</v>
+        <v>2.1900920537153879E-5</v>
       </c>
       <c r="K16">
-        <v>6.4750703187275986</v>
+        <v>2.2581313428224482E-5</v>
       </c>
       <c r="L16">
-        <v>6.3562846304210554</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.216705740838182E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>5.4771777962463268</v>
+        <v>4.0494627603075015E-5</v>
       </c>
       <c r="D17">
-        <v>3.6920796938572309</v>
+        <v>2.729679368562529E-5</v>
       </c>
       <c r="E17">
-        <v>2.9999055577345368</v>
+        <v>2.2179316232551195E-5</v>
       </c>
       <c r="F17">
-        <v>2.8919309600343488</v>
+        <v>2.1381023519202086E-5</v>
       </c>
       <c r="G17">
-        <v>3.022645923760503</v>
+        <v>2.2347443448434197E-5</v>
       </c>
       <c r="H17">
-        <v>2.3857403980475231</v>
+        <v>1.7638585521681602E-5</v>
       </c>
       <c r="I17">
-        <v>2.3244976169930571</v>
+        <v>1.7185796931565558E-5</v>
       </c>
       <c r="J17">
-        <v>2.3484007076908631</v>
+        <v>1.7362520564132959E-5</v>
       </c>
       <c r="K17">
-        <v>2.1925006163514609</v>
+        <v>1.6209898469885625E-5</v>
       </c>
       <c r="L17">
-        <v>2.1987323803989018</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.6255972008813701E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>4.1800312292828773E-3</v>
+        <v>6.0391136472622327E-8</v>
       </c>
       <c r="E18">
-        <v>0.12244307550588331</v>
+        <v>1.7690002962662048E-6</v>
       </c>
       <c r="F18">
-        <v>0.20798005540156861</v>
+        <v>3.0047985817308089E-6</v>
       </c>
       <c r="G18">
-        <v>0.32938709233010588</v>
+        <v>4.7588306771192109E-6</v>
       </c>
       <c r="H18">
-        <v>0.34793427198574889</v>
+        <v>5.026791655477341E-6</v>
       </c>
       <c r="I18">
-        <v>0.41897198611144698</v>
+        <v>6.0531113294583808E-6</v>
       </c>
       <c r="J18">
-        <v>0.46561146866439429</v>
+        <v>6.7269367631383937E-6</v>
       </c>
       <c r="K18">
-        <v>0.43645878156414247</v>
+        <v>6.3057523727248775E-6</v>
       </c>
       <c r="L18">
-        <v>0.43576092633893182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>6.2956700867724202E-6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>1.214552829041422</v>
+        <v>4.5309907130297808E-6</v>
       </c>
       <c r="D19">
-        <v>4.7361045837427689</v>
+        <v>1.7668433494006876E-5</v>
       </c>
       <c r="E19">
-        <v>5.6498673547692739</v>
+        <v>2.1077301787287392E-5</v>
       </c>
       <c r="F19">
-        <v>5.5325919807972674</v>
+        <v>2.0639796215171896E-5</v>
       </c>
       <c r="G19">
-        <v>4.8033623460349171</v>
+        <v>1.7919344190551385E-5</v>
       </c>
       <c r="H19">
-        <v>5.9937651285087874</v>
+        <v>2.236024113894585E-5</v>
       </c>
       <c r="I19">
-        <v>5.8400274926208446</v>
+        <v>2.1786710055080858E-5</v>
       </c>
       <c r="J19">
-        <v>5.612033916805597</v>
+        <v>2.0936160988833441E-5</v>
       </c>
       <c r="K19">
-        <v>6.0338999587755664</v>
+        <v>2.2509967473494283E-5</v>
       </c>
       <c r="L19">
-        <v>6.0242523384446383</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.2473976220518675E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>3.2766168589566842</v>
+        <v>2.4225136454825605E-5</v>
       </c>
       <c r="D20">
-        <v>2.9267499697059609</v>
+        <v>2.1638452232056018E-5</v>
       </c>
       <c r="E20">
-        <v>2.5141245117955129</v>
+        <v>1.8587772688827899E-5</v>
       </c>
       <c r="F20">
-        <v>2.3588976249525242</v>
+        <v>1.7440127823072519E-5</v>
       </c>
       <c r="G20">
-        <v>2.1451830344567822</v>
+        <v>1.5860063586085393E-5</v>
       </c>
       <c r="H20">
-        <v>2.129188963076023</v>
+        <v>1.5741814007832762E-5</v>
       </c>
       <c r="I20">
-        <v>2.077750814724006</v>
+        <v>1.5361514382807952E-5</v>
       </c>
       <c r="J20">
-        <v>2.0542832324134919</v>
+        <v>1.518801061101876E-5</v>
       </c>
       <c r="K20">
-        <v>2.083488666332304</v>
+        <v>1.5403936260052652E-5</v>
       </c>
       <c r="L20">
-        <v>1.881250248342587</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.3908719247170362E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>0.47640824372113949</v>
+        <v>4.3643005252433348E-6</v>
       </c>
       <c r="D21">
-        <v>0.75602466753360709</v>
+        <v>6.9258223322121546E-6</v>
       </c>
       <c r="E21">
-        <v>0.67777081134160266</v>
+        <v>6.2089511399475072E-6</v>
       </c>
       <c r="F21">
-        <v>0.72330390830866353</v>
+        <v>6.626072635279182E-6</v>
       </c>
       <c r="G21">
-        <v>0.42637375738991062</v>
+        <v>3.9059425143280567E-6</v>
       </c>
       <c r="H21">
-        <v>0.329307025021008</v>
+        <v>3.016729540697772E-6</v>
       </c>
       <c r="I21">
-        <v>0.30266085959383388</v>
+        <v>2.7726282361922031E-6</v>
       </c>
       <c r="J21">
-        <v>0.29924239449958112</v>
+        <v>2.7413122184637069E-6</v>
       </c>
       <c r="K21">
-        <v>0.29443080707703018</v>
+        <v>2.6972340275586297E-6</v>
       </c>
       <c r="L21">
-        <v>0.41342735979324008</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.7873426148178577E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>1.368262981321504E-2</v>
+        <v>2.7428305385419503E-8</v>
       </c>
       <c r="D22">
-        <v>2.623491898201992E-2</v>
+        <v>5.2590721186185483E-8</v>
       </c>
       <c r="E22">
-        <v>1.9056803054861691</v>
+        <v>3.8201414566789525E-6</v>
       </c>
       <c r="F22">
-        <v>2.2701024127565348</v>
+        <v>4.5506648271026569E-6</v>
       </c>
       <c r="G22">
-        <v>4.4152574523319084</v>
+        <v>8.8508591850409099E-6</v>
       </c>
       <c r="H22">
-        <v>4.917830868895174</v>
+        <v>9.8583217369238235E-6</v>
       </c>
       <c r="I22">
-        <v>5.2293137204144351</v>
+        <v>1.0482722666454202E-5</v>
       </c>
       <c r="J22">
-        <v>5.3314882193129671</v>
+        <v>1.068754245597189E-5</v>
       </c>
       <c r="K22">
-        <v>5.2457619915756712</v>
+        <v>1.0515694997843076E-5</v>
       </c>
       <c r="L22">
-        <v>5.447850620243238</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.0920803423466138E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>4.8809763631479983</v>
+        <v>3.6086708797466337E-5</v>
       </c>
       <c r="D23">
-        <v>4.8809763631479983</v>
+        <v>3.6086708797466337E-5</v>
       </c>
       <c r="E23">
-        <v>4.8809763631479983</v>
+        <v>3.6086708797466337E-5</v>
       </c>
       <c r="F23">
-        <v>3.477416141619559</v>
+        <v>2.5709713453580391E-5</v>
       </c>
       <c r="G23">
-        <v>2.429489920368376</v>
+        <v>1.7962040534482077E-5</v>
       </c>
       <c r="H23">
-        <v>1.1554674746861351</v>
+        <v>8.5427617717553883E-6</v>
       </c>
       <c r="I23">
-        <v>1.8801126600748179</v>
+        <v>1.3900308672421357E-5</v>
       </c>
       <c r="J23">
-        <v>1.3549578182318081</v>
+        <v>1.0017661340987525E-5</v>
       </c>
       <c r="K23">
-        <v>1.1733866512012461</v>
+        <v>8.675244303257375E-6</v>
       </c>
       <c r="L23">
-        <v>1.3808201759173959</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.0208870496938814E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1293,27 +1267,27 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>1.568030898479303</v>
+        <v>1.8923839367812572E-5</v>
       </c>
       <c r="I24">
-        <v>0.97218719864916747</v>
+        <v>1.1732877458296698E-5</v>
       </c>
       <c r="J24">
-        <v>0.75904912546574299</v>
+        <v>9.1606126744841852E-6</v>
       </c>
       <c r="K24">
-        <v>0.96834857212991798</v>
+        <v>1.1686550851012522E-5</v>
       </c>
       <c r="L24">
-        <v>0.88455637664129605</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.067530161527308E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1325,71 +1299,71 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>4.0613657474014433</v>
+        <v>1.037699534388595E-5</v>
       </c>
       <c r="G25">
-        <v>7.0936628982559329</v>
+        <v>1.8124668262984267E-5</v>
       </c>
       <c r="H25">
-        <v>3.373752114221451</v>
+        <v>8.6201076578983843E-6</v>
       </c>
       <c r="I25">
-        <v>4.0913171386773932</v>
+        <v>1.0453522666748289E-5</v>
       </c>
       <c r="J25">
-        <v>6.617651409685255</v>
+        <v>1.6908434781994632E-5</v>
       </c>
       <c r="K25">
-        <v>6.154442932168438</v>
+        <v>1.5724913643196442E-5</v>
       </c>
       <c r="L25">
-        <v>5.949994166999879</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.5202536685254451E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>4.8710556794830628</v>
+        <v>3.6013361828365801E-5</v>
       </c>
       <c r="D26">
-        <v>4.2236715462440682</v>
+        <v>3.1227032012740872E-5</v>
       </c>
       <c r="E26">
-        <v>2.1735390754818522</v>
+        <v>1.6069709386226235E-5</v>
       </c>
       <c r="F26">
-        <v>2.782360946465817</v>
+        <v>2.0570935356834532E-5</v>
       </c>
       <c r="G26">
-        <v>2.617526639841099</v>
+        <v>1.9352259587800058E-5</v>
       </c>
       <c r="H26">
-        <v>2.032111965230432</v>
+        <v>1.5024090935327096E-5</v>
       </c>
       <c r="I26">
-        <v>2.1355388365986938</v>
+        <v>1.5788760770050962E-5</v>
       </c>
       <c r="J26">
-        <v>2.2572541141629898</v>
+        <v>1.6688642976166111E-5</v>
       </c>
       <c r="K26">
-        <v>2.183168203445172</v>
+        <v>1.6140900785432632E-5</v>
       </c>
       <c r="L26">
-        <v>2.0083334961518768</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.4848288672532698E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1407,100 +1381,100 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0.26932285439654863</v>
+        <v>2.5182759490081578E-6</v>
       </c>
       <c r="I27">
-        <v>0.2536333276032906</v>
+        <v>2.3715726249872191E-6</v>
       </c>
       <c r="J27">
-        <v>0.24418108355280849</v>
+        <v>2.2831903786686927E-6</v>
       </c>
       <c r="K27">
-        <v>0.211390779714698</v>
+        <v>1.9765879787305105E-6</v>
       </c>
       <c r="L27">
-        <v>0.36890136032244392</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.4493746375068418E-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C28">
-        <v>1.615823926264855E-2</v>
+        <v>7.334696910054131E-8</v>
       </c>
       <c r="D28">
-        <v>1.0705803005860419</v>
+        <v>4.8596767847254667E-6</v>
       </c>
       <c r="E28">
-        <v>4.409718217037077</v>
+        <v>2.0016999411240102E-5</v>
       </c>
       <c r="F28">
-        <v>3.418104151721876</v>
+        <v>1.5515773440631809E-5</v>
       </c>
       <c r="G28">
-        <v>3.6865767948471659</v>
+        <v>1.6734449209666287E-5</v>
       </c>
       <c r="H28">
-        <v>4.0852937384500922</v>
+        <v>1.8544341913131089E-5</v>
       </c>
       <c r="I28">
-        <v>3.9491565420711319</v>
+        <v>1.7926375402428162E-5</v>
       </c>
       <c r="J28">
-        <v>3.7703841855194988</v>
+        <v>1.7114875442631537E-5</v>
       </c>
       <c r="K28">
-        <v>3.9585951569898969</v>
+        <v>1.7969220033303196E-5</v>
       </c>
       <c r="L28">
-        <v>3.918902945341463</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.7789045487426799E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>4.1778070766617921</v>
+        <v>3.0887940479648834E-5</v>
       </c>
       <c r="D29">
-        <v>3.537499700816173</v>
+        <v>2.615393152450036E-5</v>
       </c>
       <c r="E29">
-        <v>4.1925366303827563</v>
+        <v>3.0996841051234936E-5</v>
       </c>
       <c r="F29">
-        <v>3.9557032237438858</v>
+        <v>2.9245851588672428E-5</v>
       </c>
       <c r="G29">
-        <v>3.9428003241884282</v>
+        <v>2.9150456089030943E-5</v>
       </c>
       <c r="H29">
-        <v>3.585598009430659</v>
+        <v>2.6509538584949669E-5</v>
       </c>
       <c r="I29">
-        <v>3.3848545241845929</v>
+        <v>2.5025374115365736E-5</v>
       </c>
       <c r="J29">
-        <v>3.3304430566864509</v>
+        <v>2.462309173643984E-5</v>
       </c>
       <c r="K29">
-        <v>3.226095945683582</v>
+        <v>2.3851618258910257E-5</v>
       </c>
       <c r="L29">
-        <v>3.2484374098131479</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.4016796258181032E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1509,112 +1483,112 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>0.48323536101051451</v>
+        <v>5.1291559698929063E-6</v>
       </c>
       <c r="E30">
-        <v>8.6798442076182841E-2</v>
+        <v>9.2129588037902295E-7</v>
       </c>
       <c r="F30">
-        <v>7.2187487054985885E-2</v>
+        <v>7.6621230574968485E-7</v>
       </c>
       <c r="G30">
-        <v>5.3497939584949021E-2</v>
+        <v>5.6783774189310772E-7</v>
       </c>
       <c r="H30">
-        <v>0.12215212390985609</v>
+        <v>1.296546871646887E-6</v>
       </c>
       <c r="I30">
-        <v>0.25210602951339428</v>
+        <v>2.675903401647976E-6</v>
       </c>
       <c r="J30">
-        <v>0.32101318667296352</v>
+        <v>3.4072976352451792E-6</v>
       </c>
       <c r="K30">
-        <v>0.3698850151462526</v>
+        <v>3.9260329162253689E-6</v>
       </c>
       <c r="L30">
-        <v>0.36617134946198221</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.8866153320592816E-6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>1.5067288038853092E-6</v>
+      </c>
+      <c r="D31">
+        <v>1.1115817891408777E-6</v>
+      </c>
+      <c r="E31">
+        <v>4.7653235192018425E-7</v>
+      </c>
+      <c r="F31">
+        <v>2.3826053891120343E-6</v>
+      </c>
+      <c r="G31">
+        <v>2.6763754526100888E-6</v>
+      </c>
+      <c r="H31">
+        <v>4.5885838269375901E-6</v>
+      </c>
+      <c r="I31">
+        <v>4.6933917665204363E-6</v>
+      </c>
+      <c r="J31">
+        <v>4.3642799118491263E-6</v>
+      </c>
+      <c r="K31">
+        <v>4.6170181083985214E-6</v>
+      </c>
+      <c r="L31">
+        <v>4.4912576932938377E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
         <v>1</v>
       </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <v>0.69382052300823405</v>
-      </c>
-      <c r="D31">
-        <v>0.51186268976832949</v>
-      </c>
-      <c r="E31">
-        <v>0.2194342636757432</v>
-      </c>
-      <c r="F31">
-        <v>1.0971453608195449</v>
-      </c>
-      <c r="G31">
-        <v>1.232420998064147</v>
-      </c>
-      <c r="H31">
-        <v>2.1129573035727929</v>
-      </c>
-      <c r="I31">
-        <v>2.1612194057303098</v>
-      </c>
-      <c r="J31">
-        <v>2.009669532556424</v>
-      </c>
-      <c r="K31">
-        <v>2.1260507600619198</v>
-      </c>
-      <c r="L31">
-        <v>2.0681404335607838</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>2</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
       <c r="C32">
-        <v>4.9274662932560336</v>
+        <v>3.6430424571730246E-5</v>
       </c>
       <c r="D32">
-        <v>4.3712685755523086</v>
+        <v>3.2318266761639015E-5</v>
       </c>
       <c r="E32">
-        <v>3.0158905049045019</v>
+        <v>2.2297498352427999E-5</v>
       </c>
       <c r="F32">
-        <v>3.1030183816523711</v>
+        <v>2.2941664208276165E-5</v>
       </c>
       <c r="G32">
-        <v>2.3841962265132208</v>
+        <v>1.7627168939353435E-5</v>
       </c>
       <c r="H32">
-        <v>2.395517140767629</v>
+        <v>1.7710868286702136E-5</v>
       </c>
       <c r="I32">
-        <v>2.5831477540069079</v>
+        <v>1.9098084859307897E-5</v>
       </c>
       <c r="J32">
-        <v>2.7295179679955162</v>
+        <v>2.0180249347689699E-5</v>
       </c>
       <c r="K32">
-        <v>2.829238768600181</v>
+        <v>2.0917518948018147E-5</v>
       </c>
       <c r="L32">
-        <v>2.6342958917336179</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.9476240337710187E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1629,106 +1603,106 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>6.1882007341698025E-4</v>
+        <v>7.5619395291796389E-9</v>
       </c>
       <c r="G33">
-        <v>0.1575011277896064</v>
+        <v>1.9246531508683876E-6</v>
       </c>
       <c r="H33">
-        <v>0.19612493011377991</v>
+        <v>2.3966334083116231E-6</v>
       </c>
       <c r="I33">
-        <v>0.1851430400245018</v>
+        <v>2.2624354526560054E-6</v>
       </c>
       <c r="J33">
-        <v>0.1697022885169972</v>
+        <v>2.0737505114256625E-6</v>
       </c>
       <c r="K33">
-        <v>0.21088547529021101</v>
+        <v>2.5770062740875609E-6</v>
       </c>
       <c r="L33">
-        <v>0.21101094835304529</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.5785395464464457E-6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34">
-        <v>0.16805386971851341</v>
+        <v>6.0951804302766173E-7</v>
       </c>
       <c r="D34">
-        <v>1.3018415250376461</v>
+        <v>4.7216758531188917E-6</v>
       </c>
       <c r="E34">
-        <v>4.0647275921274062</v>
+        <v>1.4742444262329914E-5</v>
       </c>
       <c r="F34">
-        <v>3.885035818817081</v>
+        <v>1.4090716466952561E-5</v>
       </c>
       <c r="G34">
-        <v>4.821754436756958</v>
+        <v>1.748812052453608E-5</v>
       </c>
       <c r="H34">
-        <v>4.668544685253833</v>
+        <v>1.6932440919744146E-5</v>
       </c>
       <c r="I34">
-        <v>4.3230674187207168</v>
+        <v>1.5679422302794002E-5</v>
       </c>
       <c r="J34">
-        <v>4.0767208222076867</v>
+        <v>1.4785942755642548E-5</v>
       </c>
       <c r="K34">
-        <v>3.7346881455391951</v>
+        <v>1.3545417392652196E-5</v>
       </c>
       <c r="L34">
-        <v>4.1316489545247146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.4985162730601275E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>5.3968519137246167</v>
+        <v>3.9900751190694494E-5</v>
       </c>
       <c r="D35">
-        <v>5.3968519137246167</v>
+        <v>3.9900751190694494E-5</v>
       </c>
       <c r="E35">
-        <v>4.8405948987819896</v>
+        <v>3.5788154976064178E-5</v>
       </c>
       <c r="F35">
-        <v>4.9845387627403444</v>
+        <v>3.6852380638180906E-5</v>
       </c>
       <c r="G35">
-        <v>4.5522684124788793</v>
+        <v>3.3656459762710099E-5</v>
       </c>
       <c r="H35">
-        <v>4.1956719420314412</v>
+        <v>3.1020021470486641E-5</v>
       </c>
       <c r="I35">
-        <v>3.579107511098091</v>
+        <v>2.6461552135958386E-5</v>
       </c>
       <c r="J35">
-        <v>3.0907606380089798</v>
+        <v>2.2851038564457683E-5</v>
       </c>
       <c r="K35">
-        <v>2.989675091895172</v>
+        <v>2.210367893907954E-5</v>
       </c>
       <c r="L35">
-        <v>2.6977691055037689</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.9945519271133552E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1761,15 +1735,15 @@
         <v>0</v>
       </c>
       <c r="L36">
-        <v>0.2053891063873198</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.4506053402540262E-6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1778,71 +1752,71 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>0.99882646478749182</v>
+        <v>4.1125962146303122E-6</v>
       </c>
       <c r="F37">
-        <v>0.74035792074548212</v>
+        <v>3.0483705525135859E-6</v>
       </c>
       <c r="G37">
-        <v>1.516551396397456</v>
+        <v>6.2442914279843937E-6</v>
       </c>
       <c r="H37">
-        <v>2.1568633068359202</v>
+        <v>8.8807297202078515E-6</v>
       </c>
       <c r="I37">
-        <v>3.2639790003366822</v>
+        <v>1.3439199054736107E-5</v>
       </c>
       <c r="J37">
-        <v>4.1408646264674944</v>
+        <v>1.7049712626236815E-5</v>
       </c>
       <c r="K37">
-        <v>4.3223758990514112</v>
+        <v>1.7797072251614948E-5</v>
       </c>
       <c r="L37">
-        <v>4.251349602821624</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.750462657930691E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>5.625532079560406</v>
+        <v>4.1591460986910369E-5</v>
       </c>
       <c r="D38">
-        <v>5.5873928790210128</v>
+        <v>4.130948498021945E-5</v>
       </c>
       <c r="E38">
-        <v>3.7239437709766068</v>
+        <v>2.7532375582884329E-5</v>
       </c>
       <c r="F38">
-        <v>1.0374439765557031</v>
+        <v>7.6701741394021926E-6</v>
       </c>
       <c r="G38">
-        <v>0.69530953712374055</v>
+        <v>5.1406585329380192E-6</v>
       </c>
       <c r="H38">
-        <v>0.47714462883469561</v>
+        <v>3.5276915915912479E-6</v>
       </c>
       <c r="I38">
-        <v>0.79263534663537938</v>
+        <v>5.8602211542286105E-6</v>
       </c>
       <c r="J38">
-        <v>1.0334062829034989</v>
+        <v>7.6403221048501382E-6</v>
       </c>
       <c r="K38">
-        <v>1.299251144473031</v>
+        <v>9.6058030641914605E-6</v>
       </c>
       <c r="L38">
-        <v>1.369447802122544</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.0124790691806121E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -1878,126 +1852,126 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>7.3177653067452428E-2</v>
+        <v>2.8197600669091774E-7</v>
       </c>
       <c r="E40">
-        <v>3.6485759416729802</v>
+        <v>1.405908540402604E-5</v>
       </c>
       <c r="F40">
-        <v>8.8031609130821931</v>
+        <v>3.3921286847508178E-5</v>
       </c>
       <c r="G40">
-        <v>9.4596139838622193</v>
+        <v>3.6450802453972348E-5</v>
       </c>
       <c r="H40">
-        <v>9.8782068160265641</v>
+        <v>3.8063769395319121E-5</v>
       </c>
       <c r="I40">
-        <v>9.2728750322789111</v>
+        <v>3.5731239832681757E-5</v>
       </c>
       <c r="J40">
-        <v>8.8109080326099996</v>
+        <v>3.3951138882060231E-5</v>
       </c>
       <c r="K40">
-        <v>8.3008317128505738</v>
+        <v>3.1985657922718916E-5</v>
       </c>
       <c r="L40">
-        <v>8.1661454428889062</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.1466670295104245E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>4.2396880611031493</v>
+        <v>3.134544752321821E-5</v>
       </c>
       <c r="D41">
-        <v>4.3740582412032891</v>
+        <v>3.2338891703146476E-5</v>
       </c>
       <c r="E41">
-        <v>4.4058673391209933</v>
+        <v>3.2574067120575858E-5</v>
       </c>
       <c r="F41">
-        <v>4.4280652012731698</v>
+        <v>3.2738183421867529E-5</v>
       </c>
       <c r="G41">
-        <v>3.786097766171383</v>
+        <v>2.7991901087274682E-5</v>
       </c>
       <c r="H41">
-        <v>2.8105752326058822</v>
+        <v>2.0779533115174878E-5</v>
       </c>
       <c r="I41">
-        <v>2.8089099631704948</v>
+        <v>2.0767221215113687E-5</v>
       </c>
       <c r="J41">
-        <v>2.5708451056621229</v>
+        <v>1.90071272198471E-5</v>
       </c>
       <c r="K41">
-        <v>2.4178804657074879</v>
+        <v>1.7876207910335818E-5</v>
       </c>
       <c r="L41">
-        <v>2.3485898812335191</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.7363919188104496E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42">
-        <v>0.17165381969924379</v>
+        <v>1.5927564798383231E-6</v>
       </c>
       <c r="D42">
-        <v>6.4588809886833382E-2</v>
+        <v>5.9931229991005322E-7</v>
       </c>
       <c r="E42">
-        <v>3.6336660027232182E-2</v>
+        <v>3.3716378007468944E-7</v>
       </c>
       <c r="F42">
-        <v>1.995974647665626E-2</v>
+        <v>1.8520424184166545E-7</v>
       </c>
       <c r="G42">
-        <v>0.46276174678164711</v>
+        <v>4.2939141820391241E-6</v>
       </c>
       <c r="H42">
-        <v>1.1151533447861079</v>
+        <v>1.0347382417900702E-5</v>
       </c>
       <c r="I42">
-        <v>1.0759381871949869</v>
+        <v>9.9835093827968231E-6</v>
       </c>
       <c r="J42">
-        <v>1.0855460191026369</v>
+        <v>1.0072659374069482E-5</v>
       </c>
       <c r="K42">
-        <v>1.115409647929865</v>
+        <v>1.0349760625934394E-5</v>
       </c>
       <c r="L42">
-        <v>1.1761403144367051</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.0913273647509731E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>13</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2006,71 +1980,71 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1.1565881574625391E-2</v>
+        <v>2.6973102405975148E-8</v>
       </c>
       <c r="F43">
-        <v>6.3531448359739921E-3</v>
+        <v>1.4816339347333239E-8</v>
       </c>
       <c r="G43">
-        <v>0.27973982086008309</v>
+        <v>6.5238873374272422E-7</v>
       </c>
       <c r="H43">
-        <v>0.77666809052871033</v>
+        <v>1.81128846998095E-6</v>
       </c>
       <c r="I43">
-        <v>0.93797361426088244</v>
+        <v>2.1874734051460198E-6</v>
       </c>
       <c r="J43">
-        <v>1.654462958984648</v>
+        <v>3.8584174091399478E-6</v>
       </c>
       <c r="K43">
-        <v>2.020574294358032</v>
+        <v>4.7122354667863194E-6</v>
       </c>
       <c r="L43">
-        <v>1.998609665631274</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+        <v>4.6610111674423023E-6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>14</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>6.4202688133367722</v>
+        <v>4.7467218406874669E-5</v>
       </c>
       <c r="D44">
-        <v>4.2544811202022768</v>
+        <v>3.1454817611539962E-5</v>
       </c>
       <c r="E44">
-        <v>2.130847535114814</v>
+        <v>1.575407639177613E-5</v>
       </c>
       <c r="F44">
-        <v>2.3050206475562591</v>
+        <v>1.7041797110212283E-5</v>
       </c>
       <c r="G44">
-        <v>2.3223196195863922</v>
+        <v>1.7169694260229273E-5</v>
       </c>
       <c r="H44">
-        <v>1.6432614332041831</v>
+        <v>1.2149187458859345E-5</v>
       </c>
       <c r="I44">
-        <v>1.843248906373117</v>
+        <v>1.3627762475504958E-5</v>
       </c>
       <c r="J44">
-        <v>1.593990322712489</v>
+        <v>1.178490947753865E-5</v>
       </c>
       <c r="K44">
-        <v>1.417608827549363</v>
+        <v>1.0480861438857243E-5</v>
       </c>
       <c r="L44">
-        <v>1.48586609493753</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.0985510498448055E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -2091,100 +2065,100 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <v>3.878736425699323E-2</v>
+        <v>4.1249401610495894E-7</v>
       </c>
       <c r="I45">
-        <v>2.9075641857770122E-2</v>
+        <v>3.0921225276550345E-7</v>
       </c>
       <c r="J45">
-        <v>3.2583057107999053E-2</v>
+        <v>3.4651274560458205E-7</v>
       </c>
       <c r="K45">
-        <v>3.3769928719094837E-2</v>
+        <v>3.5913483134926103E-7</v>
       </c>
       <c r="L45">
-        <v>3.736032342996691E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.9731779020866852E-7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C46">
-        <v>0.16882640047840811</v>
+        <v>8.8541604096199626E-7</v>
       </c>
       <c r="D46">
-        <v>3.2219854401055121</v>
+        <v>1.6897816836296716E-5</v>
       </c>
       <c r="E46">
-        <v>6.2157188968607544</v>
+        <v>3.2598558056060539E-5</v>
       </c>
       <c r="F46">
-        <v>5.970183189738437</v>
+        <v>3.1310837337624385E-5</v>
       </c>
       <c r="G46">
-        <v>5.9457964444459588</v>
+        <v>3.1182940187607395E-5</v>
       </c>
       <c r="H46">
-        <v>6.8244277046719759</v>
+        <v>3.5790952972872375E-5</v>
       </c>
       <c r="I46">
-        <v>6.5621941344447512</v>
+        <v>3.4415659719566209E-5</v>
       </c>
       <c r="J46">
-        <v>6.9064672402089222</v>
+        <v>3.6221212224693437E-5</v>
       </c>
       <c r="K46">
-        <v>7.1527094416511066</v>
+        <v>3.7512638177630169E-5</v>
       </c>
       <c r="L46">
-        <v>7.0492051323776872</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.6969806159179957E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47">
-        <v>4.775631549554876</v>
+        <v>3.5307858967305202E-5</v>
       </c>
       <c r="D47">
-        <v>4.775631549554876</v>
+        <v>3.5307858967305202E-5</v>
       </c>
       <c r="E47">
-        <v>4.775631549554876</v>
+        <v>3.5307858967305202E-5</v>
       </c>
       <c r="F47">
-        <v>4.7283480688662154</v>
+        <v>3.4958276205252673E-5</v>
       </c>
       <c r="G47">
-        <v>4.6055118230543677</v>
+        <v>3.4050106301818193E-5</v>
       </c>
       <c r="H47">
-        <v>2.7060178162271109</v>
+        <v>2.0006504778884667E-5</v>
       </c>
       <c r="I47">
-        <v>3.150261056383302</v>
+        <v>2.3290945278084292E-5</v>
       </c>
       <c r="J47">
-        <v>3.1533153605936568</v>
+        <v>2.3313526781951046E-5</v>
       </c>
       <c r="K47">
-        <v>3.0438596213185942</v>
+        <v>2.2504283488077949E-5</v>
       </c>
       <c r="L47">
-        <v>2.6144489971716829</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.9329505534813363E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -2205,27 +2179,27 @@
         <v>0</v>
       </c>
       <c r="H48">
-        <v>1.1175503288175981</v>
+        <v>1.4236340891621799E-5</v>
       </c>
       <c r="I48">
-        <v>0.8426990428230352</v>
+        <v>1.07350430072937E-5</v>
       </c>
       <c r="J48">
-        <v>0.57723810832072697</v>
+        <v>7.3533676952011805E-6</v>
       </c>
       <c r="K48">
-        <v>0.65303929584495402</v>
+        <v>8.3189900190981269E-6</v>
       </c>
       <c r="L48">
-        <v>0.78765677536471568</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.0033866100287165E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2237,68 +2211,68 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>0.13692507949425081</v>
+        <v>3.4958276205252673E-7</v>
       </c>
       <c r="G49">
-        <v>0.49263837465772248</v>
+        <v>1.257752665487006E-6</v>
       </c>
       <c r="H49">
-        <v>0.41714594126551657</v>
+        <v>1.065013296798731E-6</v>
       </c>
       <c r="I49">
-        <v>0.502084954056915</v>
+        <v>1.281870681927207E-6</v>
       </c>
       <c r="J49">
-        <v>1.817779652558235</v>
+        <v>4.6409644901529689E-6</v>
       </c>
       <c r="K49">
-        <v>1.7565288889578501</v>
+        <v>4.4845854601291204E-6</v>
       </c>
       <c r="L49">
-        <v>2.328345355862802</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+        <v>5.9444873322046726E-6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50">
-        <v>5.0866880106369949</v>
+        <v>3.7607604570539635E-5</v>
       </c>
       <c r="D50">
-        <v>5.0866880106369949</v>
+        <v>3.7607604570539635E-5</v>
       </c>
       <c r="E50">
-        <v>4.3919957147379689</v>
+        <v>3.247150951070144E-5</v>
       </c>
       <c r="F50">
-        <v>4.1580101253687944</v>
+        <v>3.0741574924228019E-5</v>
       </c>
       <c r="G50">
-        <v>3.503293089265902</v>
+        <v>2.5901030478045263E-5</v>
       </c>
       <c r="H50">
-        <v>3.5162106543847331</v>
+        <v>2.5996534405156056E-5</v>
       </c>
       <c r="I50">
-        <v>2.9253888406435342</v>
+        <v>2.1628388944619828E-5</v>
       </c>
       <c r="J50">
-        <v>2.2467620116184368</v>
+        <v>1.6611071314058277E-5</v>
       </c>
       <c r="K50">
-        <v>2.435061015493666</v>
+        <v>1.800322952465774E-5</v>
       </c>
       <c r="L50">
-        <v>2.5148701009693948</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.8593285081717893E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -2334,12 +2308,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2348,71 +2322,71 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>1.4861859772921779</v>
+        <v>5.1360950598382016E-6</v>
       </c>
       <c r="F52">
-        <v>1.986761705368856</v>
+        <v>6.8660296463116151E-6</v>
       </c>
       <c r="G52">
-        <v>3.387426839982421</v>
+        <v>1.1706574092494371E-5</v>
       </c>
       <c r="H52">
-        <v>3.359791721162626</v>
+        <v>1.161107016538358E-5</v>
       </c>
       <c r="I52">
-        <v>4.6237629784286334</v>
+        <v>1.5979215625919806E-5</v>
       </c>
       <c r="J52">
-        <v>6.0755793913429796</v>
+        <v>2.0996533256481354E-5</v>
       </c>
       <c r="K52">
-        <v>5.6727429978066297</v>
+        <v>1.9604375045881894E-5</v>
       </c>
       <c r="L52">
-        <v>5.5020038887151106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.9014319488821745E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53">
-        <v>3.9378724556922831</v>
+        <v>2.9114022690837249E-5</v>
       </c>
       <c r="D53">
-        <v>4.0010633639832358</v>
+        <v>2.9581214444388848E-5</v>
       </c>
       <c r="E53">
-        <v>2.3602232369355658</v>
+        <v>1.7449928520730391E-5</v>
       </c>
       <c r="F53">
-        <v>3.007079435506808</v>
+        <v>2.2232355136830906E-5</v>
       </c>
       <c r="G53">
-        <v>1.8248721770951819</v>
+        <v>1.3491897101701966E-5</v>
       </c>
       <c r="H53">
-        <v>1.3054015956979179</v>
+        <v>9.6512754299257553E-6</v>
       </c>
       <c r="I53">
-        <v>1.2990253981438009</v>
+        <v>9.6041340452413746E-6</v>
       </c>
       <c r="J53">
-        <v>1.383831260762302</v>
+        <v>1.0231132465421803E-5</v>
       </c>
       <c r="K53">
-        <v>1.356235601993879</v>
+        <v>1.0027108428434233E-5</v>
       </c>
       <c r="L53">
-        <v>1.4413550639377459</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.0656425394473435E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -2448,53 +2422,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C55">
-        <v>5.3470403924534544</v>
+        <v>1.9963901273716976E-5</v>
       </c>
       <c r="D55">
-        <v>5.2219098809862219</v>
+        <v>1.9496709520165376E-5</v>
       </c>
       <c r="E55">
-        <v>8.4710982513776472</v>
+        <v>3.1627995443823833E-5</v>
       </c>
       <c r="F55">
-        <v>7.1901948878702386</v>
+        <v>2.6845568827723318E-5</v>
       </c>
       <c r="G55">
-        <v>9.5311993599724669</v>
+        <v>3.5586026862852269E-5</v>
       </c>
       <c r="H55">
-        <v>10.55985397660071</v>
+        <v>3.9426648534628471E-5</v>
       </c>
       <c r="I55">
-        <v>10.57248011037124</v>
+        <v>3.9473789919312848E-5</v>
       </c>
       <c r="J55">
-        <v>10.40454770914649</v>
+        <v>3.884679149913243E-5</v>
       </c>
       <c r="K55">
-        <v>10.45919257799485</v>
+        <v>3.9050815536119993E-5</v>
       </c>
       <c r="L55">
-        <v>10.29063918800699</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.8421498570080786E-5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>1.763114967830353</v>
+        <v>0</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2524,15 +2498,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B57">
         <v>2</v>
       </c>
       <c r="C57">
-        <v>1.114715004849921</v>
+        <v>0</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2562,202 +2536,202 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
       <c r="C58">
-        <v>2.714980717333856</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>8.144942152001569</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>8.144942152001569</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>8.144942152001569</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>8.144942152001569</v>
+        <v>0</v>
       </c>
       <c r="H58">
-        <v>8.144942152001569</v>
+        <v>0</v>
       </c>
       <c r="I58">
-        <v>8.144942152001569</v>
+        <v>0</v>
       </c>
       <c r="J58">
-        <v>8.144942152001569</v>
+        <v>0</v>
       </c>
       <c r="K58">
-        <v>8.144942152001569</v>
+        <v>0</v>
       </c>
       <c r="L58">
-        <v>8.144942152001569</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
+        <v>19</v>
+      </c>
+      <c r="B59">
         <v>1</v>
       </c>
-      <c r="B59">
-        <v>3</v>
-      </c>
       <c r="C59">
-        <v>4.8645822440656694</v>
+        <v>3.596550153127638E-5</v>
       </c>
       <c r="D59">
-        <v>4.3785599141254172</v>
+        <v>3.2372174093339721E-5</v>
       </c>
       <c r="E59">
-        <v>3.133735589179754</v>
+        <v>2.316876691081765E-5</v>
       </c>
       <c r="F59">
-        <v>1.595232891731093</v>
+        <v>1.1794096210478745E-5</v>
       </c>
       <c r="G59">
-        <v>0.84371526112858153</v>
+        <v>6.2378722351952938E-6</v>
       </c>
       <c r="H59">
-        <v>1.2514595343813379</v>
+        <v>9.2524635296339373E-6</v>
       </c>
       <c r="I59">
-        <v>1.2275168268179719</v>
+        <v>9.0754469961826628E-6</v>
       </c>
       <c r="J59">
-        <v>1.1821831395487501</v>
+        <v>8.7402797162197039E-6</v>
       </c>
       <c r="K59">
-        <v>1.606335543737297</v>
+        <v>1.187618187121918E-5</v>
       </c>
       <c r="L59">
-        <v>1.772483943062372</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.3104573171959302E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
+        <v>19</v>
+      </c>
+      <c r="B60">
         <v>2</v>
       </c>
-      <c r="B60">
-        <v>3</v>
-      </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>0.31072305298019998</v>
+        <v>3.6738953177110282E-6</v>
       </c>
       <c r="E60">
-        <v>0.23056971239110219</v>
+        <v>2.7261864822550765E-6</v>
       </c>
       <c r="F60">
-        <v>0.41746535609075902</v>
+        <v>4.9359839971260183E-6</v>
       </c>
       <c r="G60">
-        <v>0.68598595549327135</v>
+        <v>8.1108902790770763E-6</v>
       </c>
       <c r="H60">
-        <v>0.77468038252729909</v>
+        <v>9.1595863351374586E-6</v>
       </c>
       <c r="I60">
-        <v>0.75120545822328422</v>
+        <v>8.8820259363934467E-6</v>
       </c>
       <c r="J60">
-        <v>0.70312966570685875</v>
+        <v>8.3135923189733795E-6</v>
       </c>
       <c r="K60">
-        <v>0.60593937842510348</v>
+        <v>7.1644437831736135E-6</v>
       </c>
       <c r="L60">
-        <v>0.58441575948158586</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+        <v>6.9099550283214742E-6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B61">
         <v>3</v>
       </c>
       <c r="C61">
-        <v>0.5310502283105023</v>
+        <v>1.4985625638031827E-6</v>
       </c>
       <c r="D61">
-        <v>0.50249914076692692</v>
+        <v>1.417994684028818E-6</v>
       </c>
       <c r="E61">
-        <v>4.0997813691928817</v>
+        <v>1.1569110702006839E-5</v>
       </c>
       <c r="F61">
-        <v>7.3475656894068093</v>
+        <v>2.0733983887474801E-5</v>
       </c>
       <c r="G61">
-        <v>8.1914405700888668</v>
+        <v>2.31153015808072E-5</v>
       </c>
       <c r="H61">
-        <v>6.75152092489407</v>
+        <v>1.9052014230308172E-5</v>
       </c>
       <c r="I61">
-        <v>6.9126107515439097</v>
+        <v>1.9506591162503453E-5</v>
       </c>
       <c r="J61">
-        <v>7.2328225828330934</v>
+        <v>2.0410192059886484E-5</v>
       </c>
       <c r="K61">
-        <v>6.5287705875696531</v>
+        <v>1.8423438440686764E-5</v>
       </c>
       <c r="L61">
-        <v>6.1836457447112956</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.7449535894798787E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C62">
-        <v>5.0099078142500204</v>
+        <v>3.7039942614757905E-5</v>
       </c>
       <c r="D62">
-        <v>5.0099078142500204</v>
+        <v>3.7039942614757905E-5</v>
       </c>
       <c r="E62">
-        <v>4.9016423131378959</v>
+        <v>3.6239499154112822E-5</v>
       </c>
       <c r="F62">
-        <v>3.9148492003915871</v>
+        <v>2.8943803978884688E-5</v>
       </c>
       <c r="G62">
-        <v>2.5388158011980582</v>
+        <v>1.8770323740955706E-5</v>
       </c>
       <c r="H62">
-        <v>2.3451916731204538</v>
+        <v>1.7338795086390913E-5</v>
       </c>
       <c r="I62">
-        <v>2.097544291994041</v>
+        <v>1.5507854253602239E-5</v>
       </c>
       <c r="J62">
-        <v>1.8635527294291681</v>
+        <v>1.3777875505273133E-5</v>
       </c>
       <c r="K62">
-        <v>1.7120886602544521</v>
+        <v>1.2658050422968892E-5</v>
       </c>
       <c r="L62">
-        <v>1.8689487030086991</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.3817769762642125E-5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2772,27 +2746,27 @@
         <v>0</v>
       </c>
       <c r="G63">
-        <v>0.10165918131510771</v>
+        <v>1.3330276644094868E-6</v>
       </c>
       <c r="H63">
-        <v>0.3394726646363857</v>
+        <v>4.4514076093966692E-6</v>
       </c>
       <c r="I63">
-        <v>0.59357623663933345</v>
+        <v>7.7833948113716906E-6</v>
       </c>
       <c r="J63">
-        <v>0.74779276403161954</v>
+        <v>9.8055918688698312E-6</v>
       </c>
       <c r="K63">
-        <v>0.82459341981988921</v>
+        <v>1.0812656823418499E-5</v>
       </c>
       <c r="L63">
-        <v>0.78537181516303367</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.0298355179693281E-5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B64">
         <v>3</v>
@@ -2804,74 +2778,74 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>0.2785471630554669</v>
+        <v>8.0044346064507953E-7</v>
       </c>
       <c r="F64">
-        <v>2.8173838123542252</v>
+        <v>8.0961386358732181E-6</v>
       </c>
       <c r="G64">
-        <v>5.893782215928832</v>
+        <v>1.6936591209392716E-5</v>
       </c>
       <c r="H64">
-        <v>5.3067730584488739</v>
+        <v>1.5249739918970325E-5</v>
       </c>
       <c r="I64">
-        <v>4.7844223512363886</v>
+        <v>1.3748693549783977E-5</v>
       </c>
       <c r="J64">
-        <v>4.6827329940064581</v>
+        <v>1.3456475240614942E-5</v>
       </c>
       <c r="K64">
-        <v>4.7219725096454184</v>
+        <v>1.3569235368370513E-5</v>
       </c>
       <c r="L64">
-        <v>4.4973729257507236</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.29238176724225E-5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C65">
-        <v>4.8897960001728569</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>4.7319480828396072</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>4.4218568912111129</v>
+        <v>0</v>
       </c>
       <c r="F65">
-        <v>4.0131556991008486</v>
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>2.4818866545407872</v>
+        <v>0</v>
       </c>
       <c r="H65">
-        <v>2.6704506990745172</v>
+        <v>0</v>
       </c>
       <c r="I65">
-        <v>2.8591759288398189</v>
+        <v>0</v>
       </c>
       <c r="J65">
-        <v>2.9322109016576632</v>
+        <v>0</v>
       </c>
       <c r="K65">
-        <v>2.838406766572418</v>
+        <v>0</v>
       </c>
       <c r="L65">
-        <v>2.8683166598238592</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2880,112 +2854,112 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>1.395524831450477E-3</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>1.197619214559016E-3</v>
+        <v>0</v>
       </c>
       <c r="G66">
-        <v>2.973563001781435E-2</v>
+        <v>0</v>
       </c>
       <c r="H66">
-        <v>5.3563697162564032E-2</v>
+        <v>0</v>
       </c>
       <c r="I66">
-        <v>4.8976761295615977E-2</v>
+        <v>0</v>
       </c>
       <c r="J66">
-        <v>4.8291262449908313E-2</v>
+        <v>0</v>
       </c>
       <c r="K66">
-        <v>4.7674226765596343E-2</v>
+        <v>0</v>
       </c>
       <c r="L66">
-        <v>5.6472704347461107E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B67">
         <v>3</v>
       </c>
       <c r="C67">
-        <v>1.465208664359624E-2</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>0.26628023721601302</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>0.75774535656881903</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>1.4096682637250539</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>3.7922722832323701</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>3.442901557144054</v>
+        <v>0</v>
       </c>
       <c r="I67">
-        <v>3.1514410654693541</v>
+        <v>0</v>
       </c>
       <c r="J67">
-        <v>3.0364179829085929</v>
+        <v>0</v>
       </c>
       <c r="K67">
-        <v>3.187215918357075</v>
+        <v>0</v>
       </c>
       <c r="L67">
-        <v>3.1215250285357259</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>5.4634797151286243</v>
+        <v>4.0393353057246278E-5</v>
       </c>
       <c r="D68">
-        <v>1.138224940651797</v>
+        <v>8.4152818869263087E-6</v>
       </c>
       <c r="E68">
-        <v>3.057917751004828E-2</v>
+        <v>2.2608219994727401E-7</v>
       </c>
       <c r="F68">
-        <v>6.0369941603631218E-2</v>
+        <v>4.4633539289774912E-7</v>
       </c>
       <c r="G68">
-        <v>1.315069755203909</v>
+        <v>9.7227554025259788E-6</v>
       </c>
       <c r="H68">
-        <v>1.440690562257934</v>
+        <v>1.0651512508847549E-5</v>
       </c>
       <c r="I68">
-        <v>2.1402574505583321</v>
+        <v>1.5823647078695016E-5</v>
       </c>
       <c r="J68">
-        <v>1.951906645308163</v>
+        <v>1.4431105883013533E-5</v>
       </c>
       <c r="K68">
-        <v>1.960525947583472</v>
+        <v>1.4494831299427109E-5</v>
       </c>
       <c r="L68">
-        <v>1.933344654804672</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.4293870810322304E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -3018,9 +2992,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -3029,80 +3003,80 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <v>9.3012115946714076</v>
+        <v>3.1978071170319974E-5</v>
       </c>
       <c r="E70">
-        <v>11.68314009417092</v>
+        <v>4.0167270857299002E-5</v>
       </c>
       <c r="F70">
-        <v>11.61907676961569</v>
+        <v>3.9947017664348529E-5</v>
       </c>
       <c r="G70">
-        <v>8.9209169934664239</v>
+        <v>3.0670597654720299E-5</v>
       </c>
       <c r="H70">
-        <v>8.6507766738723681</v>
+        <v>2.9741840548398729E-5</v>
       </c>
       <c r="I70">
-        <v>7.1463983211555826</v>
+        <v>2.4569705978551265E-5</v>
       </c>
       <c r="J70">
-        <v>7.551435893507719</v>
+        <v>2.5962247174232748E-5</v>
       </c>
       <c r="K70">
-        <v>7.5329005797652382</v>
+        <v>2.5898521757819165E-5</v>
       </c>
       <c r="L70">
-        <v>7.5913523863603576</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.6099482246923979E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C71">
-        <v>3.2068250501841922</v>
+        <v>0</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <v>0.20536318055366751</v>
+        <v>1.518319439183277E-6</v>
       </c>
       <c r="F71">
-        <v>0.17917790395011959</v>
+        <v>1.3247228344736617E-6</v>
       </c>
       <c r="G71">
-        <v>0.30929614764212537</v>
+        <v>2.2867310107072324E-6</v>
       </c>
       <c r="H71">
-        <v>1.068540001362221</v>
+        <v>7.9000775661886936E-6</v>
       </c>
       <c r="I71">
-        <v>0.79459894165989509</v>
+        <v>5.8747386762516323E-6</v>
       </c>
       <c r="J71">
-        <v>0.75395716536304869</v>
+        <v>5.5742602807180468E-6</v>
       </c>
       <c r="K71">
-        <v>0.96290992287686339</v>
+        <v>7.1191186762144388E-6</v>
       </c>
       <c r="L71">
-        <v>0.94869323515383019</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+        <v>7.0140098963811483E-6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B72">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C72">
-        <v>1.114715004849921</v>
+        <v>0</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -3132,88 +3106,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B73">
         <v>3</v>
       </c>
       <c r="C73">
-        <v>3.3025511710852129</v>
+        <v>0</v>
       </c>
       <c r="D73">
-        <v>9.9076535132556387</v>
+        <v>7.1127426035585837E-5</v>
       </c>
       <c r="E73">
-        <v>9.6961600885063408</v>
+        <v>6.9609106596402553E-5</v>
       </c>
       <c r="F73">
-        <v>9.7231270151577558</v>
+        <v>6.9802703201112174E-5</v>
       </c>
       <c r="G73">
-        <v>9.5891246447883756</v>
+        <v>6.884069502487859E-5</v>
       </c>
       <c r="H73">
-        <v>8.8072167954348437</v>
+        <v>6.3227348469397146E-5</v>
       </c>
       <c r="I73">
-        <v>9.0893352002029104</v>
+        <v>6.5252687359334196E-5</v>
       </c>
       <c r="J73">
-        <v>9.1311901638519029</v>
+        <v>6.5553165754867786E-5</v>
       </c>
       <c r="K73">
-        <v>8.9160000105914055</v>
+        <v>6.4008307359371394E-5</v>
       </c>
       <c r="L73">
-        <v>8.9306410770524423</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+        <v>6.411341613920468E-5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B74">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C74">
-        <v>5.0755471309800413</v>
+        <v>3.7525236279850195E-5</v>
       </c>
       <c r="D74">
-        <v>4.1688501805888141</v>
+        <v>3.0821719118128809E-5</v>
       </c>
       <c r="E74">
-        <v>3.8657882401710988</v>
+        <v>2.8581079709583175E-5</v>
       </c>
       <c r="F74">
-        <v>3.5830837829052542</v>
+        <v>2.6490950058039732E-5</v>
       </c>
       <c r="G74">
-        <v>3.1286609198622388</v>
+        <v>2.3131248164509581E-5</v>
       </c>
       <c r="H74">
-        <v>3.5859171775121008</v>
+        <v>2.6511898302505238E-5</v>
       </c>
       <c r="I74">
-        <v>3.1867309861326678</v>
+        <v>2.3560579801346069E-5</v>
       </c>
       <c r="J74">
-        <v>2.603124475850136</v>
+        <v>1.9245779519197543E-5</v>
       </c>
       <c r="K74">
-        <v>2.44827753859057</v>
+        <v>1.8100943749195667E-5</v>
       </c>
       <c r="L74">
-        <v>2.4562352419549489</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.8159777741135295E-5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B75">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -3222,229 +3196,229 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>7.3029601325039044E-4</v>
+        <v>6.2299908252972484E-9</v>
       </c>
       <c r="F75">
-        <v>2.389500028484566E-3</v>
+        <v>2.0384286624062847E-8</v>
       </c>
       <c r="G75">
-        <v>1.3395333258553589E-3</v>
+        <v>1.1427257137986762E-8</v>
       </c>
       <c r="H75">
-        <v>9.636417539004399E-4</v>
+        <v>8.2206107889770553E-9</v>
       </c>
       <c r="I75">
-        <v>8.563686456407011E-4</v>
+        <v>7.3054880604757924E-9</v>
       </c>
       <c r="J75">
-        <v>6.9953635607104716E-4</v>
+        <v>5.9675871170205414E-9</v>
       </c>
       <c r="K75">
-        <v>5.9940826175604563E-3</v>
+        <v>5.11341689341413E-8</v>
       </c>
       <c r="L75">
-        <v>5.9761369493081867E-3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+        <v>5.0981078479672207E-8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B76">
         <v>3</v>
       </c>
       <c r="C76">
-        <v>3.8943008397291277E-2</v>
+        <v>2.2701292365305624E-7</v>
       </c>
       <c r="D76">
-        <v>1.188900116210557</v>
+        <v>6.9305300853744433E-6</v>
       </c>
       <c r="E76">
-        <v>1.572202631842901</v>
+        <v>9.1649395030947796E-6</v>
       </c>
       <c r="F76">
-        <v>1.928326522987045</v>
+        <v>1.1240914858839456E-5</v>
       </c>
       <c r="G76">
-        <v>2.5062042517771559</v>
+        <v>1.4609573781855682E-5</v>
       </c>
       <c r="H76">
-        <v>1.926819571204583</v>
+        <v>1.1232130290209043E-5</v>
       </c>
       <c r="I76">
-        <v>2.4332614818930232</v>
+        <v>1.4184363914096703E-5</v>
       </c>
       <c r="J76">
-        <v>3.1736748592604842</v>
+        <v>1.8500502097188691E-5</v>
       </c>
       <c r="K76">
-        <v>3.3623179802801921</v>
+        <v>1.9600171285373443E-5</v>
       </c>
       <c r="L76">
-        <v>3.3522515452837882</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.9541490383888283E-5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B77">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C77">
-        <v>3.7565858058145718</v>
+        <v>2.7773709184630078E-5</v>
       </c>
       <c r="D77">
-        <v>3.6328481777251209</v>
+        <v>2.6858875057207002E-5</v>
       </c>
       <c r="E77">
-        <v>3.769632149427935</v>
+        <v>2.7870165214698516E-5</v>
       </c>
       <c r="F77">
-        <v>3.594098465668949</v>
+        <v>2.6572385332422734E-5</v>
       </c>
       <c r="G77">
-        <v>3.42951575220803</v>
+        <v>2.5355569676726646E-5</v>
       </c>
       <c r="H77">
-        <v>3.3067196488165731</v>
+        <v>2.4447696559780618E-5</v>
       </c>
       <c r="I77">
-        <v>3.2130914345316461</v>
+        <v>2.375547151037517E-5</v>
       </c>
       <c r="J77">
-        <v>3.2512890398727321</v>
+        <v>2.4037879323515098E-5</v>
       </c>
       <c r="K77">
-        <v>3.276413231435948</v>
+        <v>2.4223630967706385E-5</v>
       </c>
       <c r="L77">
-        <v>3.2319775365487891</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.3895102849087974E-5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B78">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C78">
-        <v>0.1778308467898061</v>
+        <v>1.3777462720925715E-6</v>
       </c>
       <c r="D78">
-        <v>0.3058864263702647</v>
+        <v>2.369858161410438E-6</v>
       </c>
       <c r="E78">
-        <v>0.12954296763208009</v>
+        <v>1.00363544319094E-6</v>
       </c>
       <c r="F78">
-        <v>7.5739483265403071E-2</v>
+        <v>5.8679240752009128E-7</v>
       </c>
       <c r="G78">
-        <v>7.154477582455962E-2</v>
+        <v>5.5429386947977018E-7</v>
       </c>
       <c r="H78">
-        <v>6.1470059982839421E-2</v>
+        <v>4.7623990727979003E-7</v>
       </c>
       <c r="I78">
-        <v>5.1132567859351372E-2</v>
+        <v>3.9615008319681535E-7</v>
       </c>
       <c r="J78">
-        <v>4.7783855532988598E-2</v>
+        <v>3.7020590080527526E-7</v>
       </c>
       <c r="K78">
-        <v>4.3883732218968567E-2</v>
+        <v>3.3998965624707616E-7</v>
       </c>
       <c r="L78">
-        <v>4.3197542136883468E-2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.3467339169227091E-7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B79">
         <v>3</v>
       </c>
       <c r="C79">
-        <v>9.9860890259407323E-2</v>
+        <v>2.3652296516610667E-7</v>
       </c>
       <c r="D79">
-        <v>6.7233926976376826E-2</v>
+        <v>1.5924520327131838E-7</v>
       </c>
       <c r="E79">
-        <v>0.21708779622520691</v>
+        <v>5.1417776399929951E-7</v>
       </c>
       <c r="F79">
-        <v>0.94100807570033274</v>
+        <v>2.2288006819459316E-6</v>
       </c>
       <c r="G79">
-        <v>1.468473252338111</v>
+        <v>3.4781148756823397E-6</v>
       </c>
       <c r="H79">
-        <v>1.884735393247909</v>
+        <v>4.464041954828346E-6</v>
       </c>
       <c r="I79">
-        <v>2.2108096531954491</v>
+        <v>5.2363568283167743E-6</v>
       </c>
       <c r="J79">
-        <v>2.1025297385253938</v>
+        <v>4.9798931975683813E-6</v>
       </c>
       <c r="K79">
-        <v>2.0368621046729891</v>
+        <v>4.8243577979352913E-6</v>
       </c>
       <c r="L79">
-        <v>2.1778124656172948</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+        <v>5.1582021811085094E-6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B80">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C80">
-        <v>1.695562670212331</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>5.0866880106369949</v>
+        <v>3.7607604570539635E-5</v>
       </c>
       <c r="E80">
-        <v>3.537681029506452</v>
+        <v>2.6155272148825468E-5</v>
       </c>
       <c r="F80">
-        <v>3.5662882875527151</v>
+        <v>2.6366775281355212E-5</v>
       </c>
       <c r="G80">
-        <v>3.332826049105321</v>
+        <v>2.4640710005222199E-5</v>
       </c>
       <c r="H80">
-        <v>2.7439174740991619</v>
+        <v>2.0286709765632486E-5</v>
       </c>
       <c r="I80">
-        <v>2.1558072058294648</v>
+        <v>1.5938611677699823E-5</v>
       </c>
       <c r="J80">
-        <v>2.509336291365424</v>
+        <v>1.8552371756009763E-5</v>
       </c>
       <c r="K80">
-        <v>2.641038677585787</v>
+        <v>1.9526092033647094E-5</v>
       </c>
       <c r="L80">
-        <v>2.8442116599736962</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.1028218597156306E-5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C81">
-        <v>1.114715004849921</v>
+        <v>0</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -3474,88 +3448,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B82">
         <v>3</v>
       </c>
       <c r="C82">
-        <v>2.6820718601540521</v>
+        <v>0</v>
       </c>
       <c r="D82">
         <v>0</v>
       </c>
       <c r="E82">
-        <v>2.4502474065155848</v>
+        <v>1.1452332421714167E-5</v>
       </c>
       <c r="F82">
-        <v>2.4049959256060429</v>
+        <v>1.1240829289184421E-5</v>
       </c>
       <c r="G82">
-        <v>2.774290739150103</v>
+        <v>1.2966894565317436E-5</v>
       </c>
       <c r="H82">
-        <v>3.7058370305234818</v>
+        <v>1.7320894804907152E-5</v>
       </c>
       <c r="I82">
-        <v>4.636120545786456</v>
+        <v>2.1668992892839815E-5</v>
       </c>
       <c r="J82">
-        <v>4.076901810484121</v>
+        <v>1.9055232814529872E-5</v>
       </c>
       <c r="K82">
-        <v>3.868572581371911</v>
+        <v>1.8081512536892544E-5</v>
       </c>
       <c r="L82">
-        <v>3.5471898637764911</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.6579385973383325E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C83">
-        <v>5.6017956572837786</v>
+        <v>4.1415969590341123E-5</v>
       </c>
       <c r="D83">
-        <v>5.3288036661880804</v>
+        <v>3.9397647485548673E-5</v>
       </c>
       <c r="E83">
-        <v>2.266004146088751</v>
+        <v>1.675333492109285E-5</v>
       </c>
       <c r="F83">
-        <v>2.2568617662486239</v>
+        <v>1.6685742215359336E-5</v>
       </c>
       <c r="G83">
-        <v>1.2503544004825839</v>
+        <v>9.2442929010097834E-6</v>
       </c>
       <c r="H83">
-        <v>1.2503544004825839</v>
+        <v>9.2442929010097834E-6</v>
       </c>
       <c r="I83">
-        <v>0.87321668612140313</v>
+        <v>6.4559862463312983E-6</v>
       </c>
       <c r="J83">
-        <v>1.624643356216434</v>
+        <v>1.2011537719823847E-5</v>
       </c>
       <c r="K83">
-        <v>1.7050716618110551</v>
+        <v>1.260617138061766E-5</v>
       </c>
       <c r="L83">
-        <v>1.7050716618110551</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.260617138061766E-5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B84">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -3576,19 +3550,19 @@
         <v>0</v>
       </c>
       <c r="I84">
-        <v>0.18305443901553539</v>
+        <v>2.2670599051952546E-6</v>
       </c>
       <c r="J84">
-        <v>0.23592423903501761</v>
+        <v>2.921832356846577E-6</v>
       </c>
       <c r="K84">
-        <v>0.27658073006398792</v>
+        <v>3.4253476017835582E-6</v>
       </c>
       <c r="L84">
-        <v>0.27658073006398792</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.4253476017835582E-6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>27</v>
       </c>
@@ -3599,34 +3573,38 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <v>0.42012403824468231</v>
+        <v>2.0183221047924522E-6</v>
       </c>
       <c r="E85">
-        <v>5.1336531698261156</v>
+        <v>2.4662634669248273E-5</v>
       </c>
       <c r="F85">
-        <v>5.1477229362034533</v>
+        <v>2.4730227374981787E-5</v>
       </c>
       <c r="G85">
-        <v>6.6966985575446989</v>
+        <v>3.217167668933134E-5</v>
       </c>
       <c r="H85">
-        <v>6.6966985575446989</v>
+        <v>3.217167668933134E-5</v>
       </c>
       <c r="I85">
-        <v>6.8051987264695812</v>
+        <v>3.2692923438814569E-5</v>
       </c>
       <c r="J85">
-        <v>5.5124881328315514</v>
+        <v>2.64825995136707E-5</v>
       </c>
       <c r="K85">
-        <v>5.2839028382573527</v>
+        <v>2.5384450607939901E-5</v>
       </c>
       <c r="L85">
-        <v>5.2839028382573554</v>
+        <v>2.5384450607939904E-5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sortState ref="A2:L85">
+    <sortCondition ref="A2:A85"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reapply "Adjustment following integration tests"
This reverts commit 936c6c05f1aba5547681bd3fdba44f161d0e0a3a.
</commit_message>
<xml_diff>
--- a/import/raw_data/primes/renewable_energy_system_utilization_primes.xlsx
+++ b/import/raw_data/primes/renewable_energy_system_utilization_primes.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_env\workspace\micat\back_end\import\public\primes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\primes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7139926-029C-4B50-8A59-6515398CBD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="1125" windowWidth="43200" windowHeight="11325"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -47,10 +43,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -61,12 +54,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -75,13 +83,15 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -104,44 +114,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -168,15 +178,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -203,7 +212,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -215,162 +223,180 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +434,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -416,157 +442,157 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3.7043000420312024E-5</v>
+        <v>4.9289702887829936</v>
       </c>
       <c r="D2">
-        <v>2.8436730460753743E-5</v>
+        <v>3.7838133509921792</v>
       </c>
       <c r="E2">
-        <v>2.2430912134312783E-5</v>
+        <v>2.9846745189599941</v>
       </c>
       <c r="F2">
-        <v>2.1518932426900993E-5</v>
+        <v>2.8633257936731269</v>
       </c>
       <c r="G2">
-        <v>1.9274810138295901E-5</v>
+        <v>2.5647211461169608</v>
       </c>
       <c r="H2">
-        <v>1.7847643413079343E-5</v>
+        <v>2.374821237742506</v>
       </c>
       <c r="I2">
-        <v>1.7266014332376066E-5</v>
+        <v>2.2974292223725352</v>
       </c>
       <c r="J2">
-        <v>1.6584341628840938E-5</v>
+        <v>2.2067253251645589</v>
       </c>
       <c r="K2">
-        <v>1.6114278700627293E-5</v>
+        <v>2.1441783883415648</v>
       </c>
       <c r="L2">
-        <v>1.6056270525238428E-5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.13645977565485</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4.9238048114803618E-2</v>
+      </c>
+      <c r="D3">
+        <v>5.7051334009565517E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.1056434026421734</v>
+      </c>
+      <c r="F3">
+        <v>0.17174892024400601</v>
+      </c>
+      <c r="G3">
+        <v>0.25447060823031281</v>
+      </c>
+      <c r="H3">
+        <v>0.3192359057390009</v>
+      </c>
+      <c r="I3">
+        <v>0.34489903763181468</v>
+      </c>
+      <c r="J3">
+        <v>0.35738775626019043</v>
+      </c>
+      <c r="K3">
+        <v>0.35549724797416249</v>
+      </c>
+      <c r="L3">
+        <v>0.35899975162708042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>5.0714892089427259E-7</v>
-      </c>
-      <c r="D3">
-        <v>5.8762529357517089E-7</v>
-      </c>
-      <c r="E3">
-        <v>1.0881206648293039E-6</v>
-      </c>
-      <c r="F3">
-        <v>1.7690035024015598E-6</v>
-      </c>
-      <c r="G3">
-        <v>2.6210318910775744E-6</v>
-      </c>
-      <c r="H3">
-        <v>3.2881105426590639E-6</v>
-      </c>
-      <c r="I3">
-        <v>3.5524392507317729E-6</v>
-      </c>
-      <c r="J3">
-        <v>3.6810722981053272E-6</v>
-      </c>
-      <c r="K3">
-        <v>3.6616001769732057E-6</v>
-      </c>
-      <c r="L3">
-        <v>3.6976757529965261E-6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.57434484172056188</v>
+      </c>
+      <c r="D4">
+        <v>2.7989278185775639</v>
+      </c>
+      <c r="E4">
+        <v>4.2353979375655451</v>
+      </c>
+      <c r="F4">
+        <v>4.295696625002833</v>
+      </c>
+      <c r="G4">
+        <v>4.6589271396068037</v>
+      </c>
+      <c r="H4">
+        <v>4.8572522541302368</v>
+      </c>
+      <c r="I4">
+        <v>4.9400434923078507</v>
+      </c>
+      <c r="J4">
+        <v>5.0843447344253594</v>
+      </c>
+      <c r="K4">
+        <v>5.2120761093703978</v>
+      </c>
+      <c r="L4">
+        <v>5.2177988478685364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>3</v>
-      </c>
-      <c r="C4">
-        <v>2.2011970868875508E-6</v>
-      </c>
-      <c r="D4">
-        <v>1.0726990673764926E-5</v>
-      </c>
-      <c r="E4">
-        <v>1.6232313628951761E-5</v>
-      </c>
-      <c r="F4">
-        <v>1.6463410498791292E-5</v>
-      </c>
-      <c r="G4">
-        <v>1.7855504398720366E-5</v>
-      </c>
-      <c r="H4">
-        <v>1.8615592472355438E-5</v>
-      </c>
-      <c r="I4">
-        <v>1.8932892844986002E-5</v>
-      </c>
-      <c r="J4">
-        <v>1.9485932501147579E-5</v>
-      </c>
-      <c r="K4">
-        <v>1.9975467550493345E-5</v>
-      </c>
-      <c r="L4">
-        <v>1.9997400149858884E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>4.2381815082829986E-5</v>
+        <v>5.7324329244767958</v>
       </c>
       <c r="D5">
-        <v>3.8043850109028021E-5</v>
+        <v>5.1456932298117648</v>
       </c>
       <c r="E5">
-        <v>3.2155418311938866E-5</v>
+        <v>4.3492421990760608</v>
       </c>
       <c r="F5">
-        <v>2.93828826237283E-5</v>
+        <v>3.9742376167493352</v>
       </c>
       <c r="G5">
-        <v>3.1587203303243795E-5</v>
+        <v>4.2723871984664923</v>
       </c>
       <c r="H5">
-        <v>2.2713150533125333E-5</v>
+        <v>3.0721103303438642</v>
       </c>
       <c r="I5">
-        <v>2.2957864049545577E-5</v>
+        <v>3.105209521962963</v>
       </c>
       <c r="J5">
-        <v>2.3209289793360049E-5</v>
+        <v>3.1392165886515042</v>
       </c>
       <c r="K5">
-        <v>2.1954335577394848E-5</v>
+        <v>2.9694753717581208</v>
       </c>
       <c r="L5">
-        <v>1.8860871334834992E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.5510629880486291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
       <c r="C6">
         <v>0</v>
       </c>
@@ -598,205 +624,205 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
       <c r="C7">
-        <v>1.634260221702956E-6</v>
+        <v>0.41422713124311172</v>
       </c>
       <c r="D7">
-        <v>5.9722251955049098E-6</v>
+        <v>1.513747735531362</v>
       </c>
       <c r="E7">
-        <v>1.1860656992594071E-5</v>
+        <v>3.006256809935246</v>
       </c>
       <c r="F7">
-        <v>1.4633192680804638E-5</v>
+        <v>3.7089964894214629</v>
       </c>
       <c r="G7">
-        <v>1.2428872001289148E-5</v>
+        <v>3.1502792060355298</v>
       </c>
       <c r="H7">
-        <v>2.1302924771407601E-5</v>
+        <v>5.3995375387359168</v>
       </c>
       <c r="I7">
-        <v>2.1058211254987361E-5</v>
+        <v>5.3375113225085258</v>
       </c>
       <c r="J7">
-        <v>2.0806785511172896E-5</v>
+        <v>5.2737837941762216</v>
       </c>
       <c r="K7">
-        <v>2.2061739727138092E-5</v>
+        <v>5.5918702762537382</v>
       </c>
       <c r="L7">
-        <v>2.5155203969697942E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.3759539869026174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>4.2541333447942263E-5</v>
+        <v>5.7540088840349499</v>
       </c>
       <c r="D8">
-        <v>1.6997484099710846E-5</v>
+        <v>2.2990270071261669</v>
       </c>
       <c r="E8">
-        <v>1.2103223904064955E-5</v>
+        <v>1.637044545269714</v>
       </c>
       <c r="F8">
-        <v>1.2007695290135007E-5</v>
+        <v>1.6241236410882529</v>
       </c>
       <c r="G8">
-        <v>1.5877208797756263E-5</v>
+        <v>2.1475020426372269</v>
       </c>
       <c r="H8">
-        <v>1.4088003557587992E-5</v>
+        <v>1.9054996883883131</v>
       </c>
       <c r="I8">
-        <v>1.2329215950373367E-5</v>
+        <v>1.667611528878046</v>
       </c>
       <c r="J8">
-        <v>1.0902757222002617E-5</v>
+        <v>1.4746731433006779</v>
       </c>
       <c r="K8">
-        <v>1.0570203477268059E-5</v>
+        <v>1.4296929547044901</v>
       </c>
       <c r="L8">
-        <v>1.0166861692361196E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.375138195237521</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>4.622746721678682E-6</v>
+        <v>0.34770466624767632</v>
       </c>
       <c r="E9">
-        <v>5.6622320945290487E-6</v>
+        <v>0.42589063151834738</v>
       </c>
       <c r="F9">
-        <v>9.4143030516393675E-6</v>
+        <v>0.70810652142673769</v>
       </c>
       <c r="G9">
-        <v>7.1469449419290075E-6</v>
+        <v>0.53756484084889322</v>
       </c>
       <c r="H9">
-        <v>8.9834306755934125E-6</v>
+        <v>0.67569801091807657</v>
       </c>
       <c r="I9">
-        <v>8.4804635197105733E-6</v>
+        <v>0.63786681712810422</v>
       </c>
       <c r="J9">
-        <v>8.2879553884757958E-6</v>
+        <v>0.62338711933132651</v>
       </c>
       <c r="K9">
-        <v>7.7883984608326586E-6</v>
+        <v>0.58581242937842437</v>
       </c>
       <c r="L9">
-        <v>7.2409012421206561E-6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.54463186094904292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>5.0947704728074559E-7</v>
+        <v>0.1454772705211764</v>
       </c>
       <c r="D10">
-        <v>2.1430579673833477E-5</v>
+        <v>6.119337962869837</v>
       </c>
       <c r="E10">
-        <v>2.5285354496629004E-5</v>
+        <v>7.2200394030762816</v>
       </c>
       <c r="F10">
-        <v>2.1628812153448629E-5</v>
+        <v>6.1759417298441814</v>
       </c>
       <c r="G10">
-        <v>2.0026656755537735E-5</v>
+        <v>5.7184585213603851</v>
       </c>
       <c r="H10">
-        <v>1.9979376262041604E-5</v>
+        <v>5.7049579384010114</v>
       </c>
       <c r="I10">
-        <v>2.2241131025139061E-5</v>
+        <v>6.3507846960142427</v>
       </c>
       <c r="J10">
-        <v>2.3860097884744589E-5</v>
+        <v>6.8130682886838629</v>
       </c>
       <c r="K10">
-        <v>2.469220855712229E-5</v>
+        <v>7.0506711209118338</v>
       </c>
       <c r="L10">
-        <v>2.5643047560741154E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.3221759191943816</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2.7832821190277892</v>
       </c>
       <c r="D11">
-        <v>5.6877814502062717E-5</v>
+        <v>7.6931168683240037</v>
       </c>
       <c r="E11">
-        <v>4.1641052926002553E-5</v>
+        <v>5.6322397315070027</v>
       </c>
       <c r="F11">
-        <v>3.5212460488157338E-5</v>
+        <v>4.7627282470006218</v>
       </c>
       <c r="G11">
-        <v>2.326957573374657E-5</v>
+        <v>3.147370678061769</v>
       </c>
       <c r="H11">
-        <v>1.2709087681499121E-5</v>
+        <v>1.718991801627749</v>
       </c>
       <c r="I11">
-        <v>1.2341661546412258E-5</v>
+        <v>1.6692948816169191</v>
       </c>
       <c r="J11">
-        <v>1.0153828934348794E-5</v>
+        <v>1.373375424790314</v>
       </c>
       <c r="K11">
-        <v>7.9092721005946686E-6</v>
+        <v>1.069783625582917</v>
       </c>
       <c r="L11">
-        <v>1.0882021865123346E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.4718685432087939</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1.114715004849921</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -826,88 +852,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>2.3921181455428031</v>
       </c>
       <c r="D13">
-        <v>4.8554231892004752E-6</v>
+        <v>0.56443237142021196</v>
       </c>
       <c r="E13">
-        <v>2.0092184765260637E-5</v>
+        <v>2.33567272144131</v>
       </c>
       <c r="F13">
-        <v>2.6520777203105845E-5</v>
+        <v>3.082982591908956</v>
       </c>
       <c r="G13">
-        <v>3.8463661957516614E-5</v>
+        <v>4.4713169349428892</v>
       </c>
       <c r="H13">
-        <v>4.9024150009764061E-5</v>
+        <v>5.6989506719861813</v>
       </c>
       <c r="I13">
-        <v>4.9391576144850919E-5</v>
+        <v>5.7416631599954897</v>
       </c>
       <c r="J13">
-        <v>5.1579408756914386E-5</v>
+        <v>5.9959939364032202</v>
       </c>
       <c r="K13">
-        <v>5.3823965590668515E-5</v>
+        <v>6.2569187800463339</v>
       </c>
       <c r="L13">
-        <v>5.0851215826139829E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.9113430940867966</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>3.5429510327159738E-5</v>
+        <v>4.7920857353695858</v>
       </c>
       <c r="D14">
-        <v>4.0667565860533169E-6</v>
+        <v>0.55005688888415194</v>
       </c>
       <c r="E14">
-        <v>4.418444375916347E-6</v>
+        <v>0.59762508910887646</v>
       </c>
       <c r="F14">
-        <v>5.9372430373945241E-6</v>
+        <v>0.80305308778456319</v>
       </c>
       <c r="G14">
-        <v>1.0164013798060665E-5</v>
+        <v>1.3747529978829041</v>
       </c>
       <c r="H14">
-        <v>1.0728414118673707E-5</v>
+        <v>1.4510920356080299</v>
       </c>
       <c r="I14">
-        <v>1.4420569619335652E-5</v>
+        <v>1.95048154294551</v>
       </c>
       <c r="J14">
-        <v>1.5139022077604027E-5</v>
+        <v>2.0476571952482692</v>
       </c>
       <c r="K14">
-        <v>1.4458629186533428E-5</v>
+        <v>1.955629362020022</v>
       </c>
       <c r="L14">
-        <v>1.487288520637609E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.0116603470702792</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -940,316 +966,316 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>1.6104322875981698E-6</v>
+        <v>0.46178280722652371</v>
       </c>
       <c r="D16">
-        <v>3.2973186028704584E-5</v>
+        <v>9.4548839617756428</v>
       </c>
       <c r="E16">
-        <v>3.2621498238841553E-5</v>
+        <v>9.3540393772992267</v>
       </c>
       <c r="F16">
-        <v>3.110269957736338E-5</v>
+        <v>8.9185320201067722</v>
       </c>
       <c r="G16">
-        <v>2.6875928816697243E-5</v>
+        <v>7.7065282106982904</v>
       </c>
       <c r="H16">
-        <v>2.6311528496084202E-5</v>
+        <v>7.5446894507210223</v>
       </c>
       <c r="I16">
-        <v>2.261937299542225E-5</v>
+        <v>6.4859836951655643</v>
       </c>
       <c r="J16">
-        <v>2.1900920537153879E-5</v>
+        <v>6.279971312283716</v>
       </c>
       <c r="K16">
-        <v>2.2581313428224482E-5</v>
+        <v>6.4750703187275986</v>
       </c>
       <c r="L16">
-        <v>2.216705740838182E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.3562846304210554</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>4.0494627603075015E-5</v>
+        <v>5.4771777962463268</v>
       </c>
       <c r="D17">
-        <v>2.729679368562529E-5</v>
+        <v>3.6920796938572309</v>
       </c>
       <c r="E17">
-        <v>2.2179316232551195E-5</v>
+        <v>2.9999055577345368</v>
       </c>
       <c r="F17">
-        <v>2.1381023519202086E-5</v>
+        <v>2.8919309600343488</v>
       </c>
       <c r="G17">
-        <v>2.2347443448434197E-5</v>
+        <v>3.022645923760503</v>
       </c>
       <c r="H17">
-        <v>1.7638585521681602E-5</v>
+        <v>2.3857403980475231</v>
       </c>
       <c r="I17">
-        <v>1.7185796931565558E-5</v>
+        <v>2.3244976169930571</v>
       </c>
       <c r="J17">
-        <v>1.7362520564132959E-5</v>
+        <v>2.3484007076908631</v>
       </c>
       <c r="K17">
-        <v>1.6209898469885625E-5</v>
+        <v>2.1925006163514609</v>
       </c>
       <c r="L17">
-        <v>1.6255972008813701E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.1987323803989018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>6.0391136472622327E-8</v>
+        <v>4.1800312292828773E-3</v>
       </c>
       <c r="E18">
-        <v>1.7690002962662048E-6</v>
+        <v>0.12244307550588331</v>
       </c>
       <c r="F18">
-        <v>3.0047985817308089E-6</v>
+        <v>0.20798005540156861</v>
       </c>
       <c r="G18">
-        <v>4.7588306771192109E-6</v>
+        <v>0.32938709233010588</v>
       </c>
       <c r="H18">
-        <v>5.026791655477341E-6</v>
+        <v>0.34793427198574889</v>
       </c>
       <c r="I18">
-        <v>6.0531113294583808E-6</v>
+        <v>0.41897198611144698</v>
       </c>
       <c r="J18">
-        <v>6.7269367631383937E-6</v>
+        <v>0.46561146866439429</v>
       </c>
       <c r="K18">
-        <v>6.3057523727248775E-6</v>
+        <v>0.43645878156414247</v>
       </c>
       <c r="L18">
-        <v>6.2956700867724202E-6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.43576092633893182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>4.5309907130297808E-6</v>
+        <v>1.214552829041422</v>
       </c>
       <c r="D19">
-        <v>1.7668433494006876E-5</v>
+        <v>4.7361045837427689</v>
       </c>
       <c r="E19">
-        <v>2.1077301787287392E-5</v>
+        <v>5.6498673547692739</v>
       </c>
       <c r="F19">
-        <v>2.0639796215171896E-5</v>
+        <v>5.5325919807972674</v>
       </c>
       <c r="G19">
-        <v>1.7919344190551385E-5</v>
+        <v>4.8033623460349171</v>
       </c>
       <c r="H19">
-        <v>2.236024113894585E-5</v>
+        <v>5.9937651285087874</v>
       </c>
       <c r="I19">
-        <v>2.1786710055080858E-5</v>
+        <v>5.8400274926208446</v>
       </c>
       <c r="J19">
-        <v>2.0936160988833441E-5</v>
+        <v>5.612033916805597</v>
       </c>
       <c r="K19">
-        <v>2.2509967473494283E-5</v>
+        <v>6.0338999587755664</v>
       </c>
       <c r="L19">
-        <v>2.2473976220518675E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.0242523384446383</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>2.4225136454825605E-5</v>
+        <v>3.2766168589566842</v>
       </c>
       <c r="D20">
-        <v>2.1638452232056018E-5</v>
+        <v>2.9267499697059609</v>
       </c>
       <c r="E20">
-        <v>1.8587772688827899E-5</v>
+        <v>2.5141245117955129</v>
       </c>
       <c r="F20">
-        <v>1.7440127823072519E-5</v>
+        <v>2.3588976249525242</v>
       </c>
       <c r="G20">
-        <v>1.5860063586085393E-5</v>
+        <v>2.1451830344567822</v>
       </c>
       <c r="H20">
-        <v>1.5741814007832762E-5</v>
+        <v>2.129188963076023</v>
       </c>
       <c r="I20">
-        <v>1.5361514382807952E-5</v>
+        <v>2.077750814724006</v>
       </c>
       <c r="J20">
-        <v>1.518801061101876E-5</v>
+        <v>2.0542832324134919</v>
       </c>
       <c r="K20">
-        <v>1.5403936260052652E-5</v>
+        <v>2.083488666332304</v>
       </c>
       <c r="L20">
-        <v>1.3908719247170362E-5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.881250248342587</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>4.3643005252433348E-6</v>
+        <v>0.47640824372113949</v>
       </c>
       <c r="D21">
-        <v>6.9258223322121546E-6</v>
+        <v>0.75602466753360709</v>
       </c>
       <c r="E21">
-        <v>6.2089511399475072E-6</v>
+        <v>0.67777081134160266</v>
       </c>
       <c r="F21">
-        <v>6.626072635279182E-6</v>
+        <v>0.72330390830866353</v>
       </c>
       <c r="G21">
-        <v>3.9059425143280567E-6</v>
+        <v>0.42637375738991062</v>
       </c>
       <c r="H21">
-        <v>3.016729540697772E-6</v>
+        <v>0.329307025021008</v>
       </c>
       <c r="I21">
-        <v>2.7726282361922031E-6</v>
+        <v>0.30266085959383388</v>
       </c>
       <c r="J21">
-        <v>2.7413122184637069E-6</v>
+        <v>0.29924239449958112</v>
       </c>
       <c r="K21">
-        <v>2.6972340275586297E-6</v>
+        <v>0.29443080707703018</v>
       </c>
       <c r="L21">
-        <v>3.7873426148178577E-6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.41342735979324008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>2.7428305385419503E-8</v>
+        <v>1.368262981321504E-2</v>
       </c>
       <c r="D22">
-        <v>5.2590721186185483E-8</v>
+        <v>2.623491898201992E-2</v>
       </c>
       <c r="E22">
-        <v>3.8201414566789525E-6</v>
+        <v>1.9056803054861691</v>
       </c>
       <c r="F22">
-        <v>4.5506648271026569E-6</v>
+        <v>2.2701024127565348</v>
       </c>
       <c r="G22">
-        <v>8.8508591850409099E-6</v>
+        <v>4.4152574523319084</v>
       </c>
       <c r="H22">
-        <v>9.8583217369238235E-6</v>
+        <v>4.917830868895174</v>
       </c>
       <c r="I22">
-        <v>1.0482722666454202E-5</v>
+        <v>5.2293137204144351</v>
       </c>
       <c r="J22">
-        <v>1.068754245597189E-5</v>
+        <v>5.3314882193129671</v>
       </c>
       <c r="K22">
-        <v>1.0515694997843076E-5</v>
+        <v>5.2457619915756712</v>
       </c>
       <c r="L22">
-        <v>1.0920803423466138E-5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.447850620243238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>3.6086708797466337E-5</v>
+        <v>4.8809763631479983</v>
       </c>
       <c r="D23">
-        <v>3.6086708797466337E-5</v>
+        <v>4.8809763631479983</v>
       </c>
       <c r="E23">
-        <v>3.6086708797466337E-5</v>
+        <v>4.8809763631479983</v>
       </c>
       <c r="F23">
-        <v>2.5709713453580391E-5</v>
+        <v>3.477416141619559</v>
       </c>
       <c r="G23">
-        <v>1.7962040534482077E-5</v>
+        <v>2.429489920368376</v>
       </c>
       <c r="H23">
-        <v>8.5427617717553883E-6</v>
+        <v>1.1554674746861351</v>
       </c>
       <c r="I23">
-        <v>1.3900308672421357E-5</v>
+        <v>1.8801126600748179</v>
       </c>
       <c r="J23">
-        <v>1.0017661340987525E-5</v>
+        <v>1.3549578182318081</v>
       </c>
       <c r="K23">
-        <v>8.675244303257375E-6</v>
+        <v>1.1733866512012461</v>
       </c>
       <c r="L23">
-        <v>1.0208870496938814E-5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.3808201759173959</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1267,27 +1293,27 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>1.8923839367812572E-5</v>
+        <v>1.568030898479303</v>
       </c>
       <c r="I24">
-        <v>1.1732877458296698E-5</v>
+        <v>0.97218719864916747</v>
       </c>
       <c r="J24">
-        <v>9.1606126744841852E-6</v>
+        <v>0.75904912546574299</v>
       </c>
       <c r="K24">
-        <v>1.1686550851012522E-5</v>
+        <v>0.96834857212991798</v>
       </c>
       <c r="L24">
-        <v>1.067530161527308E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.88455637664129605</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1299,71 +1325,71 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>1.037699534388595E-5</v>
+        <v>4.0613657474014433</v>
       </c>
       <c r="G25">
-        <v>1.8124668262984267E-5</v>
+        <v>7.0936628982559329</v>
       </c>
       <c r="H25">
-        <v>8.6201076578983843E-6</v>
+        <v>3.373752114221451</v>
       </c>
       <c r="I25">
-        <v>1.0453522666748289E-5</v>
+        <v>4.0913171386773932</v>
       </c>
       <c r="J25">
-        <v>1.6908434781994632E-5</v>
+        <v>6.617651409685255</v>
       </c>
       <c r="K25">
-        <v>1.5724913643196442E-5</v>
+        <v>6.154442932168438</v>
       </c>
       <c r="L25">
-        <v>1.5202536685254451E-5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.949994166999879</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>3.6013361828365801E-5</v>
+        <v>4.8710556794830628</v>
       </c>
       <c r="D26">
-        <v>3.1227032012740872E-5</v>
+        <v>4.2236715462440682</v>
       </c>
       <c r="E26">
-        <v>1.6069709386226235E-5</v>
+        <v>2.1735390754818522</v>
       </c>
       <c r="F26">
-        <v>2.0570935356834532E-5</v>
+        <v>2.782360946465817</v>
       </c>
       <c r="G26">
-        <v>1.9352259587800058E-5</v>
+        <v>2.617526639841099</v>
       </c>
       <c r="H26">
-        <v>1.5024090935327096E-5</v>
+        <v>2.032111965230432</v>
       </c>
       <c r="I26">
-        <v>1.5788760770050962E-5</v>
+        <v>2.1355388365986938</v>
       </c>
       <c r="J26">
-        <v>1.6688642976166111E-5</v>
+        <v>2.2572541141629898</v>
       </c>
       <c r="K26">
-        <v>1.6140900785432632E-5</v>
+        <v>2.183168203445172</v>
       </c>
       <c r="L26">
-        <v>1.4848288672532698E-5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.0083334961518768</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1381,100 +1407,100 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>2.5182759490081578E-6</v>
+        <v>0.26932285439654863</v>
       </c>
       <c r="I27">
-        <v>2.3715726249872191E-6</v>
+        <v>0.2536333276032906</v>
       </c>
       <c r="J27">
-        <v>2.2831903786686927E-6</v>
+        <v>0.24418108355280849</v>
       </c>
       <c r="K27">
-        <v>1.9765879787305105E-6</v>
+        <v>0.211390779714698</v>
       </c>
       <c r="L27">
-        <v>3.4493746375068418E-6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.36890136032244392</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>7.334696910054131E-8</v>
+        <v>1.615823926264855E-2</v>
       </c>
       <c r="D28">
-        <v>4.8596767847254667E-6</v>
+        <v>1.0705803005860419</v>
       </c>
       <c r="E28">
-        <v>2.0016999411240102E-5</v>
+        <v>4.409718217037077</v>
       </c>
       <c r="F28">
-        <v>1.5515773440631809E-5</v>
+        <v>3.418104151721876</v>
       </c>
       <c r="G28">
-        <v>1.6734449209666287E-5</v>
+        <v>3.6865767948471659</v>
       </c>
       <c r="H28">
-        <v>1.8544341913131089E-5</v>
+        <v>4.0852937384500922</v>
       </c>
       <c r="I28">
-        <v>1.7926375402428162E-5</v>
+        <v>3.9491565420711319</v>
       </c>
       <c r="J28">
-        <v>1.7114875442631537E-5</v>
+        <v>3.7703841855194988</v>
       </c>
       <c r="K28">
-        <v>1.7969220033303196E-5</v>
+        <v>3.9585951569898969</v>
       </c>
       <c r="L28">
-        <v>1.7789045487426799E-5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.918902945341463</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>3.0887940479648834E-5</v>
+        <v>4.1778070766617921</v>
       </c>
       <c r="D29">
-        <v>2.615393152450036E-5</v>
+        <v>3.537499700816173</v>
       </c>
       <c r="E29">
-        <v>3.0996841051234936E-5</v>
+        <v>4.1925366303827563</v>
       </c>
       <c r="F29">
-        <v>2.9245851588672428E-5</v>
+        <v>3.9557032237438858</v>
       </c>
       <c r="G29">
-        <v>2.9150456089030943E-5</v>
+        <v>3.9428003241884282</v>
       </c>
       <c r="H29">
-        <v>2.6509538584949669E-5</v>
+        <v>3.585598009430659</v>
       </c>
       <c r="I29">
-        <v>2.5025374115365736E-5</v>
+        <v>3.3848545241845929</v>
       </c>
       <c r="J29">
-        <v>2.462309173643984E-5</v>
+        <v>3.3304430566864509</v>
       </c>
       <c r="K29">
-        <v>2.3851618258910257E-5</v>
+        <v>3.226095945683582</v>
       </c>
       <c r="L29">
-        <v>2.4016796258181032E-5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.2484374098131479</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1483,112 +1509,112 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>5.1291559698929063E-6</v>
+        <v>0.48323536101051451</v>
       </c>
       <c r="E30">
-        <v>9.2129588037902295E-7</v>
+        <v>8.6798442076182841E-2</v>
       </c>
       <c r="F30">
-        <v>7.6621230574968485E-7</v>
+        <v>7.2187487054985885E-2</v>
       </c>
       <c r="G30">
-        <v>5.6783774189310772E-7</v>
+        <v>5.3497939584949021E-2</v>
       </c>
       <c r="H30">
-        <v>1.296546871646887E-6</v>
+        <v>0.12215212390985609</v>
       </c>
       <c r="I30">
-        <v>2.675903401647976E-6</v>
+        <v>0.25210602951339428</v>
       </c>
       <c r="J30">
-        <v>3.4072976352451792E-6</v>
+        <v>0.32101318667296352</v>
       </c>
       <c r="K30">
-        <v>3.9260329162253689E-6</v>
+        <v>0.3698850151462526</v>
       </c>
       <c r="L30">
-        <v>3.8866153320592816E-6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.36617134946198221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>0.69382052300823405</v>
+      </c>
+      <c r="D31">
+        <v>0.51186268976832949</v>
+      </c>
+      <c r="E31">
+        <v>0.2194342636757432</v>
+      </c>
+      <c r="F31">
+        <v>1.0971453608195449</v>
+      </c>
+      <c r="G31">
+        <v>1.232420998064147</v>
+      </c>
+      <c r="H31">
+        <v>2.1129573035727929</v>
+      </c>
+      <c r="I31">
+        <v>2.1612194057303098</v>
+      </c>
+      <c r="J31">
+        <v>2.009669532556424</v>
+      </c>
+      <c r="K31">
+        <v>2.1260507600619198</v>
+      </c>
+      <c r="L31">
+        <v>2.0681404335607838</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>4.9274662932560336</v>
+      </c>
+      <c r="D32">
+        <v>4.3712685755523086</v>
+      </c>
+      <c r="E32">
+        <v>3.0158905049045019</v>
+      </c>
+      <c r="F32">
+        <v>3.1030183816523711</v>
+      </c>
+      <c r="G32">
+        <v>2.3841962265132208</v>
+      </c>
+      <c r="H32">
+        <v>2.395517140767629</v>
+      </c>
+      <c r="I32">
+        <v>2.5831477540069079</v>
+      </c>
+      <c r="J32">
+        <v>2.7295179679955162</v>
+      </c>
+      <c r="K32">
+        <v>2.829238768600181</v>
+      </c>
+      <c r="L32">
+        <v>2.6342958917336179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>3</v>
-      </c>
-      <c r="C31">
-        <v>1.5067288038853092E-6</v>
-      </c>
-      <c r="D31">
-        <v>1.1115817891408777E-6</v>
-      </c>
-      <c r="E31">
-        <v>4.7653235192018425E-7</v>
-      </c>
-      <c r="F31">
-        <v>2.3826053891120343E-6</v>
-      </c>
-      <c r="G31">
-        <v>2.6763754526100888E-6</v>
-      </c>
-      <c r="H31">
-        <v>4.5885838269375901E-6</v>
-      </c>
-      <c r="I31">
-        <v>4.6933917665204363E-6</v>
-      </c>
-      <c r="J31">
-        <v>4.3642799118491263E-6</v>
-      </c>
-      <c r="K31">
-        <v>4.6170181083985214E-6</v>
-      </c>
-      <c r="L31">
-        <v>4.4912576932938377E-6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>10</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>3.6430424571730246E-5</v>
-      </c>
-      <c r="D32">
-        <v>3.2318266761639015E-5</v>
-      </c>
-      <c r="E32">
-        <v>2.2297498352427999E-5</v>
-      </c>
-      <c r="F32">
-        <v>2.2941664208276165E-5</v>
-      </c>
-      <c r="G32">
-        <v>1.7627168939353435E-5</v>
-      </c>
-      <c r="H32">
-        <v>1.7710868286702136E-5</v>
-      </c>
-      <c r="I32">
-        <v>1.9098084859307897E-5</v>
-      </c>
-      <c r="J32">
-        <v>2.0180249347689699E-5</v>
-      </c>
-      <c r="K32">
-        <v>2.0917518948018147E-5</v>
-      </c>
-      <c r="L32">
-        <v>1.9476240337710187E-5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>10</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1603,106 +1629,106 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>7.5619395291796389E-9</v>
+        <v>6.1882007341698025E-4</v>
       </c>
       <c r="G33">
-        <v>1.9246531508683876E-6</v>
+        <v>0.1575011277896064</v>
       </c>
       <c r="H33">
-        <v>2.3966334083116231E-6</v>
+        <v>0.19612493011377991</v>
       </c>
       <c r="I33">
-        <v>2.2624354526560054E-6</v>
+        <v>0.1851430400245018</v>
       </c>
       <c r="J33">
-        <v>2.0737505114256625E-6</v>
+        <v>0.1697022885169972</v>
       </c>
       <c r="K33">
-        <v>2.5770062740875609E-6</v>
+        <v>0.21088547529021101</v>
       </c>
       <c r="L33">
-        <v>2.5785395464464457E-6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.21101094835304529</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>6.0951804302766173E-7</v>
+        <v>0.16805386971851341</v>
       </c>
       <c r="D34">
-        <v>4.7216758531188917E-6</v>
+        <v>1.3018415250376461</v>
       </c>
       <c r="E34">
-        <v>1.4742444262329914E-5</v>
+        <v>4.0647275921274062</v>
       </c>
       <c r="F34">
-        <v>1.4090716466952561E-5</v>
+        <v>3.885035818817081</v>
       </c>
       <c r="G34">
-        <v>1.748812052453608E-5</v>
+        <v>4.821754436756958</v>
       </c>
       <c r="H34">
-        <v>1.6932440919744146E-5</v>
+        <v>4.668544685253833</v>
       </c>
       <c r="I34">
-        <v>1.5679422302794002E-5</v>
+        <v>4.3230674187207168</v>
       </c>
       <c r="J34">
-        <v>1.4785942755642548E-5</v>
+        <v>4.0767208222076867</v>
       </c>
       <c r="K34">
-        <v>1.3545417392652196E-5</v>
+        <v>3.7346881455391951</v>
       </c>
       <c r="L34">
-        <v>1.4985162730601275E-5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.1316489545247146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>3.9900751190694494E-5</v>
+        <v>5.3968519137246167</v>
       </c>
       <c r="D35">
-        <v>3.9900751190694494E-5</v>
+        <v>5.3968519137246167</v>
       </c>
       <c r="E35">
-        <v>3.5788154976064178E-5</v>
+        <v>4.8405948987819896</v>
       </c>
       <c r="F35">
-        <v>3.6852380638180906E-5</v>
+        <v>4.9845387627403444</v>
       </c>
       <c r="G35">
-        <v>3.3656459762710099E-5</v>
+        <v>4.5522684124788793</v>
       </c>
       <c r="H35">
-        <v>3.1020021470486641E-5</v>
+        <v>4.1956719420314412</v>
       </c>
       <c r="I35">
-        <v>2.6461552135958386E-5</v>
+        <v>3.579107511098091</v>
       </c>
       <c r="J35">
-        <v>2.2851038564457683E-5</v>
+        <v>3.0907606380089798</v>
       </c>
       <c r="K35">
-        <v>2.210367893907954E-5</v>
+        <v>2.989675091895172</v>
       </c>
       <c r="L35">
-        <v>1.9945519271133552E-5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.6977691055037689</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1735,15 +1761,15 @@
         <v>0</v>
       </c>
       <c r="L36">
-        <v>2.4506053402540262E-6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.2053891063873198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1752,71 +1778,71 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>4.1125962146303122E-6</v>
+        <v>0.99882646478749182</v>
       </c>
       <c r="F37">
-        <v>3.0483705525135859E-6</v>
+        <v>0.74035792074548212</v>
       </c>
       <c r="G37">
-        <v>6.2442914279843937E-6</v>
+        <v>1.516551396397456</v>
       </c>
       <c r="H37">
-        <v>8.8807297202078515E-6</v>
+        <v>2.1568633068359202</v>
       </c>
       <c r="I37">
-        <v>1.3439199054736107E-5</v>
+        <v>3.2639790003366822</v>
       </c>
       <c r="J37">
-        <v>1.7049712626236815E-5</v>
+        <v>4.1408646264674944</v>
       </c>
       <c r="K37">
-        <v>1.7797072251614948E-5</v>
+        <v>4.3223758990514112</v>
       </c>
       <c r="L37">
-        <v>1.750462657930691E-5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.251349602821624</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38">
-        <v>4.1591460986910369E-5</v>
+        <v>5.625532079560406</v>
       </c>
       <c r="D38">
-        <v>4.130948498021945E-5</v>
+        <v>5.5873928790210128</v>
       </c>
       <c r="E38">
-        <v>2.7532375582884329E-5</v>
+        <v>3.7239437709766068</v>
       </c>
       <c r="F38">
-        <v>7.6701741394021926E-6</v>
+        <v>1.0374439765557031</v>
       </c>
       <c r="G38">
-        <v>5.1406585329380192E-6</v>
+        <v>0.69530953712374055</v>
       </c>
       <c r="H38">
-        <v>3.5276915915912479E-6</v>
+        <v>0.47714462883469561</v>
       </c>
       <c r="I38">
-        <v>5.8602211542286105E-6</v>
+        <v>0.79263534663537938</v>
       </c>
       <c r="J38">
-        <v>7.6403221048501382E-6</v>
+        <v>1.0334062829034989</v>
       </c>
       <c r="K38">
-        <v>9.6058030641914605E-6</v>
+        <v>1.299251144473031</v>
       </c>
       <c r="L38">
-        <v>1.0124790691806121E-5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.369447802122544</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -1852,126 +1878,126 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>7.3177653067452428E-2</v>
+      </c>
+      <c r="E40">
+        <v>3.6485759416729802</v>
+      </c>
+      <c r="F40">
+        <v>8.8031609130821931</v>
+      </c>
+      <c r="G40">
+        <v>9.4596139838622193</v>
+      </c>
+      <c r="H40">
+        <v>9.8782068160265641</v>
+      </c>
+      <c r="I40">
+        <v>9.2728750322789111</v>
+      </c>
+      <c r="J40">
+        <v>8.8109080326099996</v>
+      </c>
+      <c r="K40">
+        <v>8.3008317128505738</v>
+      </c>
+      <c r="L40">
+        <v>8.1661454428889062</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>4.2396880611031493</v>
+      </c>
+      <c r="D41">
+        <v>4.3740582412032891</v>
+      </c>
+      <c r="E41">
+        <v>4.4058673391209933</v>
+      </c>
+      <c r="F41">
+        <v>4.4280652012731698</v>
+      </c>
+      <c r="G41">
+        <v>3.786097766171383</v>
+      </c>
+      <c r="H41">
+        <v>2.8105752326058822</v>
+      </c>
+      <c r="I41">
+        <v>2.8089099631704948</v>
+      </c>
+      <c r="J41">
+        <v>2.5708451056621229</v>
+      </c>
+      <c r="K41">
+        <v>2.4178804657074879</v>
+      </c>
+      <c r="L41">
+        <v>2.3485898812335191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>12</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>2.8197600669091774E-7</v>
-      </c>
-      <c r="E40">
-        <v>1.405908540402604E-5</v>
-      </c>
-      <c r="F40">
-        <v>3.3921286847508178E-5</v>
-      </c>
-      <c r="G40">
-        <v>3.6450802453972348E-5</v>
-      </c>
-      <c r="H40">
-        <v>3.8063769395319121E-5</v>
-      </c>
-      <c r="I40">
-        <v>3.5731239832681757E-5</v>
-      </c>
-      <c r="J40">
-        <v>3.3951138882060231E-5</v>
-      </c>
-      <c r="K40">
-        <v>3.1985657922718916E-5</v>
-      </c>
-      <c r="L40">
-        <v>3.1466670295104245E-5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>13</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>3.134544752321821E-5</v>
-      </c>
-      <c r="D41">
-        <v>3.2338891703146476E-5</v>
-      </c>
-      <c r="E41">
-        <v>3.2574067120575858E-5</v>
-      </c>
-      <c r="F41">
-        <v>3.2738183421867529E-5</v>
-      </c>
-      <c r="G41">
-        <v>2.7991901087274682E-5</v>
-      </c>
-      <c r="H41">
-        <v>2.0779533115174878E-5</v>
-      </c>
-      <c r="I41">
-        <v>2.0767221215113687E-5</v>
-      </c>
-      <c r="J41">
-        <v>1.90071272198471E-5</v>
-      </c>
-      <c r="K41">
-        <v>1.7876207910335818E-5</v>
-      </c>
-      <c r="L41">
-        <v>1.7363919188104496E-5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>13</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42">
-        <v>1.5927564798383231E-6</v>
+        <v>0.17165381969924379</v>
       </c>
       <c r="D42">
-        <v>5.9931229991005322E-7</v>
+        <v>6.4588809886833382E-2</v>
       </c>
       <c r="E42">
-        <v>3.3716378007468944E-7</v>
+        <v>3.6336660027232182E-2</v>
       </c>
       <c r="F42">
-        <v>1.8520424184166545E-7</v>
+        <v>1.995974647665626E-2</v>
       </c>
       <c r="G42">
-        <v>4.2939141820391241E-6</v>
+        <v>0.46276174678164711</v>
       </c>
       <c r="H42">
-        <v>1.0347382417900702E-5</v>
+        <v>1.1151533447861079</v>
       </c>
       <c r="I42">
-        <v>9.9835093827968231E-6</v>
+        <v>1.0759381871949869</v>
       </c>
       <c r="J42">
-        <v>1.0072659374069482E-5</v>
+        <v>1.0855460191026369</v>
       </c>
       <c r="K42">
-        <v>1.0349760625934394E-5</v>
+        <v>1.115409647929865</v>
       </c>
       <c r="L42">
-        <v>1.0913273647509731E-5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.1761403144367051</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>13</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1980,71 +2006,71 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>2.6973102405975148E-8</v>
+        <v>1.1565881574625391E-2</v>
       </c>
       <c r="F43">
-        <v>1.4816339347333239E-8</v>
+        <v>6.3531448359739921E-3</v>
       </c>
       <c r="G43">
-        <v>6.5238873374272422E-7</v>
+        <v>0.27973982086008309</v>
       </c>
       <c r="H43">
-        <v>1.81128846998095E-6</v>
+        <v>0.77666809052871033</v>
       </c>
       <c r="I43">
-        <v>2.1874734051460198E-6</v>
+        <v>0.93797361426088244</v>
       </c>
       <c r="J43">
-        <v>3.8584174091399478E-6</v>
+        <v>1.654462958984648</v>
       </c>
       <c r="K43">
-        <v>4.7122354667863194E-6</v>
+        <v>2.020574294358032</v>
       </c>
       <c r="L43">
-        <v>4.6610111674423023E-6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.998609665631274</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>14</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>4.7467218406874669E-5</v>
+        <v>6.4202688133367722</v>
       </c>
       <c r="D44">
-        <v>3.1454817611539962E-5</v>
+        <v>4.2544811202022768</v>
       </c>
       <c r="E44">
-        <v>1.575407639177613E-5</v>
+        <v>2.130847535114814</v>
       </c>
       <c r="F44">
-        <v>1.7041797110212283E-5</v>
+        <v>2.3050206475562591</v>
       </c>
       <c r="G44">
-        <v>1.7169694260229273E-5</v>
+        <v>2.3223196195863922</v>
       </c>
       <c r="H44">
-        <v>1.2149187458859345E-5</v>
+        <v>1.6432614332041831</v>
       </c>
       <c r="I44">
-        <v>1.3627762475504958E-5</v>
+        <v>1.843248906373117</v>
       </c>
       <c r="J44">
-        <v>1.178490947753865E-5</v>
+        <v>1.593990322712489</v>
       </c>
       <c r="K44">
-        <v>1.0480861438857243E-5</v>
+        <v>1.417608827549363</v>
       </c>
       <c r="L44">
-        <v>1.0985510498448055E-5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.48586609493753</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -2065,100 +2091,100 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <v>4.1249401610495894E-7</v>
+        <v>3.878736425699323E-2</v>
       </c>
       <c r="I45">
-        <v>3.0921225276550345E-7</v>
+        <v>2.9075641857770122E-2</v>
       </c>
       <c r="J45">
-        <v>3.4651274560458205E-7</v>
+        <v>3.2583057107999053E-2</v>
       </c>
       <c r="K45">
-        <v>3.5913483134926103E-7</v>
+        <v>3.3769928719094837E-2</v>
       </c>
       <c r="L45">
-        <v>3.9731779020866852E-7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.736032342996691E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46">
-        <v>8.8541604096199626E-7</v>
+        <v>0.16882640047840811</v>
       </c>
       <c r="D46">
-        <v>1.6897816836296716E-5</v>
+        <v>3.2219854401055121</v>
       </c>
       <c r="E46">
-        <v>3.2598558056060539E-5</v>
+        <v>6.2157188968607544</v>
       </c>
       <c r="F46">
-        <v>3.1310837337624385E-5</v>
+        <v>5.970183189738437</v>
       </c>
       <c r="G46">
-        <v>3.1182940187607395E-5</v>
+        <v>5.9457964444459588</v>
       </c>
       <c r="H46">
-        <v>3.5790952972872375E-5</v>
+        <v>6.8244277046719759</v>
       </c>
       <c r="I46">
-        <v>3.4415659719566209E-5</v>
+        <v>6.5621941344447512</v>
       </c>
       <c r="J46">
-        <v>3.6221212224693437E-5</v>
+        <v>6.9064672402089222</v>
       </c>
       <c r="K46">
-        <v>3.7512638177630169E-5</v>
+        <v>7.1527094416511066</v>
       </c>
       <c r="L46">
-        <v>3.6969806159179957E-5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.0492051323776872</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47">
-        <v>3.5307858967305202E-5</v>
+        <v>4.775631549554876</v>
       </c>
       <c r="D47">
-        <v>3.5307858967305202E-5</v>
+        <v>4.775631549554876</v>
       </c>
       <c r="E47">
-        <v>3.5307858967305202E-5</v>
+        <v>4.775631549554876</v>
       </c>
       <c r="F47">
-        <v>3.4958276205252673E-5</v>
+        <v>4.7283480688662154</v>
       </c>
       <c r="G47">
-        <v>3.4050106301818193E-5</v>
+        <v>4.6055118230543677</v>
       </c>
       <c r="H47">
-        <v>2.0006504778884667E-5</v>
+        <v>2.7060178162271109</v>
       </c>
       <c r="I47">
-        <v>2.3290945278084292E-5</v>
+        <v>3.150261056383302</v>
       </c>
       <c r="J47">
-        <v>2.3313526781951046E-5</v>
+        <v>3.1533153605936568</v>
       </c>
       <c r="K47">
-        <v>2.2504283488077949E-5</v>
+        <v>3.0438596213185942</v>
       </c>
       <c r="L47">
-        <v>1.9329505534813363E-5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.6144489971716829</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -2179,27 +2205,27 @@
         <v>0</v>
       </c>
       <c r="H48">
-        <v>1.4236340891621799E-5</v>
+        <v>1.1175503288175981</v>
       </c>
       <c r="I48">
-        <v>1.07350430072937E-5</v>
+        <v>0.8426990428230352</v>
       </c>
       <c r="J48">
-        <v>7.3533676952011805E-6</v>
+        <v>0.57723810832072697</v>
       </c>
       <c r="K48">
-        <v>8.3189900190981269E-6</v>
+        <v>0.65303929584495402</v>
       </c>
       <c r="L48">
-        <v>1.0033866100287165E-5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.78765677536471568</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2211,68 +2237,68 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>3.4958276205252673E-7</v>
+        <v>0.13692507949425081</v>
       </c>
       <c r="G49">
-        <v>1.257752665487006E-6</v>
+        <v>0.49263837465772248</v>
       </c>
       <c r="H49">
-        <v>1.065013296798731E-6</v>
+        <v>0.41714594126551657</v>
       </c>
       <c r="I49">
-        <v>1.281870681927207E-6</v>
+        <v>0.502084954056915</v>
       </c>
       <c r="J49">
-        <v>4.6409644901529689E-6</v>
+        <v>1.817779652558235</v>
       </c>
       <c r="K49">
-        <v>4.4845854601291204E-6</v>
+        <v>1.7565288889578501</v>
       </c>
       <c r="L49">
-        <v>5.9444873322046726E-6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.328345355862802</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50">
-        <v>3.7607604570539635E-5</v>
+        <v>5.0866880106369949</v>
       </c>
       <c r="D50">
-        <v>3.7607604570539635E-5</v>
+        <v>5.0866880106369949</v>
       </c>
       <c r="E50">
-        <v>3.247150951070144E-5</v>
+        <v>4.3919957147379689</v>
       </c>
       <c r="F50">
-        <v>3.0741574924228019E-5</v>
+        <v>4.1580101253687944</v>
       </c>
       <c r="G50">
-        <v>2.5901030478045263E-5</v>
+        <v>3.503293089265902</v>
       </c>
       <c r="H50">
-        <v>2.5996534405156056E-5</v>
+        <v>3.5162106543847331</v>
       </c>
       <c r="I50">
-        <v>2.1628388944619828E-5</v>
+        <v>2.9253888406435342</v>
       </c>
       <c r="J50">
-        <v>1.6611071314058277E-5</v>
+        <v>2.2467620116184368</v>
       </c>
       <c r="K50">
-        <v>1.800322952465774E-5</v>
+        <v>2.435061015493666</v>
       </c>
       <c r="L50">
-        <v>1.8593285081717893E-5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.5148701009693948</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -2308,12 +2334,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2322,71 +2348,71 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>5.1360950598382016E-6</v>
+        <v>1.4861859772921779</v>
       </c>
       <c r="F52">
-        <v>6.8660296463116151E-6</v>
+        <v>1.986761705368856</v>
       </c>
       <c r="G52">
-        <v>1.1706574092494371E-5</v>
+        <v>3.387426839982421</v>
       </c>
       <c r="H52">
-        <v>1.161107016538358E-5</v>
+        <v>3.359791721162626</v>
       </c>
       <c r="I52">
-        <v>1.5979215625919806E-5</v>
+        <v>4.6237629784286334</v>
       </c>
       <c r="J52">
-        <v>2.0996533256481354E-5</v>
+        <v>6.0755793913429796</v>
       </c>
       <c r="K52">
-        <v>1.9604375045881894E-5</v>
+        <v>5.6727429978066297</v>
       </c>
       <c r="L52">
-        <v>1.9014319488821745E-5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.5020038887151106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C53">
-        <v>2.9114022690837249E-5</v>
+        <v>3.9378724556922831</v>
       </c>
       <c r="D53">
-        <v>2.9581214444388848E-5</v>
+        <v>4.0010633639832358</v>
       </c>
       <c r="E53">
-        <v>1.7449928520730391E-5</v>
+        <v>2.3602232369355658</v>
       </c>
       <c r="F53">
-        <v>2.2232355136830906E-5</v>
+        <v>3.007079435506808</v>
       </c>
       <c r="G53">
-        <v>1.3491897101701966E-5</v>
+        <v>1.8248721770951819</v>
       </c>
       <c r="H53">
-        <v>9.6512754299257553E-6</v>
+        <v>1.3054015956979179</v>
       </c>
       <c r="I53">
-        <v>9.6041340452413746E-6</v>
+        <v>1.2990253981438009</v>
       </c>
       <c r="J53">
-        <v>1.0231132465421803E-5</v>
+        <v>1.383831260762302</v>
       </c>
       <c r="K53">
-        <v>1.0027108428434233E-5</v>
+        <v>1.356235601993879</v>
       </c>
       <c r="L53">
-        <v>1.0656425394473435E-5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.4413550639377459</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -2422,53 +2448,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>1.9963901273716976E-5</v>
+        <v>5.3470403924534544</v>
       </c>
       <c r="D55">
-        <v>1.9496709520165376E-5</v>
+        <v>5.2219098809862219</v>
       </c>
       <c r="E55">
-        <v>3.1627995443823833E-5</v>
+        <v>8.4710982513776472</v>
       </c>
       <c r="F55">
-        <v>2.6845568827723318E-5</v>
+        <v>7.1901948878702386</v>
       </c>
       <c r="G55">
-        <v>3.5586026862852269E-5</v>
+        <v>9.5311993599724669</v>
       </c>
       <c r="H55">
-        <v>3.9426648534628471E-5</v>
+        <v>10.55985397660071</v>
       </c>
       <c r="I55">
-        <v>3.9473789919312848E-5</v>
+        <v>10.57248011037124</v>
       </c>
       <c r="J55">
-        <v>3.884679149913243E-5</v>
+        <v>10.40454770914649</v>
       </c>
       <c r="K55">
-        <v>3.9050815536119993E-5</v>
+        <v>10.45919257799485</v>
       </c>
       <c r="L55">
-        <v>3.8421498570080786E-5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>10.29063918800699</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1.763114967830353</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2498,15 +2524,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B57">
         <v>2</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1.114715004849921</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2536,202 +2562,202 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>2.714980717333856</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="K58">
-        <v>0</v>
+        <v>8.144942152001569</v>
       </c>
       <c r="L58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.144942152001569</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C59">
-        <v>3.596550153127638E-5</v>
+        <v>4.8645822440656694</v>
       </c>
       <c r="D59">
-        <v>3.2372174093339721E-5</v>
+        <v>4.3785599141254172</v>
       </c>
       <c r="E59">
-        <v>2.316876691081765E-5</v>
+        <v>3.133735589179754</v>
       </c>
       <c r="F59">
-        <v>1.1794096210478745E-5</v>
+        <v>1.595232891731093</v>
       </c>
       <c r="G59">
-        <v>6.2378722351952938E-6</v>
+        <v>0.84371526112858153</v>
       </c>
       <c r="H59">
-        <v>9.2524635296339373E-6</v>
+        <v>1.2514595343813379</v>
       </c>
       <c r="I59">
-        <v>9.0754469961826628E-6</v>
+        <v>1.2275168268179719</v>
       </c>
       <c r="J59">
-        <v>8.7402797162197039E-6</v>
+        <v>1.1821831395487501</v>
       </c>
       <c r="K59">
-        <v>1.187618187121918E-5</v>
+        <v>1.606335543737297</v>
       </c>
       <c r="L59">
-        <v>1.3104573171959302E-5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.772483943062372</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>3.6738953177110282E-6</v>
+        <v>0.31072305298019998</v>
       </c>
       <c r="E60">
-        <v>2.7261864822550765E-6</v>
+        <v>0.23056971239110219</v>
       </c>
       <c r="F60">
-        <v>4.9359839971260183E-6</v>
+        <v>0.41746535609075902</v>
       </c>
       <c r="G60">
-        <v>8.1108902790770763E-6</v>
+        <v>0.68598595549327135</v>
       </c>
       <c r="H60">
-        <v>9.1595863351374586E-6</v>
+        <v>0.77468038252729909</v>
       </c>
       <c r="I60">
-        <v>8.8820259363934467E-6</v>
+        <v>0.75120545822328422</v>
       </c>
       <c r="J60">
-        <v>8.3135923189733795E-6</v>
+        <v>0.70312966570685875</v>
       </c>
       <c r="K60">
-        <v>7.1644437831736135E-6</v>
+        <v>0.60593937842510348</v>
       </c>
       <c r="L60">
-        <v>6.9099550283214742E-6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.58441575948158586</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B61">
         <v>3</v>
       </c>
       <c r="C61">
-        <v>1.4985625638031827E-6</v>
+        <v>0.5310502283105023</v>
       </c>
       <c r="D61">
-        <v>1.417994684028818E-6</v>
+        <v>0.50249914076692692</v>
       </c>
       <c r="E61">
-        <v>1.1569110702006839E-5</v>
+        <v>4.0997813691928817</v>
       </c>
       <c r="F61">
-        <v>2.0733983887474801E-5</v>
+        <v>7.3475656894068093</v>
       </c>
       <c r="G61">
-        <v>2.31153015808072E-5</v>
+        <v>8.1914405700888668</v>
       </c>
       <c r="H61">
-        <v>1.9052014230308172E-5</v>
+        <v>6.75152092489407</v>
       </c>
       <c r="I61">
-        <v>1.9506591162503453E-5</v>
+        <v>6.9126107515439097</v>
       </c>
       <c r="J61">
-        <v>2.0410192059886484E-5</v>
+        <v>7.2328225828330934</v>
       </c>
       <c r="K61">
-        <v>1.8423438440686764E-5</v>
+        <v>6.5287705875696531</v>
       </c>
       <c r="L61">
-        <v>1.7449535894798787E-5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.1836457447112956</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>3.7039942614757905E-5</v>
+        <v>5.0099078142500204</v>
       </c>
       <c r="D62">
-        <v>3.7039942614757905E-5</v>
+        <v>5.0099078142500204</v>
       </c>
       <c r="E62">
-        <v>3.6239499154112822E-5</v>
+        <v>4.9016423131378959</v>
       </c>
       <c r="F62">
-        <v>2.8943803978884688E-5</v>
+        <v>3.9148492003915871</v>
       </c>
       <c r="G62">
-        <v>1.8770323740955706E-5</v>
+        <v>2.5388158011980582</v>
       </c>
       <c r="H62">
-        <v>1.7338795086390913E-5</v>
+        <v>2.3451916731204538</v>
       </c>
       <c r="I62">
-        <v>1.5507854253602239E-5</v>
+        <v>2.097544291994041</v>
       </c>
       <c r="J62">
-        <v>1.3777875505273133E-5</v>
+        <v>1.8635527294291681</v>
       </c>
       <c r="K62">
-        <v>1.2658050422968892E-5</v>
+        <v>1.7120886602544521</v>
       </c>
       <c r="L62">
-        <v>1.3817769762642125E-5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.8689487030086991</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2746,27 +2772,27 @@
         <v>0</v>
       </c>
       <c r="G63">
-        <v>1.3330276644094868E-6</v>
+        <v>0.10165918131510771</v>
       </c>
       <c r="H63">
-        <v>4.4514076093966692E-6</v>
+        <v>0.3394726646363857</v>
       </c>
       <c r="I63">
-        <v>7.7833948113716906E-6</v>
+        <v>0.59357623663933345</v>
       </c>
       <c r="J63">
-        <v>9.8055918688698312E-6</v>
+        <v>0.74779276403161954</v>
       </c>
       <c r="K63">
-        <v>1.0812656823418499E-5</v>
+        <v>0.82459341981988921</v>
       </c>
       <c r="L63">
-        <v>1.0298355179693281E-5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.78537181516303367</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B64">
         <v>3</v>
@@ -2778,74 +2804,74 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>8.0044346064507953E-7</v>
+        <v>0.2785471630554669</v>
       </c>
       <c r="F64">
-        <v>8.0961386358732181E-6</v>
+        <v>2.8173838123542252</v>
       </c>
       <c r="G64">
-        <v>1.6936591209392716E-5</v>
+        <v>5.893782215928832</v>
       </c>
       <c r="H64">
-        <v>1.5249739918970325E-5</v>
+        <v>5.3067730584488739</v>
       </c>
       <c r="I64">
-        <v>1.3748693549783977E-5</v>
+        <v>4.7844223512363886</v>
       </c>
       <c r="J64">
-        <v>1.3456475240614942E-5</v>
+        <v>4.6827329940064581</v>
       </c>
       <c r="K64">
-        <v>1.3569235368370513E-5</v>
+        <v>4.7219725096454184</v>
       </c>
       <c r="L64">
-        <v>1.29238176724225E-5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.4973729257507236</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>4.8897960001728569</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>4.7319480828396072</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>4.4218568912111129</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>4.0131556991008486</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>2.4818866545407872</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>2.6704506990745172</v>
       </c>
       <c r="I65">
-        <v>0</v>
+        <v>2.8591759288398189</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>2.9322109016576632</v>
       </c>
       <c r="K65">
-        <v>0</v>
+        <v>2.838406766572418</v>
       </c>
       <c r="L65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.8683166598238592</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2854,112 +2880,112 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>1.395524831450477E-3</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>1.197619214559016E-3</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>2.973563001781435E-2</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>5.3563697162564032E-2</v>
       </c>
       <c r="I66">
-        <v>0</v>
+        <v>4.8976761295615977E-2</v>
       </c>
       <c r="J66">
-        <v>0</v>
+        <v>4.8291262449908313E-2</v>
       </c>
       <c r="K66">
-        <v>0</v>
+        <v>4.7674226765596343E-2</v>
       </c>
       <c r="L66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.6472704347461107E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B67">
         <v>3</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1.465208664359624E-2</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>0.26628023721601302</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>0.75774535656881903</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>1.4096682637250539</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>3.7922722832323701</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>3.442901557144054</v>
       </c>
       <c r="I67">
-        <v>0</v>
+        <v>3.1514410654693541</v>
       </c>
       <c r="J67">
-        <v>0</v>
+        <v>3.0364179829085929</v>
       </c>
       <c r="K67">
-        <v>0</v>
+        <v>3.187215918357075</v>
       </c>
       <c r="L67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.1215250285357259</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C68">
-        <v>4.0393353057246278E-5</v>
+        <v>5.4634797151286243</v>
       </c>
       <c r="D68">
-        <v>8.4152818869263087E-6</v>
+        <v>1.138224940651797</v>
       </c>
       <c r="E68">
-        <v>2.2608219994727401E-7</v>
+        <v>3.057917751004828E-2</v>
       </c>
       <c r="F68">
-        <v>4.4633539289774912E-7</v>
+        <v>6.0369941603631218E-2</v>
       </c>
       <c r="G68">
-        <v>9.7227554025259788E-6</v>
+        <v>1.315069755203909</v>
       </c>
       <c r="H68">
-        <v>1.0651512508847549E-5</v>
+        <v>1.440690562257934</v>
       </c>
       <c r="I68">
-        <v>1.5823647078695016E-5</v>
+        <v>2.1402574505583321</v>
       </c>
       <c r="J68">
-        <v>1.4431105883013533E-5</v>
+        <v>1.951906645308163</v>
       </c>
       <c r="K68">
-        <v>1.4494831299427109E-5</v>
+        <v>1.960525947583472</v>
       </c>
       <c r="L68">
-        <v>1.4293870810322304E-5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.933344654804672</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2992,9 +3018,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -3003,80 +3029,80 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <v>3.1978071170319974E-5</v>
+        <v>9.3012115946714076</v>
       </c>
       <c r="E70">
-        <v>4.0167270857299002E-5</v>
+        <v>11.68314009417092</v>
       </c>
       <c r="F70">
-        <v>3.9947017664348529E-5</v>
+        <v>11.61907676961569</v>
       </c>
       <c r="G70">
-        <v>3.0670597654720299E-5</v>
+        <v>8.9209169934664239</v>
       </c>
       <c r="H70">
-        <v>2.9741840548398729E-5</v>
+        <v>8.6507766738723681</v>
       </c>
       <c r="I70">
-        <v>2.4569705978551265E-5</v>
+        <v>7.1463983211555826</v>
       </c>
       <c r="J70">
-        <v>2.5962247174232748E-5</v>
+        <v>7.551435893507719</v>
       </c>
       <c r="K70">
-        <v>2.5898521757819165E-5</v>
+        <v>7.5329005797652382</v>
       </c>
       <c r="L70">
-        <v>2.6099482246923979E-5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.5913523863603576</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>3.2068250501841922</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <v>1.518319439183277E-6</v>
+        <v>0.20536318055366751</v>
       </c>
       <c r="F71">
-        <v>1.3247228344736617E-6</v>
+        <v>0.17917790395011959</v>
       </c>
       <c r="G71">
-        <v>2.2867310107072324E-6</v>
+        <v>0.30929614764212537</v>
       </c>
       <c r="H71">
-        <v>7.9000775661886936E-6</v>
+        <v>1.068540001362221</v>
       </c>
       <c r="I71">
-        <v>5.8747386762516323E-6</v>
+        <v>0.79459894165989509</v>
       </c>
       <c r="J71">
-        <v>5.5742602807180468E-6</v>
+        <v>0.75395716536304869</v>
       </c>
       <c r="K71">
-        <v>7.1191186762144388E-6</v>
+        <v>0.96290992287686339</v>
       </c>
       <c r="L71">
-        <v>7.0140098963811483E-6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.94869323515383019</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1.114715004849921</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -3106,88 +3132,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B73">
         <v>3</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>3.3025511710852129</v>
       </c>
       <c r="D73">
-        <v>7.1127426035585837E-5</v>
+        <v>9.9076535132556387</v>
       </c>
       <c r="E73">
-        <v>6.9609106596402553E-5</v>
+        <v>9.6961600885063408</v>
       </c>
       <c r="F73">
-        <v>6.9802703201112174E-5</v>
+        <v>9.7231270151577558</v>
       </c>
       <c r="G73">
-        <v>6.884069502487859E-5</v>
+        <v>9.5891246447883756</v>
       </c>
       <c r="H73">
-        <v>6.3227348469397146E-5</v>
+        <v>8.8072167954348437</v>
       </c>
       <c r="I73">
-        <v>6.5252687359334196E-5</v>
+        <v>9.0893352002029104</v>
       </c>
       <c r="J73">
-        <v>6.5553165754867786E-5</v>
+        <v>9.1311901638519029</v>
       </c>
       <c r="K73">
-        <v>6.4008307359371394E-5</v>
+        <v>8.9160000105914055</v>
       </c>
       <c r="L73">
-        <v>6.411341613920468E-5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.9306410770524423</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C74">
-        <v>3.7525236279850195E-5</v>
+        <v>5.0755471309800413</v>
       </c>
       <c r="D74">
-        <v>3.0821719118128809E-5</v>
+        <v>4.1688501805888141</v>
       </c>
       <c r="E74">
-        <v>2.8581079709583175E-5</v>
+        <v>3.8657882401710988</v>
       </c>
       <c r="F74">
-        <v>2.6490950058039732E-5</v>
+        <v>3.5830837829052542</v>
       </c>
       <c r="G74">
-        <v>2.3131248164509581E-5</v>
+        <v>3.1286609198622388</v>
       </c>
       <c r="H74">
-        <v>2.6511898302505238E-5</v>
+        <v>3.5859171775121008</v>
       </c>
       <c r="I74">
-        <v>2.3560579801346069E-5</v>
+        <v>3.1867309861326678</v>
       </c>
       <c r="J74">
-        <v>1.9245779519197543E-5</v>
+        <v>2.603124475850136</v>
       </c>
       <c r="K74">
-        <v>1.8100943749195667E-5</v>
+        <v>2.44827753859057</v>
       </c>
       <c r="L74">
-        <v>1.8159777741135295E-5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.4562352419549489</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -3196,229 +3222,229 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>6.2299908252972484E-9</v>
+        <v>7.3029601325039044E-4</v>
       </c>
       <c r="F75">
-        <v>2.0384286624062847E-8</v>
+        <v>2.389500028484566E-3</v>
       </c>
       <c r="G75">
-        <v>1.1427257137986762E-8</v>
+        <v>1.3395333258553589E-3</v>
       </c>
       <c r="H75">
-        <v>8.2206107889770553E-9</v>
+        <v>9.636417539004399E-4</v>
       </c>
       <c r="I75">
-        <v>7.3054880604757924E-9</v>
+        <v>8.563686456407011E-4</v>
       </c>
       <c r="J75">
-        <v>5.9675871170205414E-9</v>
+        <v>6.9953635607104716E-4</v>
       </c>
       <c r="K75">
-        <v>5.11341689341413E-8</v>
+        <v>5.9940826175604563E-3</v>
       </c>
       <c r="L75">
-        <v>5.0981078479672207E-8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.9761369493081867E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B76">
         <v>3</v>
       </c>
       <c r="C76">
-        <v>2.2701292365305624E-7</v>
+        <v>3.8943008397291277E-2</v>
       </c>
       <c r="D76">
-        <v>6.9305300853744433E-6</v>
+        <v>1.188900116210557</v>
       </c>
       <c r="E76">
-        <v>9.1649395030947796E-6</v>
+        <v>1.572202631842901</v>
       </c>
       <c r="F76">
-        <v>1.1240914858839456E-5</v>
+        <v>1.928326522987045</v>
       </c>
       <c r="G76">
-        <v>1.4609573781855682E-5</v>
+        <v>2.5062042517771559</v>
       </c>
       <c r="H76">
-        <v>1.1232130290209043E-5</v>
+        <v>1.926819571204583</v>
       </c>
       <c r="I76">
-        <v>1.4184363914096703E-5</v>
+        <v>2.4332614818930232</v>
       </c>
       <c r="J76">
-        <v>1.8500502097188691E-5</v>
+        <v>3.1736748592604842</v>
       </c>
       <c r="K76">
-        <v>1.9600171285373443E-5</v>
+        <v>3.3623179802801921</v>
       </c>
       <c r="L76">
-        <v>1.9541490383888283E-5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.3522515452837882</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C77">
-        <v>2.7773709184630078E-5</v>
+        <v>3.7565858058145718</v>
       </c>
       <c r="D77">
-        <v>2.6858875057207002E-5</v>
+        <v>3.6328481777251209</v>
       </c>
       <c r="E77">
-        <v>2.7870165214698516E-5</v>
+        <v>3.769632149427935</v>
       </c>
       <c r="F77">
-        <v>2.6572385332422734E-5</v>
+        <v>3.594098465668949</v>
       </c>
       <c r="G77">
-        <v>2.5355569676726646E-5</v>
+        <v>3.42951575220803</v>
       </c>
       <c r="H77">
-        <v>2.4447696559780618E-5</v>
+        <v>3.3067196488165731</v>
       </c>
       <c r="I77">
-        <v>2.375547151037517E-5</v>
+        <v>3.2130914345316461</v>
       </c>
       <c r="J77">
-        <v>2.4037879323515098E-5</v>
+        <v>3.2512890398727321</v>
       </c>
       <c r="K77">
-        <v>2.4223630967706385E-5</v>
+        <v>3.276413231435948</v>
       </c>
       <c r="L77">
-        <v>2.3895102849087974E-5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.2319775365487891</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C78">
-        <v>1.3777462720925715E-6</v>
+        <v>0.1778308467898061</v>
       </c>
       <c r="D78">
-        <v>2.369858161410438E-6</v>
+        <v>0.3058864263702647</v>
       </c>
       <c r="E78">
-        <v>1.00363544319094E-6</v>
+        <v>0.12954296763208009</v>
       </c>
       <c r="F78">
-        <v>5.8679240752009128E-7</v>
+        <v>7.5739483265403071E-2</v>
       </c>
       <c r="G78">
-        <v>5.5429386947977018E-7</v>
+        <v>7.154477582455962E-2</v>
       </c>
       <c r="H78">
-        <v>4.7623990727979003E-7</v>
+        <v>6.1470059982839421E-2</v>
       </c>
       <c r="I78">
-        <v>3.9615008319681535E-7</v>
+        <v>5.1132567859351372E-2</v>
       </c>
       <c r="J78">
-        <v>3.7020590080527526E-7</v>
+        <v>4.7783855532988598E-2</v>
       </c>
       <c r="K78">
-        <v>3.3998965624707616E-7</v>
+        <v>4.3883732218968567E-2</v>
       </c>
       <c r="L78">
-        <v>3.3467339169227091E-7</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.3197542136883468E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B79">
         <v>3</v>
       </c>
       <c r="C79">
-        <v>2.3652296516610667E-7</v>
+        <v>9.9860890259407323E-2</v>
       </c>
       <c r="D79">
-        <v>1.5924520327131838E-7</v>
+        <v>6.7233926976376826E-2</v>
       </c>
       <c r="E79">
-        <v>5.1417776399929951E-7</v>
+        <v>0.21708779622520691</v>
       </c>
       <c r="F79">
-        <v>2.2288006819459316E-6</v>
+        <v>0.94100807570033274</v>
       </c>
       <c r="G79">
-        <v>3.4781148756823397E-6</v>
+        <v>1.468473252338111</v>
       </c>
       <c r="H79">
-        <v>4.464041954828346E-6</v>
+        <v>1.884735393247909</v>
       </c>
       <c r="I79">
-        <v>5.2363568283167743E-6</v>
+        <v>2.2108096531954491</v>
       </c>
       <c r="J79">
-        <v>4.9798931975683813E-6</v>
+        <v>2.1025297385253938</v>
       </c>
       <c r="K79">
-        <v>4.8243577979352913E-6</v>
+        <v>2.0368621046729891</v>
       </c>
       <c r="L79">
-        <v>5.1582021811085094E-6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.1778124656172948</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1.695562670212331</v>
       </c>
       <c r="D80">
-        <v>3.7607604570539635E-5</v>
+        <v>5.0866880106369949</v>
       </c>
       <c r="E80">
-        <v>2.6155272148825468E-5</v>
+        <v>3.537681029506452</v>
       </c>
       <c r="F80">
-        <v>2.6366775281355212E-5</v>
+        <v>3.5662882875527151</v>
       </c>
       <c r="G80">
-        <v>2.4640710005222199E-5</v>
+        <v>3.332826049105321</v>
       </c>
       <c r="H80">
-        <v>2.0286709765632486E-5</v>
+        <v>2.7439174740991619</v>
       </c>
       <c r="I80">
-        <v>1.5938611677699823E-5</v>
+        <v>2.1558072058294648</v>
       </c>
       <c r="J80">
-        <v>1.8552371756009763E-5</v>
+        <v>2.509336291365424</v>
       </c>
       <c r="K80">
-        <v>1.9526092033647094E-5</v>
+        <v>2.641038677585787</v>
       </c>
       <c r="L80">
-        <v>2.1028218597156306E-5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.8442116599736962</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1.114715004849921</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -3448,88 +3474,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B82">
         <v>3</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>2.6820718601540521</v>
       </c>
       <c r="D82">
         <v>0</v>
       </c>
       <c r="E82">
-        <v>1.1452332421714167E-5</v>
+        <v>2.4502474065155848</v>
       </c>
       <c r="F82">
-        <v>1.1240829289184421E-5</v>
+        <v>2.4049959256060429</v>
       </c>
       <c r="G82">
-        <v>1.2966894565317436E-5</v>
+        <v>2.774290739150103</v>
       </c>
       <c r="H82">
-        <v>1.7320894804907152E-5</v>
+        <v>3.7058370305234818</v>
       </c>
       <c r="I82">
-        <v>2.1668992892839815E-5</v>
+        <v>4.636120545786456</v>
       </c>
       <c r="J82">
-        <v>1.9055232814529872E-5</v>
+        <v>4.076901810484121</v>
       </c>
       <c r="K82">
-        <v>1.8081512536892544E-5</v>
+        <v>3.868572581371911</v>
       </c>
       <c r="L82">
-        <v>1.6579385973383325E-5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.5471898637764911</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C83">
-        <v>4.1415969590341123E-5</v>
+        <v>5.6017956572837786</v>
       </c>
       <c r="D83">
-        <v>3.9397647485548673E-5</v>
+        <v>5.3288036661880804</v>
       </c>
       <c r="E83">
-        <v>1.675333492109285E-5</v>
+        <v>2.266004146088751</v>
       </c>
       <c r="F83">
-        <v>1.6685742215359336E-5</v>
+        <v>2.2568617662486239</v>
       </c>
       <c r="G83">
-        <v>9.2442929010097834E-6</v>
+        <v>1.2503544004825839</v>
       </c>
       <c r="H83">
-        <v>9.2442929010097834E-6</v>
+        <v>1.2503544004825839</v>
       </c>
       <c r="I83">
-        <v>6.4559862463312983E-6</v>
+        <v>0.87321668612140313</v>
       </c>
       <c r="J83">
-        <v>1.2011537719823847E-5</v>
+        <v>1.624643356216434</v>
       </c>
       <c r="K83">
-        <v>1.260617138061766E-5</v>
+        <v>1.7050716618110551</v>
       </c>
       <c r="L83">
-        <v>1.260617138061766E-5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.7050716618110551</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B84">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -3550,19 +3576,19 @@
         <v>0</v>
       </c>
       <c r="I84">
-        <v>2.2670599051952546E-6</v>
+        <v>0.18305443901553539</v>
       </c>
       <c r="J84">
-        <v>2.921832356846577E-6</v>
+        <v>0.23592423903501761</v>
       </c>
       <c r="K84">
-        <v>3.4253476017835582E-6</v>
+        <v>0.27658073006398792</v>
       </c>
       <c r="L84">
-        <v>3.4253476017835582E-6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.27658073006398792</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>27</v>
       </c>
@@ -3573,38 +3599,34 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <v>2.0183221047924522E-6</v>
+        <v>0.42012403824468231</v>
       </c>
       <c r="E85">
-        <v>2.4662634669248273E-5</v>
+        <v>5.1336531698261156</v>
       </c>
       <c r="F85">
-        <v>2.4730227374981787E-5</v>
+        <v>5.1477229362034533</v>
       </c>
       <c r="G85">
-        <v>3.217167668933134E-5</v>
+        <v>6.6966985575446989</v>
       </c>
       <c r="H85">
-        <v>3.217167668933134E-5</v>
+        <v>6.6966985575446989</v>
       </c>
       <c r="I85">
-        <v>3.2692923438814569E-5</v>
+        <v>6.8051987264695812</v>
       </c>
       <c r="J85">
-        <v>2.64825995136707E-5</v>
+        <v>5.5124881328315514</v>
       </c>
       <c r="K85">
-        <v>2.5384450607939901E-5</v>
+        <v>5.2839028382573527</v>
       </c>
       <c r="L85">
-        <v>2.5384450607939904E-5</v>
+        <v>5.2839028382573554</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L85">
-    <sortCondition ref="A2:A85"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>